<commit_message>
hpf-value formula based to empirical tests exchanged testing spreadsheet with example hpf values filled
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -943,8 +943,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D97" activeCellId="0" sqref="D97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B105" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H130" activeCellId="0" sqref="H130:H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1154,7 +1154,7 @@
         <v>43</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>43</v>
@@ -1199,7 +1199,7 @@
         <v>44</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>43</v>
@@ -1244,7 +1244,7 @@
         <v>43</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>43</v>
@@ -1289,7 +1289,7 @@
         <v>44</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>43</v>
@@ -1334,7 +1334,7 @@
         <v>43</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>43</v>
@@ -1379,7 +1379,7 @@
         <v>44</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>43</v>
@@ -1424,7 +1424,7 @@
         <v>43</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>43</v>
@@ -1469,7 +1469,7 @@
         <v>44</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>43</v>
@@ -1507,7 +1507,7 @@
         <v>43</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>43</v>
@@ -1545,7 +1545,7 @@
         <v>44</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>43</v>
@@ -1583,7 +1583,7 @@
         <v>43</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>20</v>
+        <v>240</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>43</v>
@@ -1621,7 +1621,7 @@
         <v>44</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>20</v>
+        <v>260</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>43</v>
@@ -1656,7 +1656,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>20</v>
+        <v>280</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>43</v>
@@ -1691,7 +1691,7 @@
         <v>44</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>43</v>
@@ -1726,7 +1726,7 @@
         <v>43</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>43</v>
@@ -1761,7 +1761,7 @@
         <v>44</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>20</v>
+        <v>340</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>43</v>
@@ -1796,7 +1796,7 @@
         <v>43</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>20</v>
+        <v>360</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>43</v>
@@ -1831,7 +1831,7 @@
         <v>44</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>20</v>
+        <v>380</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>43</v>
@@ -1866,7 +1866,7 @@
         <v>43</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>43</v>
@@ -1901,7 +1901,7 @@
         <v>44</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>20</v>
+        <v>420</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>43</v>
@@ -1936,7 +1936,7 @@
         <v>43</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>20</v>
+        <v>440</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>43</v>
@@ -1971,7 +1971,7 @@
         <v>44</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>20</v>
+        <v>460</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>43</v>
@@ -2006,7 +2006,7 @@
         <v>43</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>20</v>
+        <v>480</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>43</v>
@@ -2041,7 +2041,7 @@
         <v>44</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>43</v>
@@ -2076,7 +2076,7 @@
         <v>43</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>20</v>
+        <v>520</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>43</v>
@@ -2111,7 +2111,7 @@
         <v>44</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>20</v>
+        <v>540</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>43</v>
@@ -2146,7 +2146,7 @@
         <v>43</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>20</v>
+        <v>560</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>43</v>
@@ -2181,7 +2181,7 @@
         <v>44</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>20</v>
+        <v>580</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>43</v>
@@ -2216,7 +2216,7 @@
         <v>43</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>20</v>
+        <v>600</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>43</v>
@@ -2251,7 +2251,7 @@
         <v>44</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>20</v>
+        <v>620</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>43</v>
@@ -2286,7 +2286,7 @@
         <v>43</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>20</v>
+        <v>640</v>
       </c>
       <c r="J33" s="7" t="s">
         <v>43</v>
@@ -2321,7 +2321,7 @@
         <v>44</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>20</v>
+        <v>660</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>43</v>
@@ -2356,7 +2356,7 @@
         <v>43</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>20</v>
+        <v>680</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>43</v>
@@ -2391,7 +2391,7 @@
         <v>44</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>20</v>
+        <v>700</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>43</v>
@@ -2426,7 +2426,7 @@
         <v>43</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>20</v>
+        <v>720</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>43</v>
@@ -2461,7 +2461,7 @@
         <v>44</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>20</v>
+        <v>740</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>43</v>
@@ -2496,7 +2496,7 @@
         <v>43</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>20</v>
+        <v>760</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>43</v>
@@ -2531,7 +2531,7 @@
         <v>44</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>20</v>
+        <v>780</v>
       </c>
       <c r="J40" s="7" t="s">
         <v>43</v>
@@ -2566,7 +2566,7 @@
         <v>43</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>20</v>
+        <v>800</v>
       </c>
       <c r="J41" s="7" t="s">
         <v>43</v>
@@ -2601,7 +2601,7 @@
         <v>44</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>20</v>
+        <v>820</v>
       </c>
       <c r="J42" s="7" t="s">
         <v>43</v>
@@ -2636,7 +2636,7 @@
         <v>43</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>20</v>
+        <v>840</v>
       </c>
       <c r="J43" s="7" t="s">
         <v>43</v>
@@ -2671,7 +2671,7 @@
         <v>44</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>20</v>
+        <v>860</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>43</v>
@@ -2706,7 +2706,7 @@
         <v>43</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>20</v>
+        <v>880</v>
       </c>
       <c r="J45" s="7" t="s">
         <v>43</v>
@@ -2741,7 +2741,7 @@
         <v>44</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>20</v>
+        <v>900</v>
       </c>
       <c r="J46" s="7" t="s">
         <v>43</v>
@@ -2776,7 +2776,7 @@
         <v>43</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>20</v>
+        <v>920</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>43</v>
@@ -2811,7 +2811,7 @@
         <v>44</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>20</v>
+        <v>940</v>
       </c>
       <c r="J48" s="7" t="s">
         <v>43</v>
@@ -2846,7 +2846,7 @@
         <v>43</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>20</v>
+        <v>960</v>
       </c>
       <c r="J49" s="7" t="s">
         <v>43</v>
@@ -2881,7 +2881,7 @@
         <v>44</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>20</v>
+        <v>980</v>
       </c>
       <c r="J50" s="7" t="s">
         <v>43</v>
@@ -2916,7 +2916,7 @@
         <v>43</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="J51" s="7" t="s">
         <v>43</v>
@@ -2951,7 +2951,7 @@
         <v>44</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>20</v>
+        <v>1020</v>
       </c>
       <c r="J52" s="7" t="s">
         <v>43</v>
@@ -2986,7 +2986,7 @@
         <v>43</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>20</v>
+        <v>1040</v>
       </c>
       <c r="J53" s="7" t="s">
         <v>43</v>
@@ -3021,7 +3021,7 @@
         <v>44</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>20</v>
+        <v>1060</v>
       </c>
       <c r="J54" s="7" t="s">
         <v>43</v>
@@ -3056,7 +3056,7 @@
         <v>43</v>
       </c>
       <c r="H55" s="2" t="n">
-        <v>20</v>
+        <v>1080</v>
       </c>
       <c r="J55" s="7" t="s">
         <v>43</v>
@@ -3091,7 +3091,7 @@
         <v>44</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>20</v>
+        <v>1100</v>
       </c>
       <c r="J56" s="7" t="s">
         <v>43</v>
@@ -3126,7 +3126,7 @@
         <v>43</v>
       </c>
       <c r="H57" s="2" t="n">
-        <v>20</v>
+        <v>1120</v>
       </c>
       <c r="J57" s="7" t="s">
         <v>43</v>
@@ -3161,7 +3161,7 @@
         <v>44</v>
       </c>
       <c r="H58" s="2" t="n">
-        <v>20</v>
+        <v>1140</v>
       </c>
       <c r="J58" s="7" t="s">
         <v>43</v>
@@ -3196,7 +3196,7 @@
         <v>43</v>
       </c>
       <c r="H59" s="2" t="n">
-        <v>20</v>
+        <v>1160</v>
       </c>
       <c r="J59" s="7" t="s">
         <v>43</v>
@@ -3231,7 +3231,7 @@
         <v>44</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>20</v>
+        <v>1180</v>
       </c>
       <c r="J60" s="7" t="s">
         <v>43</v>
@@ -3266,7 +3266,7 @@
         <v>43</v>
       </c>
       <c r="H61" s="2" t="n">
-        <v>20</v>
+        <v>1200</v>
       </c>
       <c r="J61" s="7" t="s">
         <v>43</v>
@@ -3301,7 +3301,7 @@
         <v>44</v>
       </c>
       <c r="H62" s="2" t="n">
-        <v>20</v>
+        <v>1220</v>
       </c>
       <c r="J62" s="7" t="s">
         <v>43</v>
@@ -3336,7 +3336,7 @@
         <v>43</v>
       </c>
       <c r="H63" s="2" t="n">
-        <v>20</v>
+        <v>1240</v>
       </c>
       <c r="J63" s="7" t="s">
         <v>43</v>
@@ -3371,7 +3371,7 @@
         <v>44</v>
       </c>
       <c r="H64" s="2" t="n">
-        <v>20</v>
+        <v>1260</v>
       </c>
       <c r="J64" s="7" t="s">
         <v>43</v>
@@ -3406,7 +3406,7 @@
         <v>43</v>
       </c>
       <c r="H65" s="2" t="n">
-        <v>20</v>
+        <v>1280</v>
       </c>
       <c r="J65" s="7" t="s">
         <v>43</v>
@@ -3441,7 +3441,7 @@
         <v>44</v>
       </c>
       <c r="H66" s="2" t="n">
-        <v>20</v>
+        <v>1300</v>
       </c>
       <c r="J66" s="7" t="s">
         <v>43</v>
@@ -3476,7 +3476,7 @@
         <v>43</v>
       </c>
       <c r="H67" s="2" t="n">
-        <v>20</v>
+        <v>1320</v>
       </c>
       <c r="J67" s="7" t="s">
         <v>43</v>
@@ -3511,7 +3511,7 @@
         <v>44</v>
       </c>
       <c r="H68" s="2" t="n">
-        <v>20</v>
+        <v>1340</v>
       </c>
       <c r="J68" s="7" t="s">
         <v>43</v>
@@ -3546,7 +3546,7 @@
         <v>43</v>
       </c>
       <c r="H69" s="2" t="n">
-        <v>20</v>
+        <v>1360</v>
       </c>
       <c r="J69" s="7" t="s">
         <v>43</v>
@@ -3581,7 +3581,7 @@
         <v>44</v>
       </c>
       <c r="H70" s="2" t="n">
-        <v>20</v>
+        <v>1380</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>43</v>
@@ -3616,7 +3616,7 @@
         <v>43</v>
       </c>
       <c r="H71" s="2" t="n">
-        <v>20</v>
+        <v>1400</v>
       </c>
       <c r="J71" s="7" t="s">
         <v>43</v>
@@ -3651,7 +3651,7 @@
         <v>44</v>
       </c>
       <c r="H72" s="2" t="n">
-        <v>20</v>
+        <v>1420</v>
       </c>
       <c r="J72" s="7" t="s">
         <v>43</v>
@@ -3686,7 +3686,7 @@
         <v>43</v>
       </c>
       <c r="H73" s="2" t="n">
-        <v>20</v>
+        <v>1440</v>
       </c>
       <c r="J73" s="7" t="s">
         <v>43</v>
@@ -3721,7 +3721,7 @@
         <v>44</v>
       </c>
       <c r="H74" s="2" t="n">
-        <v>20</v>
+        <v>1460</v>
       </c>
       <c r="J74" s="7" t="s">
         <v>43</v>
@@ -3756,7 +3756,7 @@
         <v>43</v>
       </c>
       <c r="H75" s="2" t="n">
-        <v>20</v>
+        <v>1480</v>
       </c>
       <c r="J75" s="7" t="s">
         <v>43</v>
@@ -3791,7 +3791,7 @@
         <v>44</v>
       </c>
       <c r="H76" s="2" t="n">
-        <v>20</v>
+        <v>1500</v>
       </c>
       <c r="J76" s="7" t="s">
         <v>43</v>
@@ -3826,7 +3826,7 @@
         <v>43</v>
       </c>
       <c r="H77" s="2" t="n">
-        <v>20</v>
+        <v>1520</v>
       </c>
       <c r="J77" s="7" t="s">
         <v>43</v>
@@ -3861,7 +3861,7 @@
         <v>44</v>
       </c>
       <c r="H78" s="2" t="n">
-        <v>20</v>
+        <v>1540</v>
       </c>
       <c r="J78" s="7" t="s">
         <v>43</v>
@@ -3896,7 +3896,7 @@
         <v>43</v>
       </c>
       <c r="H79" s="2" t="n">
-        <v>20</v>
+        <v>1560</v>
       </c>
       <c r="J79" s="7" t="s">
         <v>43</v>
@@ -3931,7 +3931,7 @@
         <v>44</v>
       </c>
       <c r="H80" s="2" t="n">
-        <v>20</v>
+        <v>1580</v>
       </c>
       <c r="J80" s="7" t="s">
         <v>43</v>
@@ -3966,7 +3966,7 @@
         <v>43</v>
       </c>
       <c r="H81" s="2" t="n">
-        <v>20</v>
+        <v>1600</v>
       </c>
       <c r="J81" s="7" t="s">
         <v>43</v>
@@ -4001,7 +4001,7 @@
         <v>44</v>
       </c>
       <c r="H82" s="2" t="n">
-        <v>20</v>
+        <v>1620</v>
       </c>
       <c r="J82" s="7" t="s">
         <v>43</v>
@@ -4036,7 +4036,7 @@
         <v>43</v>
       </c>
       <c r="H83" s="2" t="n">
-        <v>20</v>
+        <v>1640</v>
       </c>
       <c r="J83" s="7" t="s">
         <v>43</v>
@@ -4071,7 +4071,7 @@
         <v>44</v>
       </c>
       <c r="H84" s="2" t="n">
-        <v>20</v>
+        <v>1660</v>
       </c>
       <c r="J84" s="7" t="s">
         <v>43</v>
@@ -4106,7 +4106,7 @@
         <v>43</v>
       </c>
       <c r="H85" s="2" t="n">
-        <v>20</v>
+        <v>1680</v>
       </c>
       <c r="J85" s="7" t="s">
         <v>43</v>
@@ -4141,7 +4141,7 @@
         <v>44</v>
       </c>
       <c r="H86" s="2" t="n">
-        <v>20</v>
+        <v>1700</v>
       </c>
       <c r="J86" s="7" t="s">
         <v>43</v>
@@ -4176,7 +4176,7 @@
         <v>43</v>
       </c>
       <c r="H87" s="2" t="n">
-        <v>20</v>
+        <v>1720</v>
       </c>
       <c r="J87" s="7" t="s">
         <v>43</v>
@@ -4211,7 +4211,7 @@
         <v>44</v>
       </c>
       <c r="H88" s="2" t="n">
-        <v>20</v>
+        <v>1740</v>
       </c>
       <c r="J88" s="7" t="s">
         <v>43</v>
@@ -4246,7 +4246,7 @@
         <v>43</v>
       </c>
       <c r="H89" s="2" t="n">
-        <v>20</v>
+        <v>1760</v>
       </c>
       <c r="J89" s="7" t="s">
         <v>43</v>
@@ -4281,7 +4281,7 @@
         <v>44</v>
       </c>
       <c r="H90" s="2" t="n">
-        <v>20</v>
+        <v>1780</v>
       </c>
       <c r="J90" s="7" t="s">
         <v>43</v>
@@ -4316,7 +4316,7 @@
         <v>43</v>
       </c>
       <c r="H91" s="2" t="n">
-        <v>20</v>
+        <v>1800</v>
       </c>
       <c r="J91" s="7" t="s">
         <v>43</v>
@@ -4351,7 +4351,7 @@
         <v>44</v>
       </c>
       <c r="H92" s="2" t="n">
-        <v>20</v>
+        <v>1820</v>
       </c>
       <c r="J92" s="7" t="s">
         <v>43</v>
@@ -4386,7 +4386,7 @@
         <v>43</v>
       </c>
       <c r="H93" s="2" t="n">
-        <v>20</v>
+        <v>1840</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>43</v>
@@ -4421,7 +4421,7 @@
         <v>44</v>
       </c>
       <c r="H94" s="2" t="n">
-        <v>20</v>
+        <v>1860</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>43</v>
@@ -4456,7 +4456,7 @@
         <v>43</v>
       </c>
       <c r="H95" s="2" t="n">
-        <v>20</v>
+        <v>1880</v>
       </c>
       <c r="J95" s="7" t="s">
         <v>43</v>
@@ -4491,7 +4491,7 @@
         <v>44</v>
       </c>
       <c r="H96" s="2" t="n">
-        <v>20</v>
+        <v>1900</v>
       </c>
       <c r="J96" s="7" t="s">
         <v>43</v>
@@ -4526,7 +4526,7 @@
         <v>43</v>
       </c>
       <c r="H97" s="2" t="n">
-        <v>20</v>
+        <v>1920</v>
       </c>
       <c r="J97" s="7" t="s">
         <v>43</v>
@@ -4561,7 +4561,7 @@
         <v>44</v>
       </c>
       <c r="H98" s="2" t="n">
-        <v>20</v>
+        <v>1940</v>
       </c>
       <c r="J98" s="7" t="s">
         <v>43</v>
@@ -4593,7 +4593,7 @@
         <v>43</v>
       </c>
       <c r="H99" s="2" t="n">
-        <v>20</v>
+        <v>1960</v>
       </c>
       <c r="J99" s="7" t="s">
         <v>43</v>
@@ -4625,7 +4625,7 @@
         <v>44</v>
       </c>
       <c r="H100" s="2" t="n">
-        <v>20</v>
+        <v>1980</v>
       </c>
       <c r="J100" s="7" t="s">
         <v>43</v>
@@ -4657,7 +4657,7 @@
         <v>43</v>
       </c>
       <c r="H101" s="2" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="J101" s="7" t="s">
         <v>43</v>
@@ -4721,7 +4721,7 @@
         <v>43</v>
       </c>
       <c r="H103" s="2" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J103" s="7" t="s">
         <v>43</v>
@@ -4753,7 +4753,7 @@
         <v>44</v>
       </c>
       <c r="H104" s="2" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="J104" s="7" t="s">
         <v>43</v>
@@ -4785,7 +4785,7 @@
         <v>43</v>
       </c>
       <c r="H105" s="2" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J105" s="7" t="s">
         <v>43</v>
@@ -4817,7 +4817,7 @@
         <v>44</v>
       </c>
       <c r="H106" s="2" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="J106" s="7" t="s">
         <v>43</v>
@@ -4849,7 +4849,7 @@
         <v>43</v>
       </c>
       <c r="H107" s="2" t="n">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="J107" s="7" t="s">
         <v>43</v>
@@ -4881,7 +4881,7 @@
         <v>44</v>
       </c>
       <c r="H108" s="2" t="n">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="J108" s="7" t="s">
         <v>43</v>
@@ -4913,7 +4913,7 @@
         <v>43</v>
       </c>
       <c r="H109" s="2" t="n">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="J109" s="7" t="s">
         <v>43</v>
@@ -4945,7 +4945,7 @@
         <v>44</v>
       </c>
       <c r="H110" s="2" t="n">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="J110" s="7" t="s">
         <v>43</v>
@@ -4977,7 +4977,7 @@
         <v>43</v>
       </c>
       <c r="H111" s="2" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="J111" s="7" t="s">
         <v>43</v>
@@ -5009,7 +5009,7 @@
         <v>44</v>
       </c>
       <c r="H112" s="2" t="n">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="J112" s="7" t="s">
         <v>43</v>
@@ -5041,7 +5041,7 @@
         <v>43</v>
       </c>
       <c r="H113" s="2" t="n">
-        <v>20</v>
+        <v>240</v>
       </c>
       <c r="J113" s="7" t="s">
         <v>43</v>
@@ -5073,7 +5073,7 @@
         <v>44</v>
       </c>
       <c r="H114" s="2" t="n">
-        <v>20</v>
+        <v>260</v>
       </c>
       <c r="J114" s="7" t="s">
         <v>43</v>
@@ -5105,7 +5105,7 @@
         <v>43</v>
       </c>
       <c r="H115" s="2" t="n">
-        <v>20</v>
+        <v>280</v>
       </c>
       <c r="J115" s="7" t="s">
         <v>43</v>
@@ -5137,7 +5137,7 @@
         <v>44</v>
       </c>
       <c r="H116" s="2" t="n">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="J116" s="7" t="s">
         <v>43</v>
@@ -5169,7 +5169,7 @@
         <v>43</v>
       </c>
       <c r="H117" s="2" t="n">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="J117" s="7" t="s">
         <v>43</v>
@@ -5201,7 +5201,7 @@
         <v>44</v>
       </c>
       <c r="H118" s="2" t="n">
-        <v>20</v>
+        <v>340</v>
       </c>
       <c r="J118" s="7" t="s">
         <v>43</v>
@@ -5233,7 +5233,7 @@
         <v>43</v>
       </c>
       <c r="H119" s="2" t="n">
-        <v>20</v>
+        <v>360</v>
       </c>
       <c r="J119" s="7" t="s">
         <v>43</v>
@@ -5265,7 +5265,7 @@
         <v>44</v>
       </c>
       <c r="H120" s="2" t="n">
-        <v>20</v>
+        <v>380</v>
       </c>
       <c r="J120" s="7" t="s">
         <v>43</v>
@@ -5297,7 +5297,7 @@
         <v>43</v>
       </c>
       <c r="H121" s="2" t="n">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="J121" s="7" t="s">
         <v>43</v>
@@ -5329,7 +5329,7 @@
         <v>44</v>
       </c>
       <c r="H122" s="2" t="n">
-        <v>20</v>
+        <v>420</v>
       </c>
       <c r="J122" s="7" t="s">
         <v>43</v>
@@ -5361,7 +5361,7 @@
         <v>43</v>
       </c>
       <c r="H123" s="2" t="n">
-        <v>20</v>
+        <v>440</v>
       </c>
       <c r="J123" s="7" t="s">
         <v>43</v>
@@ -5393,7 +5393,7 @@
         <v>44</v>
       </c>
       <c r="H124" s="2" t="n">
-        <v>20</v>
+        <v>460</v>
       </c>
       <c r="J124" s="7" t="s">
         <v>43</v>
@@ -5425,7 +5425,7 @@
         <v>43</v>
       </c>
       <c r="H125" s="2" t="n">
-        <v>20</v>
+        <v>480</v>
       </c>
       <c r="J125" s="7" t="s">
         <v>43</v>
@@ -5457,7 +5457,7 @@
         <v>44</v>
       </c>
       <c r="H126" s="2" t="n">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="J126" s="7" t="s">
         <v>43</v>
@@ -5489,7 +5489,7 @@
         <v>43</v>
       </c>
       <c r="H127" s="2" t="n">
-        <v>20</v>
+        <v>520</v>
       </c>
       <c r="J127" s="7" t="s">
         <v>43</v>
@@ -5521,7 +5521,7 @@
         <v>44</v>
       </c>
       <c r="H128" s="2" t="n">
-        <v>20</v>
+        <v>540</v>
       </c>
       <c r="J128" s="7" t="s">
         <v>43</v>
@@ -5553,7 +5553,7 @@
         <v>43</v>
       </c>
       <c r="H129" s="2" t="n">
-        <v>20</v>
+        <v>560</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>43</v>
@@ -5602,7 +5602,7 @@
       <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H129" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H137" type="decimal">
       <formula1>20</formula1>
       <formula2>2000</formula2>
     </dataValidation>
@@ -5629,7 +5629,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="H130:H137 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8684,7 +8684,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="H130:H137 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fx send mono added fx send stereo added fx return added
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="588">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -697,6 +697,33 @@
     <t xml:space="preserve">StMatrix Color</t>
   </si>
   <si>
+    <t xml:space="preserve">Mono FX Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FX Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FX Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stereo FX Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StFX Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StFX Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FX Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FX Return Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FX Return Color</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA01</t>
   </si>
   <si>
@@ -718,6 +745,15 @@
     <t xml:space="preserve">TSMTX1</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET1</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA02</t>
   </si>
   <si>
@@ -739,6 +775,15 @@
     <t xml:space="preserve">TSMTX2</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET2</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA03</t>
   </si>
   <si>
@@ -760,6 +805,15 @@
     <t xml:space="preserve">TSMTX3</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA04</t>
   </si>
   <si>
@@ -781,6 +835,15 @@
     <t xml:space="preserve">TSMTX4</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET4</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA05</t>
   </si>
   <si>
@@ -802,6 +865,15 @@
     <t xml:space="preserve">TSMTX5</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET5</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA06</t>
   </si>
   <si>
@@ -823,6 +895,15 @@
     <t xml:space="preserve">TSMTX6</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET6</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA07</t>
   </si>
   <si>
@@ -844,6 +925,15 @@
     <t xml:space="preserve">TSMTX7</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET7</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA08</t>
   </si>
   <si>
@@ -865,6 +955,15 @@
     <t xml:space="preserve">TSMTX8</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET8</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA09</t>
   </si>
   <si>
@@ -886,6 +985,15 @@
     <t xml:space="preserve">TSMTX9</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET9</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA10</t>
   </si>
   <si>
@@ -907,6 +1015,15 @@
     <t xml:space="preserve">TSMTX10</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET10</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA11</t>
   </si>
   <si>
@@ -928,6 +1045,15 @@
     <t xml:space="preserve">TSMTX11</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET11</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA12</t>
   </si>
   <si>
@@ -949,6 +1075,15 @@
     <t xml:space="preserve">TSMTX12</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET12</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA13</t>
   </si>
   <si>
@@ -970,6 +1105,15 @@
     <t xml:space="preserve">TSMTX13</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET13</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA14</t>
   </si>
   <si>
@@ -991,6 +1135,15 @@
     <t xml:space="preserve">TSMTX14</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET14</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA15</t>
   </si>
   <si>
@@ -1012,6 +1165,15 @@
     <t xml:space="preserve">TSMTX15</t>
   </si>
   <si>
+    <t xml:space="preserve">TMFXS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET15</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDCA16</t>
   </si>
   <si>
@@ -1031,6 +1193,15 @@
   </si>
   <si>
     <t xml:space="preserve">TSMTX16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMFXS16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSFXS16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFXRET16</t>
   </si>
   <si>
     <t xml:space="preserve">TDCA17</t>
@@ -1739,7 +1910,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1808,19 +1979,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1832,12 +2003,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1977,7 +2144,7 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -6662,7 +6829,7 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -9715,32 +9882,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA65"/>
+  <dimension ref="A1:AM65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL17" activeCellId="0" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="16" width="13.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="16" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="16" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="16" width="12.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="16" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="14.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="12.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="16" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="14.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="15.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9813,13 +9986,40 @@
       <c r="AA1" s="17" t="s">
         <v>222</v>
       </c>
+      <c r="AC1" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="AL1" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>42</v>
@@ -9828,7 +10028,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>42</v>
@@ -9837,7 +10037,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>42</v>
@@ -9846,7 +10046,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>42</v>
@@ -9855,7 +10055,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="S2" s="21" t="s">
         <v>42</v>
@@ -9864,7 +10064,7 @@
         <v>1</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="W2" s="21" t="s">
         <v>42</v>
@@ -9873,9 +10073,36 @@
         <v>1</v>
       </c>
       <c r="Z2" s="20" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="AA2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="AM2" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -9884,7 +10111,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>58</v>
@@ -9893,7 +10120,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>58</v>
@@ -9902,7 +10129,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>58</v>
@@ -9911,7 +10138,7 @@
         <v>2</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="O3" s="21" t="s">
         <v>58</v>
@@ -9920,7 +10147,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="S3" s="21" t="s">
         <v>58</v>
@@ -9929,7 +10156,7 @@
         <v>2</v>
       </c>
       <c r="V3" s="20" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="W3" s="21" t="s">
         <v>58</v>
@@ -9938,9 +10165,36 @@
         <v>2</v>
       </c>
       <c r="Z3" s="20" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="AA3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="AM3" s="21" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9949,7 +10203,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>71</v>
@@ -9958,7 +10212,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>71</v>
@@ -9967,7 +10221,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>71</v>
@@ -9976,7 +10230,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>71</v>
@@ -9985,7 +10239,7 @@
         <v>3</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="S4" s="21" t="s">
         <v>71</v>
@@ -9994,7 +10248,7 @@
         <v>3</v>
       </c>
       <c r="V4" s="20" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="W4" s="21" t="s">
         <v>71</v>
@@ -10003,9 +10257,36 @@
         <v>3</v>
       </c>
       <c r="Z4" s="20" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="AA4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="AI4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="AM4" s="21" t="s">
         <v>71</v>
       </c>
     </row>
@@ -10014,7 +10295,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>84</v>
@@ -10023,7 +10304,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>84</v>
@@ -10032,7 +10313,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>84</v>
@@ -10041,7 +10322,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>84</v>
@@ -10050,7 +10331,7 @@
         <v>4</v>
       </c>
       <c r="R5" s="20" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="S5" s="21" t="s">
         <v>84</v>
@@ -10059,7 +10340,7 @@
         <v>4</v>
       </c>
       <c r="V5" s="20" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="W5" s="21" t="s">
         <v>84</v>
@@ -10068,18 +10349,45 @@
         <v>4</v>
       </c>
       <c r="Z5" s="20" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="AA5" s="21" t="s">
         <v>84</v>
       </c>
+      <c r="AC5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE5" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="AI5" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="AM5" s="21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>97</v>
@@ -10088,7 +10396,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>97</v>
@@ -10097,7 +10405,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>253</v>
+        <v>274</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>97</v>
@@ -10106,7 +10414,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>254</v>
+        <v>275</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>97</v>
@@ -10115,7 +10423,7 @@
         <v>5</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="S6" s="21" t="s">
         <v>97</v>
@@ -10124,7 +10432,7 @@
         <v>5</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="W6" s="21" t="s">
         <v>97</v>
@@ -10133,9 +10441,36 @@
         <v>5</v>
       </c>
       <c r="Z6" s="20" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="AA6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="AE6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="AM6" s="21" t="s">
         <v>97</v>
       </c>
     </row>
@@ -10144,17 +10479,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="19" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>110</v>
@@ -10163,7 +10498,7 @@
         <v>6</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>110</v>
@@ -10172,7 +10507,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="O7" s="21" t="s">
         <v>110</v>
@@ -10181,7 +10516,7 @@
         <v>6</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="S7" s="21" t="s">
         <v>110</v>
@@ -10190,7 +10525,7 @@
         <v>6</v>
       </c>
       <c r="V7" s="20" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="W7" s="21" t="s">
         <v>110</v>
@@ -10199,9 +10534,36 @@
         <v>6</v>
       </c>
       <c r="Z7" s="20" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="AA7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="AI7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="AL7" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="AM7" s="21" t="s">
         <v>110</v>
       </c>
     </row>
@@ -10210,7 +10572,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>123</v>
@@ -10219,7 +10581,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>123</v>
@@ -10228,7 +10590,7 @@
         <v>7</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>123</v>
@@ -10237,7 +10599,7 @@
         <v>7</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="O8" s="21" t="s">
         <v>123</v>
@@ -10246,7 +10608,7 @@
         <v>7</v>
       </c>
       <c r="R8" s="20" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="S8" s="21" t="s">
         <v>123</v>
@@ -10255,7 +10617,7 @@
         <v>7</v>
       </c>
       <c r="V8" s="20" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="W8" s="21" t="s">
         <v>123</v>
@@ -10264,9 +10626,36 @@
         <v>7</v>
       </c>
       <c r="Z8" s="20" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AA8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AI8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL8" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="AM8" s="21" t="s">
         <v>123</v>
       </c>
     </row>
@@ -10275,7 +10664,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>136</v>
@@ -10284,7 +10673,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>273</v>
+        <v>303</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>136</v>
@@ -10293,7 +10682,7 @@
         <v>8</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>274</v>
+        <v>304</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>136</v>
@@ -10302,7 +10691,7 @@
         <v>8</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>275</v>
+        <v>305</v>
       </c>
       <c r="O9" s="21" t="s">
         <v>136</v>
@@ -10311,7 +10700,7 @@
         <v>8</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
       <c r="S9" s="21" t="s">
         <v>136</v>
@@ -10320,7 +10709,7 @@
         <v>8</v>
       </c>
       <c r="V9" s="20" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
       <c r="W9" s="21" t="s">
         <v>136</v>
@@ -10329,9 +10718,36 @@
         <v>8</v>
       </c>
       <c r="Z9" s="20" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
       <c r="AA9" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD9" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE9" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="AI9" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL9" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="AM9" s="21" t="s">
         <v>136</v>
       </c>
     </row>
@@ -10340,7 +10756,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>279</v>
+        <v>312</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>42</v>
@@ -10349,7 +10765,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>42</v>
@@ -10358,7 +10774,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>42</v>
@@ -10367,7 +10783,7 @@
         <v>9</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="O10" s="21" t="s">
         <v>42</v>
@@ -10376,7 +10792,7 @@
         <v>9</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>283</v>
+        <v>316</v>
       </c>
       <c r="S10" s="21" t="s">
         <v>42</v>
@@ -10385,7 +10801,7 @@
         <v>9</v>
       </c>
       <c r="V10" s="20" t="s">
-        <v>284</v>
+        <v>317</v>
       </c>
       <c r="W10" s="21" t="s">
         <v>42</v>
@@ -10394,9 +10810,36 @@
         <v>9</v>
       </c>
       <c r="Z10" s="20" t="s">
-        <v>285</v>
+        <v>318</v>
       </c>
       <c r="AA10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="AE10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="AI10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="AM10" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -10405,7 +10848,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>58</v>
@@ -10414,7 +10857,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>287</v>
+        <v>323</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>58</v>
@@ -10423,7 +10866,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>288</v>
+        <v>324</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>58</v>
@@ -10432,7 +10875,7 @@
         <v>10</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>289</v>
+        <v>325</v>
       </c>
       <c r="O11" s="21" t="s">
         <v>58</v>
@@ -10441,7 +10884,7 @@
         <v>10</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>290</v>
+        <v>326</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>58</v>
@@ -10450,7 +10893,7 @@
         <v>10</v>
       </c>
       <c r="V11" s="20" t="s">
-        <v>291</v>
+        <v>327</v>
       </c>
       <c r="W11" s="21" t="s">
         <v>58</v>
@@ -10459,9 +10902,36 @@
         <v>10</v>
       </c>
       <c r="Z11" s="20" t="s">
-        <v>292</v>
+        <v>328</v>
       </c>
       <c r="AA11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD11" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="AI11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL11" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="AM11" s="21" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10470,7 +10940,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>71</v>
@@ -10479,7 +10949,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>71</v>
@@ -10488,7 +10958,7 @@
         <v>11</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>71</v>
@@ -10497,7 +10967,7 @@
         <v>11</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="O12" s="21" t="s">
         <v>71</v>
@@ -10506,7 +10976,7 @@
         <v>11</v>
       </c>
       <c r="R12" s="20" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>71</v>
@@ -10515,7 +10985,7 @@
         <v>11</v>
       </c>
       <c r="V12" s="20" t="s">
-        <v>298</v>
+        <v>337</v>
       </c>
       <c r="W12" s="21" t="s">
         <v>71</v>
@@ -10524,9 +10994,36 @@
         <v>11</v>
       </c>
       <c r="Z12" s="20" t="s">
-        <v>299</v>
+        <v>338</v>
       </c>
       <c r="AA12" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE12" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="AI12" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="AL12" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="AM12" s="21" t="s">
         <v>71</v>
       </c>
     </row>
@@ -10535,7 +11032,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>300</v>
+        <v>342</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>84</v>
@@ -10544,7 +11041,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>301</v>
+        <v>343</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>84</v>
@@ -10553,7 +11050,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>84</v>
@@ -10562,7 +11059,7 @@
         <v>12</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>303</v>
+        <v>345</v>
       </c>
       <c r="O13" s="21" t="s">
         <v>84</v>
@@ -10571,7 +11068,7 @@
         <v>12</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>304</v>
+        <v>346</v>
       </c>
       <c r="S13" s="21" t="s">
         <v>84</v>
@@ -10580,7 +11077,7 @@
         <v>12</v>
       </c>
       <c r="V13" s="20" t="s">
-        <v>305</v>
+        <v>347</v>
       </c>
       <c r="W13" s="21" t="s">
         <v>84</v>
@@ -10589,9 +11086,36 @@
         <v>12</v>
       </c>
       <c r="Z13" s="20" t="s">
-        <v>306</v>
+        <v>348</v>
       </c>
       <c r="AA13" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="AE13" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="AH13" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="AI13" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="AL13" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="AM13" s="21" t="s">
         <v>84</v>
       </c>
     </row>
@@ -10600,7 +11124,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>307</v>
+        <v>352</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>97</v>
@@ -10609,7 +11133,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="G14" s="21" t="s">
         <v>97</v>
@@ -10618,7 +11142,7 @@
         <v>13</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>309</v>
+        <v>354</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>97</v>
@@ -10627,7 +11151,7 @@
         <v>13</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>310</v>
+        <v>355</v>
       </c>
       <c r="O14" s="21" t="s">
         <v>97</v>
@@ -10636,7 +11160,7 @@
         <v>13</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>311</v>
+        <v>356</v>
       </c>
       <c r="S14" s="21" t="s">
         <v>97</v>
@@ -10645,7 +11169,7 @@
         <v>13</v>
       </c>
       <c r="V14" s="20" t="s">
-        <v>312</v>
+        <v>357</v>
       </c>
       <c r="W14" s="21" t="s">
         <v>97</v>
@@ -10654,9 +11178,36 @@
         <v>13</v>
       </c>
       <c r="Z14" s="20" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
       <c r="AA14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="AH14" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="AI14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="AL14" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="AM14" s="21" t="s">
         <v>97</v>
       </c>
     </row>
@@ -10665,7 +11216,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>314</v>
+        <v>362</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>110</v>
@@ -10674,7 +11225,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>315</v>
+        <v>363</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>110</v>
@@ -10683,7 +11234,7 @@
         <v>14</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>316</v>
+        <v>364</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>110</v>
@@ -10692,7 +11243,7 @@
         <v>14</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>317</v>
+        <v>365</v>
       </c>
       <c r="O15" s="21" t="s">
         <v>110</v>
@@ -10701,7 +11252,7 @@
         <v>14</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>318</v>
+        <v>366</v>
       </c>
       <c r="S15" s="21" t="s">
         <v>110</v>
@@ -10710,7 +11261,7 @@
         <v>14</v>
       </c>
       <c r="V15" s="20" t="s">
-        <v>319</v>
+        <v>367</v>
       </c>
       <c r="W15" s="21" t="s">
         <v>110</v>
@@ -10719,9 +11270,36 @@
         <v>14</v>
       </c>
       <c r="Z15" s="20" t="s">
-        <v>320</v>
+        <v>368</v>
       </c>
       <c r="AA15" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD15" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="AE15" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="AH15" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI15" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="AL15" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="AM15" s="21" t="s">
         <v>110</v>
       </c>
     </row>
@@ -10730,7 +11308,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>321</v>
+        <v>372</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>123</v>
@@ -10739,7 +11317,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>322</v>
+        <v>373</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>123</v>
@@ -10748,7 +11326,7 @@
         <v>15</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>323</v>
+        <v>374</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>123</v>
@@ -10757,7 +11335,7 @@
         <v>15</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>324</v>
+        <v>375</v>
       </c>
       <c r="O16" s="21" t="s">
         <v>123</v>
@@ -10766,7 +11344,7 @@
         <v>15</v>
       </c>
       <c r="R16" s="20" t="s">
-        <v>325</v>
+        <v>376</v>
       </c>
       <c r="S16" s="21" t="s">
         <v>123</v>
@@ -10775,7 +11353,7 @@
         <v>15</v>
       </c>
       <c r="V16" s="20" t="s">
-        <v>326</v>
+        <v>377</v>
       </c>
       <c r="W16" s="21" t="s">
         <v>123</v>
@@ -10784,9 +11362,36 @@
         <v>15</v>
       </c>
       <c r="Z16" s="20" t="s">
-        <v>327</v>
+        <v>378</v>
       </c>
       <c r="AA16" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="AE16" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="AH16" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="AI16" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="AL16" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="AM16" s="21" t="s">
         <v>123</v>
       </c>
     </row>
@@ -10795,7 +11400,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>328</v>
+        <v>382</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>136</v>
@@ -10804,7 +11409,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="G17" s="21" t="s">
         <v>136</v>
@@ -10813,7 +11418,7 @@
         <v>16</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>330</v>
+        <v>384</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>136</v>
@@ -10822,7 +11427,7 @@
         <v>16</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>331</v>
+        <v>385</v>
       </c>
       <c r="O17" s="21" t="s">
         <v>136</v>
@@ -10831,7 +11436,7 @@
         <v>16</v>
       </c>
       <c r="R17" s="20" t="s">
-        <v>332</v>
+        <v>386</v>
       </c>
       <c r="S17" s="21" t="s">
         <v>136</v>
@@ -10840,7 +11445,7 @@
         <v>16</v>
       </c>
       <c r="V17" s="20" t="s">
-        <v>333</v>
+        <v>387</v>
       </c>
       <c r="W17" s="21" t="s">
         <v>136</v>
@@ -10849,9 +11454,36 @@
         <v>16</v>
       </c>
       <c r="Z17" s="20" t="s">
-        <v>334</v>
+        <v>388</v>
       </c>
       <c r="AA17" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD17" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="AE17" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="AH17" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="AI17" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="AL17" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="AM17" s="21" t="s">
         <v>136</v>
       </c>
     </row>
@@ -10860,7 +11492,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>335</v>
+        <v>392</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>42</v>
@@ -10869,7 +11501,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>336</v>
+        <v>393</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>42</v>
@@ -10878,7 +11510,7 @@
         <v>17</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>337</v>
+        <v>394</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>42</v>
@@ -10887,7 +11519,7 @@
         <v>17</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>338</v>
+        <v>395</v>
       </c>
       <c r="O18" s="21" t="s">
         <v>42</v>
@@ -10896,7 +11528,7 @@
         <v>17</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>339</v>
+        <v>396</v>
       </c>
       <c r="S18" s="21" t="s">
         <v>42</v>
@@ -10905,7 +11537,7 @@
         <v>17</v>
       </c>
       <c r="V18" s="20" t="s">
-        <v>340</v>
+        <v>397</v>
       </c>
       <c r="W18" s="21" t="s">
         <v>42</v>
@@ -10914,7 +11546,7 @@
         <v>17</v>
       </c>
       <c r="Z18" s="20" t="s">
-        <v>341</v>
+        <v>398</v>
       </c>
       <c r="AA18" s="21" t="s">
         <v>42</v>
@@ -10925,7 +11557,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>342</v>
+        <v>399</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>58</v>
@@ -10934,7 +11566,7 @@
         <v>18</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>343</v>
+        <v>400</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>58</v>
@@ -10943,7 +11575,7 @@
         <v>18</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>344</v>
+        <v>401</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>58</v>
@@ -10952,7 +11584,7 @@
         <v>18</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>345</v>
+        <v>402</v>
       </c>
       <c r="O19" s="21" t="s">
         <v>58</v>
@@ -10961,7 +11593,7 @@
         <v>18</v>
       </c>
       <c r="R19" s="20" t="s">
-        <v>346</v>
+        <v>403</v>
       </c>
       <c r="S19" s="21" t="s">
         <v>58</v>
@@ -10970,7 +11602,7 @@
         <v>18</v>
       </c>
       <c r="V19" s="20" t="s">
-        <v>347</v>
+        <v>404</v>
       </c>
       <c r="W19" s="21" t="s">
         <v>58</v>
@@ -10979,7 +11611,7 @@
         <v>18</v>
       </c>
       <c r="Z19" s="20" t="s">
-        <v>348</v>
+        <v>405</v>
       </c>
       <c r="AA19" s="21" t="s">
         <v>58</v>
@@ -10990,7 +11622,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>349</v>
+        <v>406</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>71</v>
@@ -10999,7 +11631,7 @@
         <v>19</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>350</v>
+        <v>407</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>71</v>
@@ -11008,7 +11640,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>351</v>
+        <v>408</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>71</v>
@@ -11017,7 +11649,7 @@
         <v>19</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>352</v>
+        <v>409</v>
       </c>
       <c r="O20" s="21" t="s">
         <v>71</v>
@@ -11026,7 +11658,7 @@
         <v>19</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>353</v>
+        <v>410</v>
       </c>
       <c r="S20" s="21" t="s">
         <v>71</v>
@@ -11035,7 +11667,7 @@
         <v>19</v>
       </c>
       <c r="V20" s="20" t="s">
-        <v>354</v>
+        <v>411</v>
       </c>
       <c r="W20" s="21" t="s">
         <v>71</v>
@@ -11044,7 +11676,7 @@
         <v>19</v>
       </c>
       <c r="Z20" s="20" t="s">
-        <v>355</v>
+        <v>412</v>
       </c>
       <c r="AA20" s="21" t="s">
         <v>71</v>
@@ -11055,7 +11687,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>84</v>
@@ -11064,7 +11696,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>357</v>
+        <v>414</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>84</v>
@@ -11073,7 +11705,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>358</v>
+        <v>415</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>84</v>
@@ -11082,7 +11714,7 @@
         <v>20</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>359</v>
+        <v>416</v>
       </c>
       <c r="O21" s="21" t="s">
         <v>84</v>
@@ -11091,7 +11723,7 @@
         <v>20</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>360</v>
+        <v>417</v>
       </c>
       <c r="S21" s="21" t="s">
         <v>84</v>
@@ -11100,7 +11732,7 @@
         <v>20</v>
       </c>
       <c r="V21" s="20" t="s">
-        <v>361</v>
+        <v>418</v>
       </c>
       <c r="W21" s="21" t="s">
         <v>84</v>
@@ -11109,7 +11741,7 @@
         <v>20</v>
       </c>
       <c r="Z21" s="20" t="s">
-        <v>362</v>
+        <v>419</v>
       </c>
       <c r="AA21" s="21" t="s">
         <v>84</v>
@@ -11120,7 +11752,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>363</v>
+        <v>420</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>97</v>
@@ -11129,7 +11761,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>364</v>
+        <v>421</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>97</v>
@@ -11138,7 +11770,7 @@
         <v>21</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>365</v>
+        <v>422</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>97</v>
@@ -11147,7 +11779,7 @@
         <v>21</v>
       </c>
       <c r="N22" s="20" t="s">
-        <v>366</v>
+        <v>423</v>
       </c>
       <c r="O22" s="21" t="s">
         <v>97</v>
@@ -11156,7 +11788,7 @@
         <v>21</v>
       </c>
       <c r="R22" s="20" t="s">
-        <v>367</v>
+        <v>424</v>
       </c>
       <c r="S22" s="21" t="s">
         <v>97</v>
@@ -11165,7 +11797,7 @@
         <v>21</v>
       </c>
       <c r="V22" s="20" t="s">
-        <v>368</v>
+        <v>425</v>
       </c>
       <c r="W22" s="21" t="s">
         <v>97</v>
@@ -11174,7 +11806,7 @@
         <v>21</v>
       </c>
       <c r="Z22" s="20" t="s">
-        <v>369</v>
+        <v>426</v>
       </c>
       <c r="AA22" s="21" t="s">
         <v>97</v>
@@ -11185,7 +11817,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>370</v>
+        <v>427</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>110</v>
@@ -11194,7 +11826,7 @@
         <v>22</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>110</v>
@@ -11203,7 +11835,7 @@
         <v>22</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>372</v>
+        <v>429</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>110</v>
@@ -11212,7 +11844,7 @@
         <v>22</v>
       </c>
       <c r="N23" s="20" t="s">
-        <v>373</v>
+        <v>430</v>
       </c>
       <c r="O23" s="21" t="s">
         <v>110</v>
@@ -11221,7 +11853,7 @@
         <v>22</v>
       </c>
       <c r="R23" s="20" t="s">
-        <v>374</v>
+        <v>431</v>
       </c>
       <c r="S23" s="21" t="s">
         <v>110</v>
@@ -11230,7 +11862,7 @@
         <v>22</v>
       </c>
       <c r="V23" s="20" t="s">
-        <v>375</v>
+        <v>432</v>
       </c>
       <c r="W23" s="21" t="s">
         <v>110</v>
@@ -11239,7 +11871,7 @@
         <v>22</v>
       </c>
       <c r="Z23" s="20" t="s">
-        <v>376</v>
+        <v>433</v>
       </c>
       <c r="AA23" s="21" t="s">
         <v>110</v>
@@ -11250,7 +11882,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>377</v>
+        <v>434</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>123</v>
@@ -11259,7 +11891,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>378</v>
+        <v>435</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>123</v>
@@ -11268,7 +11900,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>379</v>
+        <v>436</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>123</v>
@@ -11277,7 +11909,7 @@
         <v>23</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>380</v>
+        <v>437</v>
       </c>
       <c r="O24" s="21" t="s">
         <v>123</v>
@@ -11286,7 +11918,7 @@
         <v>23</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>381</v>
+        <v>438</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>123</v>
@@ -11295,7 +11927,7 @@
         <v>23</v>
       </c>
       <c r="V24" s="20" t="s">
-        <v>382</v>
+        <v>439</v>
       </c>
       <c r="W24" s="21" t="s">
         <v>123</v>
@@ -11304,7 +11936,7 @@
         <v>23</v>
       </c>
       <c r="Z24" s="20" t="s">
-        <v>383</v>
+        <v>440</v>
       </c>
       <c r="AA24" s="21" t="s">
         <v>123</v>
@@ -11315,7 +11947,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>384</v>
+        <v>441</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>136</v>
@@ -11324,7 +11956,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>385</v>
+        <v>442</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>136</v>
@@ -11333,7 +11965,7 @@
         <v>24</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>386</v>
+        <v>443</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>136</v>
@@ -11342,7 +11974,7 @@
         <v>24</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>387</v>
+        <v>444</v>
       </c>
       <c r="O25" s="21" t="s">
         <v>136</v>
@@ -11351,7 +11983,7 @@
         <v>24</v>
       </c>
       <c r="R25" s="20" t="s">
-        <v>388</v>
+        <v>445</v>
       </c>
       <c r="S25" s="21" t="s">
         <v>136</v>
@@ -11360,7 +11992,7 @@
         <v>24</v>
       </c>
       <c r="V25" s="20" t="s">
-        <v>389</v>
+        <v>446</v>
       </c>
       <c r="W25" s="21" t="s">
         <v>136</v>
@@ -11369,7 +12001,7 @@
         <v>24</v>
       </c>
       <c r="Z25" s="20" t="s">
-        <v>390</v>
+        <v>447</v>
       </c>
       <c r="AA25" s="21" t="s">
         <v>136</v>
@@ -11380,7 +12012,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>391</v>
+        <v>448</v>
       </c>
       <c r="G26" s="21" t="s">
         <v>42</v>
@@ -11389,7 +12021,7 @@
         <v>25</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>392</v>
+        <v>449</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>42</v>
@@ -11398,7 +12030,7 @@
         <v>25</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>393</v>
+        <v>450</v>
       </c>
       <c r="O26" s="21" t="s">
         <v>42</v>
@@ -11407,7 +12039,7 @@
         <v>25</v>
       </c>
       <c r="R26" s="20" t="s">
-        <v>394</v>
+        <v>451</v>
       </c>
       <c r="S26" s="21" t="s">
         <v>42</v>
@@ -11416,7 +12048,7 @@
         <v>25</v>
       </c>
       <c r="V26" s="20" t="s">
-        <v>395</v>
+        <v>452</v>
       </c>
       <c r="W26" s="21" t="s">
         <v>42</v>
@@ -11425,7 +12057,7 @@
         <v>25</v>
       </c>
       <c r="Z26" s="20" t="s">
-        <v>396</v>
+        <v>453</v>
       </c>
       <c r="AA26" s="21" t="s">
         <v>42</v>
@@ -11436,7 +12068,7 @@
         <v>26</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>397</v>
+        <v>454</v>
       </c>
       <c r="G27" s="21" t="s">
         <v>58</v>
@@ -11445,7 +12077,7 @@
         <v>26</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>398</v>
+        <v>455</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>58</v>
@@ -11454,7 +12086,7 @@
         <v>26</v>
       </c>
       <c r="N27" s="20" t="s">
-        <v>399</v>
+        <v>456</v>
       </c>
       <c r="O27" s="21" t="s">
         <v>58</v>
@@ -11463,7 +12095,7 @@
         <v>26</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>400</v>
+        <v>457</v>
       </c>
       <c r="S27" s="21" t="s">
         <v>58</v>
@@ -11472,7 +12104,7 @@
         <v>26</v>
       </c>
       <c r="V27" s="20" t="s">
-        <v>401</v>
+        <v>458</v>
       </c>
       <c r="W27" s="21" t="s">
         <v>58</v>
@@ -11481,7 +12113,7 @@
         <v>26</v>
       </c>
       <c r="Z27" s="20" t="s">
-        <v>402</v>
+        <v>459</v>
       </c>
       <c r="AA27" s="21" t="s">
         <v>58</v>
@@ -11492,7 +12124,7 @@
         <v>27</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>403</v>
+        <v>460</v>
       </c>
       <c r="G28" s="21" t="s">
         <v>71</v>
@@ -11501,7 +12133,7 @@
         <v>27</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>404</v>
+        <v>461</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>71</v>
@@ -11510,7 +12142,7 @@
         <v>27</v>
       </c>
       <c r="N28" s="20" t="s">
-        <v>405</v>
+        <v>462</v>
       </c>
       <c r="O28" s="21" t="s">
         <v>71</v>
@@ -11519,7 +12151,7 @@
         <v>27</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>406</v>
+        <v>463</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>71</v>
@@ -11528,7 +12160,7 @@
         <v>27</v>
       </c>
       <c r="V28" s="20" t="s">
-        <v>407</v>
+        <v>464</v>
       </c>
       <c r="W28" s="21" t="s">
         <v>71</v>
@@ -11537,7 +12169,7 @@
         <v>27</v>
       </c>
       <c r="Z28" s="20" t="s">
-        <v>408</v>
+        <v>465</v>
       </c>
       <c r="AA28" s="21" t="s">
         <v>71</v>
@@ -11548,7 +12180,7 @@
         <v>28</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>409</v>
+        <v>466</v>
       </c>
       <c r="G29" s="21" t="s">
         <v>84</v>
@@ -11557,7 +12189,7 @@
         <v>28</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>410</v>
+        <v>467</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>84</v>
@@ -11566,7 +12198,7 @@
         <v>28</v>
       </c>
       <c r="N29" s="20" t="s">
-        <v>411</v>
+        <v>468</v>
       </c>
       <c r="O29" s="21" t="s">
         <v>84</v>
@@ -11575,7 +12207,7 @@
         <v>28</v>
       </c>
       <c r="R29" s="20" t="s">
-        <v>412</v>
+        <v>469</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>84</v>
@@ -11584,7 +12216,7 @@
         <v>28</v>
       </c>
       <c r="V29" s="20" t="s">
-        <v>413</v>
+        <v>470</v>
       </c>
       <c r="W29" s="21" t="s">
         <v>84</v>
@@ -11593,7 +12225,7 @@
         <v>28</v>
       </c>
       <c r="Z29" s="20" t="s">
-        <v>414</v>
+        <v>471</v>
       </c>
       <c r="AA29" s="21" t="s">
         <v>84</v>
@@ -11604,7 +12236,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>415</v>
+        <v>472</v>
       </c>
       <c r="G30" s="21" t="s">
         <v>97</v>
@@ -11613,7 +12245,7 @@
         <v>29</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>416</v>
+        <v>473</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>97</v>
@@ -11622,7 +12254,7 @@
         <v>29</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>417</v>
+        <v>474</v>
       </c>
       <c r="O30" s="21" t="s">
         <v>97</v>
@@ -11631,7 +12263,7 @@
         <v>29</v>
       </c>
       <c r="R30" s="20" t="s">
-        <v>418</v>
+        <v>475</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>97</v>
@@ -11640,7 +12272,7 @@
         <v>29</v>
       </c>
       <c r="V30" s="20" t="s">
-        <v>419</v>
+        <v>476</v>
       </c>
       <c r="W30" s="21" t="s">
         <v>97</v>
@@ -11649,7 +12281,7 @@
         <v>29</v>
       </c>
       <c r="Z30" s="20" t="s">
-        <v>420</v>
+        <v>477</v>
       </c>
       <c r="AA30" s="21" t="s">
         <v>97</v>
@@ -11660,7 +12292,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>421</v>
+        <v>478</v>
       </c>
       <c r="G31" s="21" t="s">
         <v>110</v>
@@ -11669,7 +12301,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>422</v>
+        <v>479</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>110</v>
@@ -11678,7 +12310,7 @@
         <v>30</v>
       </c>
       <c r="N31" s="20" t="s">
-        <v>423</v>
+        <v>480</v>
       </c>
       <c r="O31" s="21" t="s">
         <v>110</v>
@@ -11687,7 +12319,7 @@
         <v>30</v>
       </c>
       <c r="R31" s="20" t="s">
-        <v>424</v>
+        <v>481</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>110</v>
@@ -11696,7 +12328,7 @@
         <v>30</v>
       </c>
       <c r="V31" s="20" t="s">
-        <v>425</v>
+        <v>482</v>
       </c>
       <c r="W31" s="21" t="s">
         <v>110</v>
@@ -11705,7 +12337,7 @@
         <v>30</v>
       </c>
       <c r="Z31" s="20" t="s">
-        <v>426</v>
+        <v>483</v>
       </c>
       <c r="AA31" s="21" t="s">
         <v>110</v>
@@ -11716,7 +12348,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>427</v>
+        <v>484</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>123</v>
@@ -11725,7 +12357,7 @@
         <v>31</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>428</v>
+        <v>485</v>
       </c>
       <c r="K32" s="21" t="s">
         <v>123</v>
@@ -11734,7 +12366,7 @@
         <v>31</v>
       </c>
       <c r="N32" s="20" t="s">
-        <v>429</v>
+        <v>486</v>
       </c>
       <c r="O32" s="21" t="s">
         <v>123</v>
@@ -11743,7 +12375,7 @@
         <v>31</v>
       </c>
       <c r="R32" s="20" t="s">
-        <v>430</v>
+        <v>487</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>123</v>
@@ -11752,7 +12384,7 @@
         <v>31</v>
       </c>
       <c r="V32" s="20" t="s">
-        <v>431</v>
+        <v>488</v>
       </c>
       <c r="W32" s="21" t="s">
         <v>123</v>
@@ -11761,7 +12393,7 @@
         <v>31</v>
       </c>
       <c r="Z32" s="20" t="s">
-        <v>432</v>
+        <v>489</v>
       </c>
       <c r="AA32" s="21" t="s">
         <v>123</v>
@@ -11772,7 +12404,7 @@
         <v>32</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>433</v>
+        <v>490</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>136</v>
@@ -11782,7 +12414,7 @@
         <v>32</v>
       </c>
       <c r="N33" s="20" t="s">
-        <v>434</v>
+        <v>491</v>
       </c>
       <c r="O33" s="21" t="s">
         <v>136</v>
@@ -11792,7 +12424,7 @@
         <v>32</v>
       </c>
       <c r="V33" s="20" t="s">
-        <v>435</v>
+        <v>492</v>
       </c>
       <c r="W33" s="21" t="s">
         <v>136</v>
@@ -11803,7 +12435,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>436</v>
+        <v>493</v>
       </c>
       <c r="G34" s="21" t="s">
         <v>42</v>
@@ -11812,7 +12444,7 @@
         <v>33</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>437</v>
+        <v>494</v>
       </c>
       <c r="O34" s="21" t="s">
         <v>42</v>
@@ -11821,7 +12453,7 @@
         <v>33</v>
       </c>
       <c r="V34" s="20" t="s">
-        <v>438</v>
+        <v>495</v>
       </c>
       <c r="W34" s="21" t="s">
         <v>42</v>
@@ -11832,7 +12464,7 @@
         <v>34</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>439</v>
+        <v>496</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>58</v>
@@ -11841,7 +12473,7 @@
         <v>34</v>
       </c>
       <c r="N35" s="20" t="s">
-        <v>440</v>
+        <v>497</v>
       </c>
       <c r="O35" s="21" t="s">
         <v>58</v>
@@ -11850,7 +12482,7 @@
         <v>34</v>
       </c>
       <c r="V35" s="20" t="s">
-        <v>441</v>
+        <v>498</v>
       </c>
       <c r="W35" s="21" t="s">
         <v>58</v>
@@ -11861,7 +12493,7 @@
         <v>35</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>442</v>
+        <v>499</v>
       </c>
       <c r="G36" s="21" t="s">
         <v>71</v>
@@ -11870,7 +12502,7 @@
         <v>35</v>
       </c>
       <c r="N36" s="20" t="s">
-        <v>443</v>
+        <v>500</v>
       </c>
       <c r="O36" s="21" t="s">
         <v>71</v>
@@ -11879,7 +12511,7 @@
         <v>35</v>
       </c>
       <c r="V36" s="20" t="s">
-        <v>444</v>
+        <v>501</v>
       </c>
       <c r="W36" s="21" t="s">
         <v>71</v>
@@ -11890,7 +12522,7 @@
         <v>36</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>445</v>
+        <v>502</v>
       </c>
       <c r="G37" s="21" t="s">
         <v>84</v>
@@ -11899,7 +12531,7 @@
         <v>36</v>
       </c>
       <c r="N37" s="20" t="s">
-        <v>446</v>
+        <v>503</v>
       </c>
       <c r="O37" s="21" t="s">
         <v>84</v>
@@ -11908,7 +12540,7 @@
         <v>36</v>
       </c>
       <c r="V37" s="20" t="s">
-        <v>447</v>
+        <v>504</v>
       </c>
       <c r="W37" s="21" t="s">
         <v>84</v>
@@ -11919,7 +12551,7 @@
         <v>37</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>448</v>
+        <v>505</v>
       </c>
       <c r="G38" s="21" t="s">
         <v>97</v>
@@ -11928,7 +12560,7 @@
         <v>37</v>
       </c>
       <c r="N38" s="20" t="s">
-        <v>449</v>
+        <v>506</v>
       </c>
       <c r="O38" s="21" t="s">
         <v>97</v>
@@ -11937,7 +12569,7 @@
         <v>37</v>
       </c>
       <c r="V38" s="20" t="s">
-        <v>450</v>
+        <v>507</v>
       </c>
       <c r="W38" s="21" t="s">
         <v>97</v>
@@ -11948,7 +12580,7 @@
         <v>38</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>451</v>
+        <v>508</v>
       </c>
       <c r="G39" s="21" t="s">
         <v>110</v>
@@ -11957,7 +12589,7 @@
         <v>38</v>
       </c>
       <c r="N39" s="20" t="s">
-        <v>452</v>
+        <v>509</v>
       </c>
       <c r="O39" s="21" t="s">
         <v>110</v>
@@ -11966,7 +12598,7 @@
         <v>38</v>
       </c>
       <c r="V39" s="20" t="s">
-        <v>453</v>
+        <v>510</v>
       </c>
       <c r="W39" s="21" t="s">
         <v>110</v>
@@ -11977,7 +12609,7 @@
         <v>39</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>454</v>
+        <v>511</v>
       </c>
       <c r="G40" s="21" t="s">
         <v>123</v>
@@ -11986,7 +12618,7 @@
         <v>39</v>
       </c>
       <c r="N40" s="20" t="s">
-        <v>455</v>
+        <v>512</v>
       </c>
       <c r="O40" s="21" t="s">
         <v>123</v>
@@ -11995,7 +12627,7 @@
         <v>39</v>
       </c>
       <c r="V40" s="20" t="s">
-        <v>456</v>
+        <v>513</v>
       </c>
       <c r="W40" s="21" t="s">
         <v>123</v>
@@ -12006,7 +12638,7 @@
         <v>40</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>457</v>
+        <v>514</v>
       </c>
       <c r="G41" s="21" t="s">
         <v>136</v>
@@ -12015,7 +12647,7 @@
         <v>40</v>
       </c>
       <c r="N41" s="20" t="s">
-        <v>458</v>
+        <v>515</v>
       </c>
       <c r="O41" s="21" t="s">
         <v>136</v>
@@ -12024,7 +12656,7 @@
         <v>40</v>
       </c>
       <c r="V41" s="20" t="s">
-        <v>459</v>
+        <v>516</v>
       </c>
       <c r="W41" s="21" t="s">
         <v>136</v>
@@ -12035,7 +12667,7 @@
         <v>41</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>460</v>
+        <v>517</v>
       </c>
       <c r="G42" s="21" t="s">
         <v>42</v>
@@ -12044,7 +12676,7 @@
         <v>41</v>
       </c>
       <c r="N42" s="20" t="s">
-        <v>461</v>
+        <v>518</v>
       </c>
       <c r="O42" s="21" t="s">
         <v>42</v>
@@ -12053,7 +12685,7 @@
         <v>41</v>
       </c>
       <c r="V42" s="20" t="s">
-        <v>462</v>
+        <v>519</v>
       </c>
       <c r="W42" s="21" t="s">
         <v>42</v>
@@ -12064,7 +12696,7 @@
         <v>42</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>463</v>
+        <v>520</v>
       </c>
       <c r="G43" s="21" t="s">
         <v>58</v>
@@ -12073,7 +12705,7 @@
         <v>42</v>
       </c>
       <c r="N43" s="20" t="s">
-        <v>464</v>
+        <v>521</v>
       </c>
       <c r="O43" s="21" t="s">
         <v>58</v>
@@ -12082,7 +12714,7 @@
         <v>42</v>
       </c>
       <c r="V43" s="20" t="s">
-        <v>465</v>
+        <v>522</v>
       </c>
       <c r="W43" s="21" t="s">
         <v>58</v>
@@ -12093,7 +12725,7 @@
         <v>43</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>466</v>
+        <v>523</v>
       </c>
       <c r="G44" s="21" t="s">
         <v>71</v>
@@ -12102,7 +12734,7 @@
         <v>43</v>
       </c>
       <c r="N44" s="20" t="s">
-        <v>467</v>
+        <v>524</v>
       </c>
       <c r="O44" s="21" t="s">
         <v>71</v>
@@ -12111,7 +12743,7 @@
         <v>43</v>
       </c>
       <c r="V44" s="20" t="s">
-        <v>468</v>
+        <v>525</v>
       </c>
       <c r="W44" s="21" t="s">
         <v>71</v>
@@ -12122,7 +12754,7 @@
         <v>44</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>469</v>
+        <v>526</v>
       </c>
       <c r="G45" s="21" t="s">
         <v>84</v>
@@ -12131,7 +12763,7 @@
         <v>44</v>
       </c>
       <c r="N45" s="20" t="s">
-        <v>470</v>
+        <v>527</v>
       </c>
       <c r="O45" s="21" t="s">
         <v>84</v>
@@ -12140,7 +12772,7 @@
         <v>44</v>
       </c>
       <c r="V45" s="20" t="s">
-        <v>471</v>
+        <v>528</v>
       </c>
       <c r="W45" s="21" t="s">
         <v>84</v>
@@ -12151,7 +12783,7 @@
         <v>45</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>472</v>
+        <v>529</v>
       </c>
       <c r="G46" s="21" t="s">
         <v>97</v>
@@ -12160,7 +12792,7 @@
         <v>45</v>
       </c>
       <c r="N46" s="20" t="s">
-        <v>473</v>
+        <v>530</v>
       </c>
       <c r="O46" s="21" t="s">
         <v>97</v>
@@ -12169,7 +12801,7 @@
         <v>45</v>
       </c>
       <c r="V46" s="20" t="s">
-        <v>474</v>
+        <v>531</v>
       </c>
       <c r="W46" s="21" t="s">
         <v>97</v>
@@ -12180,7 +12812,7 @@
         <v>46</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>475</v>
+        <v>532</v>
       </c>
       <c r="G47" s="21" t="s">
         <v>110</v>
@@ -12189,7 +12821,7 @@
         <v>46</v>
       </c>
       <c r="N47" s="20" t="s">
-        <v>476</v>
+        <v>533</v>
       </c>
       <c r="O47" s="21" t="s">
         <v>110</v>
@@ -12198,7 +12830,7 @@
         <v>46</v>
       </c>
       <c r="V47" s="20" t="s">
-        <v>477</v>
+        <v>534</v>
       </c>
       <c r="W47" s="21" t="s">
         <v>110</v>
@@ -12209,7 +12841,7 @@
         <v>47</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>478</v>
+        <v>535</v>
       </c>
       <c r="G48" s="21" t="s">
         <v>123</v>
@@ -12218,7 +12850,7 @@
         <v>47</v>
       </c>
       <c r="N48" s="20" t="s">
-        <v>479</v>
+        <v>536</v>
       </c>
       <c r="O48" s="21" t="s">
         <v>123</v>
@@ -12227,7 +12859,7 @@
         <v>47</v>
       </c>
       <c r="V48" s="20" t="s">
-        <v>480</v>
+        <v>537</v>
       </c>
       <c r="W48" s="21" t="s">
         <v>123</v>
@@ -12238,7 +12870,7 @@
         <v>48</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>481</v>
+        <v>538</v>
       </c>
       <c r="G49" s="21" t="s">
         <v>136</v>
@@ -12247,7 +12879,7 @@
         <v>48</v>
       </c>
       <c r="N49" s="20" t="s">
-        <v>482</v>
+        <v>539</v>
       </c>
       <c r="O49" s="21" t="s">
         <v>136</v>
@@ -12256,7 +12888,7 @@
         <v>48</v>
       </c>
       <c r="V49" s="20" t="s">
-        <v>483</v>
+        <v>540</v>
       </c>
       <c r="W49" s="21" t="s">
         <v>136</v>
@@ -12267,7 +12899,7 @@
         <v>49</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>484</v>
+        <v>541</v>
       </c>
       <c r="G50" s="21" t="s">
         <v>42</v>
@@ -12276,7 +12908,7 @@
         <v>49</v>
       </c>
       <c r="N50" s="20" t="s">
-        <v>485</v>
+        <v>542</v>
       </c>
       <c r="O50" s="21" t="s">
         <v>42</v>
@@ -12285,7 +12917,7 @@
         <v>49</v>
       </c>
       <c r="V50" s="20" t="s">
-        <v>486</v>
+        <v>543</v>
       </c>
       <c r="W50" s="21" t="s">
         <v>42</v>
@@ -12296,7 +12928,7 @@
         <v>50</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>487</v>
+        <v>544</v>
       </c>
       <c r="G51" s="21" t="s">
         <v>58</v>
@@ -12305,7 +12937,7 @@
         <v>50</v>
       </c>
       <c r="N51" s="20" t="s">
-        <v>488</v>
+        <v>545</v>
       </c>
       <c r="O51" s="21" t="s">
         <v>58</v>
@@ -12314,7 +12946,7 @@
         <v>50</v>
       </c>
       <c r="V51" s="20" t="s">
-        <v>489</v>
+        <v>546</v>
       </c>
       <c r="W51" s="21" t="s">
         <v>58</v>
@@ -12325,7 +12957,7 @@
         <v>51</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>490</v>
+        <v>547</v>
       </c>
       <c r="G52" s="21" t="s">
         <v>71</v>
@@ -12334,7 +12966,7 @@
         <v>51</v>
       </c>
       <c r="N52" s="20" t="s">
-        <v>491</v>
+        <v>548</v>
       </c>
       <c r="O52" s="21" t="s">
         <v>71</v>
@@ -12343,7 +12975,7 @@
         <v>51</v>
       </c>
       <c r="V52" s="20" t="s">
-        <v>492</v>
+        <v>549</v>
       </c>
       <c r="W52" s="21" t="s">
         <v>71</v>
@@ -12354,7 +12986,7 @@
         <v>52</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>493</v>
+        <v>550</v>
       </c>
       <c r="G53" s="21" t="s">
         <v>84</v>
@@ -12363,7 +12995,7 @@
         <v>52</v>
       </c>
       <c r="N53" s="20" t="s">
-        <v>494</v>
+        <v>551</v>
       </c>
       <c r="O53" s="21" t="s">
         <v>84</v>
@@ -12372,7 +13004,7 @@
         <v>52</v>
       </c>
       <c r="V53" s="20" t="s">
-        <v>495</v>
+        <v>552</v>
       </c>
       <c r="W53" s="21" t="s">
         <v>84</v>
@@ -12383,7 +13015,7 @@
         <v>53</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>496</v>
+        <v>553</v>
       </c>
       <c r="G54" s="21" t="s">
         <v>97</v>
@@ -12392,7 +13024,7 @@
         <v>53</v>
       </c>
       <c r="N54" s="20" t="s">
-        <v>497</v>
+        <v>554</v>
       </c>
       <c r="O54" s="21" t="s">
         <v>97</v>
@@ -12401,7 +13033,7 @@
         <v>53</v>
       </c>
       <c r="V54" s="20" t="s">
-        <v>498</v>
+        <v>555</v>
       </c>
       <c r="W54" s="21" t="s">
         <v>97</v>
@@ -12412,7 +13044,7 @@
         <v>54</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>499</v>
+        <v>556</v>
       </c>
       <c r="G55" s="21" t="s">
         <v>110</v>
@@ -12421,7 +13053,7 @@
         <v>54</v>
       </c>
       <c r="N55" s="20" t="s">
-        <v>500</v>
+        <v>557</v>
       </c>
       <c r="O55" s="21" t="s">
         <v>110</v>
@@ -12430,7 +13062,7 @@
         <v>54</v>
       </c>
       <c r="V55" s="20" t="s">
-        <v>501</v>
+        <v>558</v>
       </c>
       <c r="W55" s="21" t="s">
         <v>110</v>
@@ -12441,7 +13073,7 @@
         <v>55</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>502</v>
+        <v>559</v>
       </c>
       <c r="G56" s="21" t="s">
         <v>123</v>
@@ -12450,7 +13082,7 @@
         <v>55</v>
       </c>
       <c r="N56" s="20" t="s">
-        <v>503</v>
+        <v>560</v>
       </c>
       <c r="O56" s="21" t="s">
         <v>123</v>
@@ -12459,7 +13091,7 @@
         <v>55</v>
       </c>
       <c r="V56" s="20" t="s">
-        <v>504</v>
+        <v>561</v>
       </c>
       <c r="W56" s="21" t="s">
         <v>123</v>
@@ -12470,7 +13102,7 @@
         <v>56</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>505</v>
+        <v>562</v>
       </c>
       <c r="G57" s="21" t="s">
         <v>136</v>
@@ -12479,7 +13111,7 @@
         <v>56</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>506</v>
+        <v>563</v>
       </c>
       <c r="O57" s="21" t="s">
         <v>136</v>
@@ -12488,7 +13120,7 @@
         <v>56</v>
       </c>
       <c r="V57" s="20" t="s">
-        <v>507</v>
+        <v>564</v>
       </c>
       <c r="W57" s="21" t="s">
         <v>136</v>
@@ -12499,7 +13131,7 @@
         <v>57</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>508</v>
+        <v>565</v>
       </c>
       <c r="G58" s="21" t="s">
         <v>42</v>
@@ -12508,7 +13140,7 @@
         <v>57</v>
       </c>
       <c r="N58" s="20" t="s">
-        <v>509</v>
+        <v>566</v>
       </c>
       <c r="O58" s="21" t="s">
         <v>42</v>
@@ -12517,7 +13149,7 @@
         <v>57</v>
       </c>
       <c r="V58" s="20" t="s">
-        <v>510</v>
+        <v>567</v>
       </c>
       <c r="W58" s="21" t="s">
         <v>42</v>
@@ -12528,7 +13160,7 @@
         <v>58</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>511</v>
+        <v>568</v>
       </c>
       <c r="G59" s="21" t="s">
         <v>58</v>
@@ -12537,7 +13169,7 @@
         <v>58</v>
       </c>
       <c r="N59" s="20" t="s">
-        <v>512</v>
+        <v>569</v>
       </c>
       <c r="O59" s="21" t="s">
         <v>58</v>
@@ -12546,7 +13178,7 @@
         <v>58</v>
       </c>
       <c r="V59" s="20" t="s">
-        <v>513</v>
+        <v>570</v>
       </c>
       <c r="W59" s="21" t="s">
         <v>58</v>
@@ -12557,7 +13189,7 @@
         <v>59</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>514</v>
+        <v>571</v>
       </c>
       <c r="G60" s="21" t="s">
         <v>71</v>
@@ -12566,7 +13198,7 @@
         <v>59</v>
       </c>
       <c r="N60" s="20" t="s">
-        <v>515</v>
+        <v>572</v>
       </c>
       <c r="O60" s="21" t="s">
         <v>71</v>
@@ -12575,7 +13207,7 @@
         <v>59</v>
       </c>
       <c r="V60" s="20" t="s">
-        <v>516</v>
+        <v>573</v>
       </c>
       <c r="W60" s="21" t="s">
         <v>71</v>
@@ -12586,7 +13218,7 @@
         <v>60</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>517</v>
+        <v>574</v>
       </c>
       <c r="G61" s="21" t="s">
         <v>84</v>
@@ -12595,7 +13227,7 @@
         <v>60</v>
       </c>
       <c r="N61" s="20" t="s">
-        <v>518</v>
+        <v>575</v>
       </c>
       <c r="O61" s="21" t="s">
         <v>84</v>
@@ -12604,7 +13236,7 @@
         <v>60</v>
       </c>
       <c r="V61" s="20" t="s">
-        <v>519</v>
+        <v>576</v>
       </c>
       <c r="W61" s="21" t="s">
         <v>84</v>
@@ -12615,7 +13247,7 @@
         <v>61</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>520</v>
+        <v>577</v>
       </c>
       <c r="G62" s="21" t="s">
         <v>97</v>
@@ -12624,7 +13256,7 @@
         <v>61</v>
       </c>
       <c r="N62" s="20" t="s">
-        <v>521</v>
+        <v>578</v>
       </c>
       <c r="O62" s="21" t="s">
         <v>97</v>
@@ -12633,7 +13265,7 @@
         <v>61</v>
       </c>
       <c r="V62" s="20" t="s">
-        <v>522</v>
+        <v>579</v>
       </c>
       <c r="W62" s="21" t="s">
         <v>97</v>
@@ -12644,7 +13276,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>523</v>
+        <v>580</v>
       </c>
       <c r="G63" s="21" t="s">
         <v>110</v>
@@ -12653,7 +13285,7 @@
         <v>62</v>
       </c>
       <c r="N63" s="20" t="s">
-        <v>524</v>
+        <v>581</v>
       </c>
       <c r="O63" s="21" t="s">
         <v>110</v>
@@ -12662,7 +13294,7 @@
         <v>62</v>
       </c>
       <c r="V63" s="20" t="s">
-        <v>525</v>
+        <v>582</v>
       </c>
       <c r="W63" s="21" t="s">
         <v>110</v>
@@ -12680,7 +13312,7 @@
       <c r="W65" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C25 G2:G65 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33">
+  <conditionalFormatting sqref="C2:C25 G2:G65 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33 AE2:AE17 AI2:AI17 AM2:AM17">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"purple"</formula>
     </cfRule>
@@ -12704,7 +13336,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C25 G2:G34 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33 G35:G65" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C18 G2:G26 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33 AE2:AE17 AI2:AI17 AM2:AM17 C19:C25 G27:G65" type="list">
       <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12726,7 +13358,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -12738,25 +13370,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>526</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>527</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>528</v>
+      <c r="A1" s="18" t="s">
+        <v>583</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>529</v>
+        <v>586</v>
       </c>
       <c r="B2" s="8" t="n">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>530</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
1st row at Groups Tab colored
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -1799,7 +1799,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1830,8 +1830,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1866,6 +1874,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFAFD095"/>
         <bgColor rgb="FFB3B3B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3838"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFB7B3CA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF3366FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1467E"/>
+        <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1910,7 +1948,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1975,15 +2013,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2093,12 +2143,12 @@
       <rgbColor rgb="FFB7B3CA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF7030A0"/>
+      <rgbColor rgb="FFA1467E"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFC6D9F1"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -2112,24 +2162,24 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFB3B3B3"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFB66C"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FF558ED5"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF7030A0"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
@@ -2144,8 +2194,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6829,8 +6879,8 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6838,8 +6888,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="4.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="5" style="2" width="3.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="2" width="3.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="3.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="3.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="6.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="2" width="3.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="3.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="6.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="2" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="3.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="3.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="3.57"/>
@@ -9884,8 +9940,8 @@
   </sheetPr>
   <dimension ref="A1:AM65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL17" activeCellId="0" sqref="AL17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9897,7 +9953,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="12.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="13.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.8"/>
@@ -9908,3408 +9964,3408 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="14.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="16" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="14.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="16.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="14.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="15.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="17" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="17" t="s">
+      <c r="P1" s="17"/>
+      <c r="Q1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="S1" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="T1" s="18"/>
-      <c r="U1" s="17" t="s">
+      <c r="T1" s="17"/>
+      <c r="U1" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="V1" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="W1" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="17" t="s">
+      <c r="X1" s="17"/>
+      <c r="Y1" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="Z1" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AA1" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AC1" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AD1" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE1" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="AG1" s="17" t="s">
+      <c r="AG1" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="AH1" s="17" t="s">
+      <c r="AH1" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="AI1" s="17" t="s">
+      <c r="AI1" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="AK1" s="17" t="s">
+      <c r="AK1" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AL1" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AM1" s="21" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="n">
+      <c r="A2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="19" t="n">
+      <c r="I2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="19" t="n">
+      <c r="M2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="19" t="n">
+      <c r="Q2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="19" t="n">
+      <c r="U2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="V2" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="19" t="n">
+      <c r="Y2" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="Z2" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="AA2" s="21" t="s">
+      <c r="AA2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" s="16" t="n">
+      <c r="AC2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="AE2" s="21" t="s">
+      <c r="AE2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AG2" s="16" t="n">
+      <c r="AG2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AH2" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="AI2" s="21" t="s">
+      <c r="AI2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="16" t="n">
+      <c r="AK2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AL2" s="0" t="s">
+      <c r="AL2" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AM2" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="n">
+      <c r="A3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="19" t="n">
+      <c r="E3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="I3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="19" t="n">
+      <c r="M3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" s="19" t="n">
+      <c r="Q3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="19" t="n">
+      <c r="U3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="V3" s="20" t="s">
+      <c r="V3" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Y3" s="19" t="n">
+      <c r="Y3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="Z3" s="20" t="s">
+      <c r="Z3" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="AA3" s="21" t="s">
+      <c r="AA3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="16" t="n">
+      <c r="AC3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="AE3" s="21" t="s">
+      <c r="AE3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AG3" s="16" t="n">
+      <c r="AG3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AH3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="AI3" s="21" t="s">
+      <c r="AI3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AK3" s="16" t="n">
+      <c r="AK3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AL3" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="AM3" s="21" t="s">
+      <c r="AM3" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="n">
+      <c r="A4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="19" t="n">
+      <c r="E4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="19" t="n">
+      <c r="I4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="19" t="n">
+      <c r="M4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Q4" s="19" t="n">
+      <c r="Q4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U4" s="19" t="n">
+      <c r="U4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="V4" s="20" t="s">
+      <c r="V4" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Y4" s="19" t="n">
+      <c r="Y4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="Z4" s="20" t="s">
+      <c r="Z4" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="AA4" s="21" t="s">
+      <c r="AA4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AC4" s="16" t="n">
+      <c r="AC4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="AD4" s="0" t="s">
+      <c r="AD4" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="AE4" s="21" t="s">
+      <c r="AE4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AG4" s="16" t="n">
+      <c r="AG4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="AH4" s="0" t="s">
+      <c r="AH4" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AI4" s="21" t="s">
+      <c r="AI4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AK4" s="16" t="n">
+      <c r="AK4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="AL4" s="0" t="s">
+      <c r="AL4" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AM4" s="21" t="s">
+      <c r="AM4" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="n">
+      <c r="A5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="19" t="n">
+      <c r="E5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="19" t="n">
+      <c r="I5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="19" t="n">
+      <c r="M5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Q5" s="19" t="n">
+      <c r="Q5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="R5" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U5" s="19" t="n">
+      <c r="U5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="V5" s="20" t="s">
+      <c r="V5" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="W5" s="21" t="s">
+      <c r="W5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="19" t="n">
+      <c r="Y5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="Z5" s="20" t="s">
+      <c r="Z5" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="AA5" s="21" t="s">
+      <c r="AA5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AC5" s="16" t="n">
+      <c r="AC5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="AD5" s="0" t="s">
+      <c r="AD5" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AE5" s="21" t="s">
+      <c r="AE5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AG5" s="16" t="n">
+      <c r="AG5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="AH5" s="0" t="s">
+      <c r="AH5" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AI5" s="21" t="s">
+      <c r="AI5" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AK5" s="16" t="n">
+      <c r="AK5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="AL5" s="0" t="s">
+      <c r="AL5" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AM5" s="21" t="s">
+      <c r="AM5" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="E6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="J6" s="20" t="s">
+      <c r="I6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" s="20" t="s">
+      <c r="M6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Q6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="R6" s="20" t="s">
+      <c r="Q6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="R6" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="S6" s="21" t="s">
+      <c r="S6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="V6" s="20" t="s">
+      <c r="U6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="V6" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="W6" s="21" t="s">
+      <c r="W6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Y6" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="Z6" s="20" t="s">
+      <c r="Y6" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="AA6" s="21" t="s">
+      <c r="AA6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AC6" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD6" s="0" t="s">
+      <c r="AC6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="AE6" s="21" t="s">
+      <c r="AE6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AG6" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH6" s="0" t="s">
+      <c r="AG6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="AI6" s="21" t="s">
+      <c r="AI6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AK6" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="AL6" s="0" t="s">
+      <c r="AK6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="AM6" s="21" t="s">
+      <c r="AM6" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="n">
+      <c r="A7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="24" t="s">
         <v>110</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="19" t="n">
+      <c r="E7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="19" t="n">
+      <c r="I7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="19" t="n">
+      <c r="M7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Q7" s="19" t="n">
+      <c r="Q7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="S7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U7" s="19" t="n">
+      <c r="U7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="V7" s="20" t="s">
+      <c r="V7" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="W7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Y7" s="19" t="n">
+      <c r="Y7" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="Z7" s="20" t="s">
+      <c r="Z7" s="23" t="s">
         <v>288</v>
       </c>
-      <c r="AA7" s="21" t="s">
+      <c r="AA7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AC7" s="16" t="n">
+      <c r="AC7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="AD7" s="0" t="s">
+      <c r="AD7" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="AE7" s="21" t="s">
+      <c r="AE7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AG7" s="16" t="n">
+      <c r="AG7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="AH7" s="0" t="s">
+      <c r="AH7" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="AI7" s="21" t="s">
+      <c r="AI7" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AK7" s="16" t="n">
+      <c r="AK7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="AL7" s="0" t="s">
+      <c r="AL7" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="AM7" s="21" t="s">
+      <c r="AM7" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="n">
+      <c r="A8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="I8" s="19" t="n">
+      <c r="I8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M8" s="19" t="n">
+      <c r="M8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Q8" s="19" t="n">
+      <c r="Q8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="R8" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="S8" s="21" t="s">
+      <c r="S8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U8" s="19" t="n">
+      <c r="U8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="V8" s="20" t="s">
+      <c r="V8" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="W8" s="21" t="s">
+      <c r="W8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Y8" s="19" t="n">
+      <c r="Y8" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="Z8" s="20" t="s">
+      <c r="Z8" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="AA8" s="21" t="s">
+      <c r="AA8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AC8" s="16" t="n">
+      <c r="AC8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="AD8" s="0" t="s">
+      <c r="AD8" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AE8" s="21" t="s">
+      <c r="AE8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AG8" s="16" t="n">
+      <c r="AG8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="AH8" s="0" t="s">
+      <c r="AH8" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AI8" s="21" t="s">
+      <c r="AI8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AK8" s="16" t="n">
+      <c r="AK8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="AL8" s="0" t="s">
+      <c r="AL8" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AM8" s="21" t="s">
+      <c r="AM8" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="n">
+      <c r="A9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="19" t="n">
+      <c r="E9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="19" t="n">
+      <c r="I9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M9" s="19" t="n">
+      <c r="M9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="N9" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="O9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="Q9" s="19" t="n">
+      <c r="Q9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="R9" s="20" t="s">
+      <c r="R9" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="S9" s="21" t="s">
+      <c r="S9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="U9" s="19" t="n">
+      <c r="U9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="V9" s="20" t="s">
+      <c r="V9" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="W9" s="21" t="s">
+      <c r="W9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="Y9" s="19" t="n">
+      <c r="Y9" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="Z9" s="20" t="s">
+      <c r="Z9" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="AA9" s="21" t="s">
+      <c r="AA9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AC9" s="16" t="n">
+      <c r="AC9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="AD9" s="0" t="s">
+      <c r="AD9" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="AE9" s="21" t="s">
+      <c r="AE9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AG9" s="16" t="n">
+      <c r="AG9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="AH9" s="0" t="s">
+      <c r="AH9" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="AI9" s="21" t="s">
+      <c r="AI9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AK9" s="16" t="n">
+      <c r="AK9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="AL9" s="0" t="s">
+      <c r="AL9" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="AM9" s="21" t="s">
+      <c r="AM9" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="n">
+      <c r="A10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="19" t="n">
+      <c r="E10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="19" t="n">
+      <c r="I10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="19" t="n">
+      <c r="M10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q10" s="19" t="n">
+      <c r="Q10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="R10" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="S10" s="21" t="s">
+      <c r="S10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U10" s="19" t="n">
+      <c r="U10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="V10" s="20" t="s">
+      <c r="V10" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="W10" s="21" t="s">
+      <c r="W10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Y10" s="19" t="n">
+      <c r="Y10" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="Z10" s="20" t="s">
+      <c r="Z10" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="AA10" s="21" t="s">
+      <c r="AA10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AC10" s="16" t="n">
+      <c r="AC10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="AD10" s="0" t="s">
+      <c r="AD10" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="AE10" s="21" t="s">
+      <c r="AE10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AG10" s="16" t="n">
+      <c r="AG10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="AH10" s="0" t="s">
+      <c r="AH10" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="AI10" s="21" t="s">
+      <c r="AI10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AK10" s="16" t="n">
+      <c r="AK10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="AL10" s="0" t="s">
+      <c r="AL10" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="AM10" s="21" t="s">
+      <c r="AM10" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="n">
+      <c r="A11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="19" t="n">
+      <c r="E11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="19" t="n">
+      <c r="I11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M11" s="19" t="n">
+      <c r="M11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Q11" s="19" t="n">
+      <c r="Q11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="S11" s="21" t="s">
+      <c r="S11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U11" s="19" t="n">
+      <c r="U11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="V11" s="20" t="s">
+      <c r="V11" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="W11" s="21" t="s">
+      <c r="W11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Y11" s="19" t="n">
+      <c r="Y11" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="Z11" s="20" t="s">
+      <c r="Z11" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="AA11" s="21" t="s">
+      <c r="AA11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AC11" s="16" t="n">
+      <c r="AC11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="AD11" s="0" t="s">
+      <c r="AD11" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="AE11" s="21" t="s">
+      <c r="AE11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AG11" s="16" t="n">
+      <c r="AG11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="AH11" s="0" t="s">
+      <c r="AH11" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="AI11" s="21" t="s">
+      <c r="AI11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AK11" s="16" t="n">
+      <c r="AK11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="AL11" s="0" t="s">
+      <c r="AL11" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="AM11" s="21" t="s">
+      <c r="AM11" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="n">
+      <c r="A12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="19" t="n">
+      <c r="E12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="19" t="n">
+      <c r="I12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="19" t="n">
+      <c r="M12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Q12" s="19" t="n">
+      <c r="Q12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="S12" s="21" t="s">
+      <c r="S12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U12" s="19" t="n">
+      <c r="U12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="V12" s="20" t="s">
+      <c r="V12" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="W12" s="21" t="s">
+      <c r="W12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Y12" s="19" t="n">
+      <c r="Y12" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="Z12" s="20" t="s">
+      <c r="Z12" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="AA12" s="21" t="s">
+      <c r="AA12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AC12" s="16" t="n">
+      <c r="AC12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="AD12" s="0" t="s">
+      <c r="AD12" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="AE12" s="21" t="s">
+      <c r="AE12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AG12" s="16" t="n">
+      <c r="AG12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="AH12" s="0" t="s">
+      <c r="AH12" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="AI12" s="21" t="s">
+      <c r="AI12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AK12" s="16" t="n">
+      <c r="AK12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="AL12" s="0" t="s">
+      <c r="AL12" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="AM12" s="21" t="s">
+      <c r="AM12" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="n">
+      <c r="A13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="19" t="n">
+      <c r="E13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="19" t="n">
+      <c r="I13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M13" s="19" t="n">
+      <c r="M13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Q13" s="19" t="n">
+      <c r="Q13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="S13" s="21" t="s">
+      <c r="S13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U13" s="19" t="n">
+      <c r="U13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="V13" s="20" t="s">
+      <c r="V13" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="W13" s="21" t="s">
+      <c r="W13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Y13" s="19" t="n">
+      <c r="Y13" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="Z13" s="20" t="s">
+      <c r="Z13" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="AA13" s="21" t="s">
+      <c r="AA13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AC13" s="16" t="n">
+      <c r="AC13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="AD13" s="0" t="s">
+      <c r="AD13" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="AE13" s="21" t="s">
+      <c r="AE13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AG13" s="16" t="n">
+      <c r="AG13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="AH13" s="0" t="s">
+      <c r="AH13" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="AI13" s="21" t="s">
+      <c r="AI13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AK13" s="16" t="n">
+      <c r="AK13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="AL13" s="0" t="s">
+      <c r="AL13" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="AM13" s="21" t="s">
+      <c r="AM13" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="n">
+      <c r="A14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="23" t="s">
         <v>352</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="19" t="n">
+      <c r="E14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="23" t="s">
         <v>353</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="19" t="n">
+      <c r="I14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M14" s="19" t="n">
+      <c r="M14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="N14" s="20" t="s">
+      <c r="N14" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Q14" s="19" t="n">
+      <c r="Q14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="S14" s="21" t="s">
+      <c r="S14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U14" s="19" t="n">
+      <c r="U14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="V14" s="20" t="s">
+      <c r="V14" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="W14" s="21" t="s">
+      <c r="W14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Y14" s="19" t="n">
+      <c r="Y14" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="Z14" s="20" t="s">
+      <c r="Z14" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="AA14" s="21" t="s">
+      <c r="AA14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AC14" s="16" t="n">
+      <c r="AC14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="AD14" s="0" t="s">
+      <c r="AD14" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="AE14" s="21" t="s">
+      <c r="AE14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AG14" s="16" t="n">
+      <c r="AG14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="AH14" s="0" t="s">
+      <c r="AH14" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="AI14" s="21" t="s">
+      <c r="AI14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AK14" s="16" t="n">
+      <c r="AK14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="AL14" s="0" t="s">
+      <c r="AL14" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="AM14" s="21" t="s">
+      <c r="AM14" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="n">
+      <c r="A15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="E15" s="19" t="n">
+      <c r="E15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I15" s="19" t="n">
+      <c r="I15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="19" t="n">
+      <c r="M15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="N15" s="20" t="s">
+      <c r="N15" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="O15" s="21" t="s">
+      <c r="O15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Q15" s="19" t="n">
+      <c r="Q15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="R15" s="20" t="s">
+      <c r="R15" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="S15" s="21" t="s">
+      <c r="S15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U15" s="19" t="n">
+      <c r="U15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="V15" s="20" t="s">
+      <c r="V15" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="W15" s="21" t="s">
+      <c r="W15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Y15" s="19" t="n">
+      <c r="Y15" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="Z15" s="20" t="s">
+      <c r="Z15" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="AA15" s="21" t="s">
+      <c r="AA15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AC15" s="16" t="n">
+      <c r="AC15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="AD15" s="0" t="s">
+      <c r="AD15" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="AE15" s="21" t="s">
+      <c r="AE15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AG15" s="16" t="n">
+      <c r="AG15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="AH15" s="0" t="s">
+      <c r="AH15" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="AI15" s="21" t="s">
+      <c r="AI15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AK15" s="16" t="n">
+      <c r="AK15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="AL15" s="0" t="s">
+      <c r="AL15" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="AM15" s="21" t="s">
+      <c r="AM15" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="n">
+      <c r="A16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E16" s="19" t="n">
+      <c r="E16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="I16" s="19" t="n">
+      <c r="I16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="J16" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M16" s="19" t="n">
+      <c r="M16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="N16" s="20" t="s">
+      <c r="N16" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="O16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Q16" s="19" t="n">
+      <c r="Q16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="R16" s="20" t="s">
+      <c r="R16" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="S16" s="21" t="s">
+      <c r="S16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U16" s="19" t="n">
+      <c r="U16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="V16" s="20" t="s">
+      <c r="V16" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="W16" s="21" t="s">
+      <c r="W16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Y16" s="19" t="n">
+      <c r="Y16" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="Z16" s="20" t="s">
+      <c r="Z16" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="AA16" s="21" t="s">
+      <c r="AA16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AC16" s="16" t="n">
+      <c r="AC16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="AD16" s="0" t="s">
+      <c r="AD16" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="AE16" s="21" t="s">
+      <c r="AE16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AG16" s="16" t="n">
+      <c r="AG16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="AH16" s="0" t="s">
+      <c r="AH16" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="AI16" s="21" t="s">
+      <c r="AI16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AK16" s="16" t="n">
+      <c r="AK16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="AL16" s="0" t="s">
+      <c r="AL16" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="AM16" s="21" t="s">
+      <c r="AM16" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="n">
+      <c r="A17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="19" t="n">
+      <c r="E17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="I17" s="19" t="n">
+      <c r="I17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M17" s="19" t="n">
+      <c r="M17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="N17" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="O17" s="21" t="s">
+      <c r="O17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="19" t="n">
+      <c r="Q17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="R17" s="20" t="s">
+      <c r="R17" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="S17" s="21" t="s">
+      <c r="S17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="U17" s="19" t="n">
+      <c r="U17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="V17" s="20" t="s">
+      <c r="V17" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="W17" s="21" t="s">
+      <c r="W17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="Y17" s="19" t="n">
+      <c r="Y17" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="Z17" s="20" t="s">
+      <c r="Z17" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="AA17" s="21" t="s">
+      <c r="AA17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AC17" s="16" t="n">
+      <c r="AC17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="AD17" s="0" t="s">
+      <c r="AD17" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="AE17" s="21" t="s">
+      <c r="AE17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AG17" s="16" t="n">
+      <c r="AG17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="AH17" s="0" t="s">
+      <c r="AH17" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="AI17" s="21" t="s">
+      <c r="AI17" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AK17" s="16" t="n">
+      <c r="AK17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="AL17" s="0" t="s">
+      <c r="AL17" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="AM17" s="21" t="s">
+      <c r="AM17" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="n">
+      <c r="A18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="19" t="n">
+      <c r="E18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="19" t="n">
+      <c r="I18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="K18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M18" s="19" t="n">
+      <c r="M18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="N18" s="20" t="s">
+      <c r="N18" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="O18" s="21" t="s">
+      <c r="O18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q18" s="19" t="n">
+      <c r="Q18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="R18" s="20" t="s">
+      <c r="R18" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="S18" s="21" t="s">
+      <c r="S18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U18" s="19" t="n">
+      <c r="U18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="V18" s="20" t="s">
+      <c r="V18" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="W18" s="21" t="s">
+      <c r="W18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Y18" s="19" t="n">
+      <c r="Y18" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="Z18" s="20" t="s">
+      <c r="Z18" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="AA18" s="21" t="s">
+      <c r="AA18" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="n">
+      <c r="A19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="19" t="n">
+      <c r="E19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="19" t="n">
+      <c r="I19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="K19" s="21" t="s">
+      <c r="K19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M19" s="19" t="n">
+      <c r="M19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="N19" s="20" t="s">
+      <c r="N19" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="O19" s="21" t="s">
+      <c r="O19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Q19" s="19" t="n">
+      <c r="Q19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="R19" s="20" t="s">
+      <c r="R19" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="S19" s="21" t="s">
+      <c r="S19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="19" t="n">
+      <c r="U19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="V19" s="20" t="s">
+      <c r="V19" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="W19" s="21" t="s">
+      <c r="W19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Y19" s="19" t="n">
+      <c r="Y19" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="Z19" s="20" t="s">
+      <c r="Z19" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="AA19" s="21" t="s">
+      <c r="AA19" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="n">
+      <c r="A20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="19" t="n">
+      <c r="E20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="19" t="n">
+      <c r="I20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="K20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M20" s="19" t="n">
+      <c r="M20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="N20" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="O20" s="21" t="s">
+      <c r="O20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Q20" s="19" t="n">
+      <c r="Q20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="R20" s="20" t="s">
+      <c r="R20" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="S20" s="21" t="s">
+      <c r="S20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U20" s="19" t="n">
+      <c r="U20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="V20" s="20" t="s">
+      <c r="V20" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="W20" s="21" t="s">
+      <c r="W20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Y20" s="19" t="n">
+      <c r="Y20" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="Z20" s="20" t="s">
+      <c r="Z20" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="AA20" s="21" t="s">
+      <c r="AA20" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="n">
+      <c r="A21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="23" t="s">
         <v>413</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="19" t="n">
+      <c r="E21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="19" t="n">
+      <c r="I21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="23" t="s">
         <v>415</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="K21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M21" s="19" t="n">
+      <c r="M21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="N21" s="20" t="s">
+      <c r="N21" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="O21" s="21" t="s">
+      <c r="O21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Q21" s="19" t="n">
+      <c r="Q21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="R21" s="20" t="s">
+      <c r="R21" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="S21" s="21" t="s">
+      <c r="S21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U21" s="19" t="n">
+      <c r="U21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="V21" s="20" t="s">
+      <c r="V21" s="23" t="s">
         <v>418</v>
       </c>
-      <c r="W21" s="21" t="s">
+      <c r="W21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Y21" s="19" t="n">
+      <c r="Y21" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="Z21" s="20" t="s">
+      <c r="Z21" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="AA21" s="21" t="s">
+      <c r="AA21" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="n">
+      <c r="A22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="19" t="n">
+      <c r="E22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="I22" s="19" t="n">
+      <c r="I22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="K22" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M22" s="19" t="n">
+      <c r="M22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="N22" s="23" t="s">
         <v>423</v>
       </c>
-      <c r="O22" s="21" t="s">
+      <c r="O22" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Q22" s="19" t="n">
+      <c r="Q22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="R22" s="20" t="s">
+      <c r="R22" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="S22" s="21" t="s">
+      <c r="S22" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U22" s="19" t="n">
+      <c r="U22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="V22" s="20" t="s">
+      <c r="V22" s="23" t="s">
         <v>425</v>
       </c>
-      <c r="W22" s="21" t="s">
+      <c r="W22" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Y22" s="19" t="n">
+      <c r="Y22" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="Z22" s="20" t="s">
+      <c r="Z22" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="AA22" s="21" t="s">
+      <c r="AA22" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19" t="n">
+      <c r="A23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="E23" s="19" t="n">
+      <c r="E23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I23" s="19" t="n">
+      <c r="I23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="23" t="s">
         <v>429</v>
       </c>
-      <c r="K23" s="21" t="s">
+      <c r="K23" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M23" s="19" t="n">
+      <c r="M23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="N23" s="23" t="s">
         <v>430</v>
       </c>
-      <c r="O23" s="21" t="s">
+      <c r="O23" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Q23" s="19" t="n">
+      <c r="Q23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="R23" s="20" t="s">
+      <c r="R23" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="S23" s="21" t="s">
+      <c r="S23" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U23" s="19" t="n">
+      <c r="U23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="V23" s="20" t="s">
+      <c r="V23" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="W23" s="21" t="s">
+      <c r="W23" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Y23" s="19" t="n">
+      <c r="Y23" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="Z23" s="20" t="s">
+      <c r="Z23" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="AA23" s="21" t="s">
+      <c r="AA23" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="n">
+      <c r="A24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="23" t="s">
         <v>434</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="19" t="n">
+      <c r="E24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="19" t="n">
+      <c r="I24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="J24" s="20" t="s">
+      <c r="J24" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="K24" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="19" t="n">
+      <c r="M24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="N24" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="O24" s="21" t="s">
+      <c r="O24" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Q24" s="19" t="n">
+      <c r="Q24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="R24" s="20" t="s">
+      <c r="R24" s="23" t="s">
         <v>438</v>
       </c>
-      <c r="S24" s="21" t="s">
+      <c r="S24" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U24" s="19" t="n">
+      <c r="U24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="V24" s="20" t="s">
+      <c r="V24" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="W24" s="21" t="s">
+      <c r="W24" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Y24" s="19" t="n">
+      <c r="Y24" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="Z24" s="20" t="s">
+      <c r="Z24" s="23" t="s">
         <v>440</v>
       </c>
-      <c r="AA24" s="21" t="s">
+      <c r="AA24" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="n">
+      <c r="A25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="23" t="s">
         <v>441</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="19" t="n">
+      <c r="E25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="I25" s="19" t="n">
+      <c r="I25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="K25" s="21" t="s">
+      <c r="K25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M25" s="19" t="n">
+      <c r="M25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="N25" s="20" t="s">
+      <c r="N25" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="O25" s="21" t="s">
+      <c r="O25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="Q25" s="19" t="n">
+      <c r="Q25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="R25" s="20" t="s">
+      <c r="R25" s="23" t="s">
         <v>445</v>
       </c>
-      <c r="S25" s="21" t="s">
+      <c r="S25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="U25" s="19" t="n">
+      <c r="U25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="V25" s="20" t="s">
+      <c r="V25" s="23" t="s">
         <v>446</v>
       </c>
-      <c r="W25" s="21" t="s">
+      <c r="W25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="Y25" s="19" t="n">
+      <c r="Y25" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="Z25" s="20" t="s">
+      <c r="Z25" s="23" t="s">
         <v>447</v>
       </c>
-      <c r="AA25" s="21" t="s">
+      <c r="AA25" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="19" t="n">
+      <c r="E26" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="23" t="s">
         <v>448</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="19" t="n">
+      <c r="I26" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="J26" s="20" t="s">
+      <c r="J26" s="23" t="s">
         <v>449</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M26" s="19" t="n">
+      <c r="M26" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="N26" s="20" t="s">
+      <c r="N26" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q26" s="19" t="n">
+      <c r="Q26" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="R26" s="20" t="s">
+      <c r="R26" s="23" t="s">
         <v>451</v>
       </c>
-      <c r="S26" s="21" t="s">
+      <c r="S26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U26" s="19" t="n">
+      <c r="U26" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="V26" s="20" t="s">
+      <c r="V26" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="W26" s="21" t="s">
+      <c r="W26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Y26" s="19" t="n">
+      <c r="Y26" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="Z26" s="20" t="s">
+      <c r="Z26" s="23" t="s">
         <v>453</v>
       </c>
-      <c r="AA26" s="21" t="s">
+      <c r="AA26" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="19" t="n">
+      <c r="E27" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="23" t="s">
         <v>454</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I27" s="19" t="n">
+      <c r="I27" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="J27" s="20" t="s">
+      <c r="J27" s="23" t="s">
         <v>455</v>
       </c>
-      <c r="K27" s="21" t="s">
+      <c r="K27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M27" s="19" t="n">
+      <c r="M27" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="N27" s="20" t="s">
+      <c r="N27" s="23" t="s">
         <v>456</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Q27" s="19" t="n">
+      <c r="Q27" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="R27" s="20" t="s">
+      <c r="R27" s="23" t="s">
         <v>457</v>
       </c>
-      <c r="S27" s="21" t="s">
+      <c r="S27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U27" s="19" t="n">
+      <c r="U27" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="V27" s="20" t="s">
+      <c r="V27" s="23" t="s">
         <v>458</v>
       </c>
-      <c r="W27" s="21" t="s">
+      <c r="W27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Y27" s="19" t="n">
+      <c r="Y27" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="Z27" s="20" t="s">
+      <c r="Z27" s="23" t="s">
         <v>459</v>
       </c>
-      <c r="AA27" s="21" t="s">
+      <c r="AA27" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="19" t="n">
+      <c r="E28" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="23" t="s">
         <v>460</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I28" s="19" t="n">
+      <c r="I28" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="J28" s="20" t="s">
+      <c r="J28" s="23" t="s">
         <v>461</v>
       </c>
-      <c r="K28" s="21" t="s">
+      <c r="K28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M28" s="19" t="n">
+      <c r="M28" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="N28" s="20" t="s">
+      <c r="N28" s="23" t="s">
         <v>462</v>
       </c>
-      <c r="O28" s="21" t="s">
+      <c r="O28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Q28" s="19" t="n">
+      <c r="Q28" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="R28" s="20" t="s">
+      <c r="R28" s="23" t="s">
         <v>463</v>
       </c>
-      <c r="S28" s="21" t="s">
+      <c r="S28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U28" s="19" t="n">
+      <c r="U28" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="V28" s="20" t="s">
+      <c r="V28" s="23" t="s">
         <v>464</v>
       </c>
-      <c r="W28" s="21" t="s">
+      <c r="W28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="Y28" s="19" t="n">
+      <c r="Y28" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="Z28" s="20" t="s">
+      <c r="Z28" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="AA28" s="21" t="s">
+      <c r="AA28" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="19" t="n">
+      <c r="E29" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="19" t="n">
+      <c r="I29" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="23" t="s">
         <v>467</v>
       </c>
-      <c r="K29" s="21" t="s">
+      <c r="K29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M29" s="19" t="n">
+      <c r="M29" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="N29" s="20" t="s">
+      <c r="N29" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="O29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Q29" s="19" t="n">
+      <c r="Q29" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="R29" s="20" t="s">
+      <c r="R29" s="23" t="s">
         <v>469</v>
       </c>
-      <c r="S29" s="21" t="s">
+      <c r="S29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U29" s="19" t="n">
+      <c r="U29" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="V29" s="20" t="s">
+      <c r="V29" s="23" t="s">
         <v>470</v>
       </c>
-      <c r="W29" s="21" t="s">
+      <c r="W29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="Y29" s="19" t="n">
+      <c r="Y29" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="Z29" s="20" t="s">
+      <c r="Z29" s="23" t="s">
         <v>471</v>
       </c>
-      <c r="AA29" s="21" t="s">
+      <c r="AA29" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="19" t="n">
+      <c r="E30" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="23" t="s">
         <v>472</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="I30" s="19" t="n">
+      <c r="I30" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="J30" s="20" t="s">
+      <c r="J30" s="23" t="s">
         <v>473</v>
       </c>
-      <c r="K30" s="21" t="s">
+      <c r="K30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M30" s="19" t="n">
+      <c r="M30" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="N30" s="20" t="s">
+      <c r="N30" s="23" t="s">
         <v>474</v>
       </c>
-      <c r="O30" s="21" t="s">
+      <c r="O30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Q30" s="19" t="n">
+      <c r="Q30" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="R30" s="20" t="s">
+      <c r="R30" s="23" t="s">
         <v>475</v>
       </c>
-      <c r="S30" s="21" t="s">
+      <c r="S30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U30" s="19" t="n">
+      <c r="U30" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="V30" s="20" t="s">
+      <c r="V30" s="23" t="s">
         <v>476</v>
       </c>
-      <c r="W30" s="21" t="s">
+      <c r="W30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="Y30" s="19" t="n">
+      <c r="Y30" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="Z30" s="20" t="s">
+      <c r="Z30" s="23" t="s">
         <v>477</v>
       </c>
-      <c r="AA30" s="21" t="s">
+      <c r="AA30" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="19" t="n">
+      <c r="E31" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="23" t="s">
         <v>478</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="G31" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="19" t="n">
+      <c r="I31" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="J31" s="20" t="s">
+      <c r="J31" s="23" t="s">
         <v>479</v>
       </c>
-      <c r="K31" s="21" t="s">
+      <c r="K31" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M31" s="19" t="n">
+      <c r="M31" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="N31" s="20" t="s">
+      <c r="N31" s="23" t="s">
         <v>480</v>
       </c>
-      <c r="O31" s="21" t="s">
+      <c r="O31" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Q31" s="19" t="n">
+      <c r="Q31" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="R31" s="20" t="s">
+      <c r="R31" s="23" t="s">
         <v>481</v>
       </c>
-      <c r="S31" s="21" t="s">
+      <c r="S31" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U31" s="19" t="n">
+      <c r="U31" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="V31" s="20" t="s">
+      <c r="V31" s="23" t="s">
         <v>482</v>
       </c>
-      <c r="W31" s="21" t="s">
+      <c r="W31" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="Y31" s="19" t="n">
+      <c r="Y31" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="Z31" s="20" t="s">
+      <c r="Z31" s="23" t="s">
         <v>483</v>
       </c>
-      <c r="AA31" s="21" t="s">
+      <c r="AA31" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="19" t="n">
+      <c r="E32" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="23" t="s">
         <v>484</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="I32" s="19" t="n">
+      <c r="I32" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="J32" s="20" t="s">
+      <c r="J32" s="23" t="s">
         <v>485</v>
       </c>
-      <c r="K32" s="21" t="s">
+      <c r="K32" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M32" s="19" t="n">
+      <c r="M32" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="N32" s="20" t="s">
+      <c r="N32" s="23" t="s">
         <v>486</v>
       </c>
-      <c r="O32" s="21" t="s">
+      <c r="O32" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Q32" s="19" t="n">
+      <c r="Q32" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="R32" s="20" t="s">
+      <c r="R32" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="S32" s="21" t="s">
+      <c r="S32" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U32" s="19" t="n">
+      <c r="U32" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="V32" s="20" t="s">
+      <c r="V32" s="23" t="s">
         <v>488</v>
       </c>
-      <c r="W32" s="21" t="s">
+      <c r="W32" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="Y32" s="19" t="n">
+      <c r="Y32" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="Z32" s="20" t="s">
+      <c r="Z32" s="23" t="s">
         <v>489</v>
       </c>
-      <c r="AA32" s="21" t="s">
+      <c r="AA32" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="19" t="n">
+      <c r="E33" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="23" t="s">
         <v>490</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="K33" s="22"/>
-      <c r="M33" s="19" t="n">
+      <c r="K33" s="25"/>
+      <c r="M33" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="N33" s="20" t="s">
+      <c r="N33" s="23" t="s">
         <v>491</v>
       </c>
-      <c r="O33" s="21" t="s">
+      <c r="O33" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="S33" s="22"/>
-      <c r="U33" s="19" t="n">
+      <c r="S33" s="25"/>
+      <c r="U33" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="V33" s="20" t="s">
+      <c r="V33" s="23" t="s">
         <v>492</v>
       </c>
-      <c r="W33" s="21" t="s">
+      <c r="W33" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="19" t="n">
+      <c r="E34" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="23" t="s">
         <v>493</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M34" s="19" t="n">
+      <c r="M34" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="N34" s="20" t="s">
+      <c r="N34" s="23" t="s">
         <v>494</v>
       </c>
-      <c r="O34" s="21" t="s">
+      <c r="O34" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U34" s="19" t="n">
+      <c r="U34" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="V34" s="20" t="s">
+      <c r="V34" s="23" t="s">
         <v>495</v>
       </c>
-      <c r="W34" s="21" t="s">
+      <c r="W34" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="19" t="n">
+      <c r="E35" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="23" t="s">
         <v>496</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M35" s="19" t="n">
+      <c r="M35" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="N35" s="20" t="s">
+      <c r="N35" s="23" t="s">
         <v>497</v>
       </c>
-      <c r="O35" s="21" t="s">
+      <c r="O35" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U35" s="19" t="n">
+      <c r="U35" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="V35" s="20" t="s">
+      <c r="V35" s="23" t="s">
         <v>498</v>
       </c>
-      <c r="W35" s="21" t="s">
+      <c r="W35" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="19" t="n">
+      <c r="E36" s="22" t="n">
         <v>35</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="23" t="s">
         <v>499</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M36" s="19" t="n">
+      <c r="M36" s="22" t="n">
         <v>35</v>
       </c>
-      <c r="N36" s="20" t="s">
+      <c r="N36" s="23" t="s">
         <v>500</v>
       </c>
-      <c r="O36" s="21" t="s">
+      <c r="O36" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U36" s="19" t="n">
+      <c r="U36" s="22" t="n">
         <v>35</v>
       </c>
-      <c r="V36" s="20" t="s">
+      <c r="V36" s="23" t="s">
         <v>501</v>
       </c>
-      <c r="W36" s="21" t="s">
+      <c r="W36" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="19" t="n">
+      <c r="E37" s="22" t="n">
         <v>36</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="23" t="s">
         <v>502</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M37" s="19" t="n">
+      <c r="M37" s="22" t="n">
         <v>36</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="N37" s="23" t="s">
         <v>503</v>
       </c>
-      <c r="O37" s="21" t="s">
+      <c r="O37" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U37" s="19" t="n">
+      <c r="U37" s="22" t="n">
         <v>36</v>
       </c>
-      <c r="V37" s="20" t="s">
+      <c r="V37" s="23" t="s">
         <v>504</v>
       </c>
-      <c r="W37" s="21" t="s">
+      <c r="W37" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="19" t="n">
+      <c r="E38" s="22" t="n">
         <v>37</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="23" t="s">
         <v>505</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M38" s="19" t="n">
+      <c r="M38" s="22" t="n">
         <v>37</v>
       </c>
-      <c r="N38" s="20" t="s">
+      <c r="N38" s="23" t="s">
         <v>506</v>
       </c>
-      <c r="O38" s="21" t="s">
+      <c r="O38" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U38" s="19" t="n">
+      <c r="U38" s="22" t="n">
         <v>37</v>
       </c>
-      <c r="V38" s="20" t="s">
+      <c r="V38" s="23" t="s">
         <v>507</v>
       </c>
-      <c r="W38" s="21" t="s">
+      <c r="W38" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="19" t="n">
+      <c r="E39" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="23" t="s">
         <v>508</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G39" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M39" s="19" t="n">
+      <c r="M39" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="N39" s="20" t="s">
+      <c r="N39" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="O39" s="21" t="s">
+      <c r="O39" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U39" s="19" t="n">
+      <c r="U39" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="V39" s="20" t="s">
+      <c r="V39" s="23" t="s">
         <v>510</v>
       </c>
-      <c r="W39" s="21" t="s">
+      <c r="W39" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="19" t="n">
+      <c r="E40" s="22" t="n">
         <v>39</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="23" t="s">
         <v>511</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M40" s="19" t="n">
+      <c r="M40" s="22" t="n">
         <v>39</v>
       </c>
-      <c r="N40" s="20" t="s">
+      <c r="N40" s="23" t="s">
         <v>512</v>
       </c>
-      <c r="O40" s="21" t="s">
+      <c r="O40" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U40" s="19" t="n">
+      <c r="U40" s="22" t="n">
         <v>39</v>
       </c>
-      <c r="V40" s="20" t="s">
+      <c r="V40" s="23" t="s">
         <v>513</v>
       </c>
-      <c r="W40" s="21" t="s">
+      <c r="W40" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="19" t="n">
+      <c r="E41" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="23" t="s">
         <v>514</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M41" s="19" t="n">
+      <c r="M41" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="N41" s="20" t="s">
+      <c r="N41" s="23" t="s">
         <v>515</v>
       </c>
-      <c r="O41" s="21" t="s">
+      <c r="O41" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="U41" s="19" t="n">
+      <c r="U41" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="V41" s="20" t="s">
+      <c r="V41" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="W41" s="21" t="s">
+      <c r="W41" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E42" s="19" t="n">
+      <c r="E42" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="23" t="s">
         <v>517</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M42" s="19" t="n">
+      <c r="M42" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="N42" s="20" t="s">
+      <c r="N42" s="23" t="s">
         <v>518</v>
       </c>
-      <c r="O42" s="21" t="s">
+      <c r="O42" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U42" s="19" t="n">
+      <c r="U42" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="V42" s="20" t="s">
+      <c r="V42" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="W42" s="21" t="s">
+      <c r="W42" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E43" s="19" t="n">
+      <c r="E43" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="23" t="s">
         <v>520</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M43" s="19" t="n">
+      <c r="M43" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="N43" s="20" t="s">
+      <c r="N43" s="23" t="s">
         <v>521</v>
       </c>
-      <c r="O43" s="21" t="s">
+      <c r="O43" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U43" s="19" t="n">
+      <c r="U43" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="V43" s="20" t="s">
+      <c r="V43" s="23" t="s">
         <v>522</v>
       </c>
-      <c r="W43" s="21" t="s">
+      <c r="W43" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E44" s="19" t="n">
-        <v>43</v>
-      </c>
-      <c r="F44" s="20" t="s">
+      <c r="E44" s="22" t="n">
+        <v>43</v>
+      </c>
+      <c r="F44" s="23" t="s">
         <v>523</v>
       </c>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M44" s="19" t="n">
-        <v>43</v>
-      </c>
-      <c r="N44" s="20" t="s">
+      <c r="M44" s="22" t="n">
+        <v>43</v>
+      </c>
+      <c r="N44" s="23" t="s">
         <v>524</v>
       </c>
-      <c r="O44" s="21" t="s">
+      <c r="O44" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U44" s="19" t="n">
-        <v>43</v>
-      </c>
-      <c r="V44" s="20" t="s">
+      <c r="U44" s="22" t="n">
+        <v>43</v>
+      </c>
+      <c r="V44" s="23" t="s">
         <v>525</v>
       </c>
-      <c r="W44" s="21" t="s">
+      <c r="W44" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E45" s="19" t="n">
-        <v>44</v>
-      </c>
-      <c r="F45" s="20" t="s">
+      <c r="E45" s="22" t="n">
+        <v>44</v>
+      </c>
+      <c r="F45" s="23" t="s">
         <v>526</v>
       </c>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M45" s="19" t="n">
-        <v>44</v>
-      </c>
-      <c r="N45" s="20" t="s">
+      <c r="M45" s="22" t="n">
+        <v>44</v>
+      </c>
+      <c r="N45" s="23" t="s">
         <v>527</v>
       </c>
-      <c r="O45" s="21" t="s">
+      <c r="O45" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U45" s="19" t="n">
-        <v>44</v>
-      </c>
-      <c r="V45" s="20" t="s">
+      <c r="U45" s="22" t="n">
+        <v>44</v>
+      </c>
+      <c r="V45" s="23" t="s">
         <v>528</v>
       </c>
-      <c r="W45" s="21" t="s">
+      <c r="W45" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E46" s="19" t="n">
-        <v>45</v>
-      </c>
-      <c r="F46" s="20" t="s">
+      <c r="E46" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="F46" s="23" t="s">
         <v>529</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M46" s="19" t="n">
-        <v>45</v>
-      </c>
-      <c r="N46" s="20" t="s">
+      <c r="M46" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="N46" s="23" t="s">
         <v>530</v>
       </c>
-      <c r="O46" s="21" t="s">
+      <c r="O46" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U46" s="19" t="n">
-        <v>45</v>
-      </c>
-      <c r="V46" s="20" t="s">
+      <c r="U46" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="V46" s="23" t="s">
         <v>531</v>
       </c>
-      <c r="W46" s="21" t="s">
+      <c r="W46" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="19" t="n">
+      <c r="E47" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="F47" s="20" t="s">
+      <c r="F47" s="23" t="s">
         <v>532</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M47" s="19" t="n">
+      <c r="M47" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="N47" s="20" t="s">
+      <c r="N47" s="23" t="s">
         <v>533</v>
       </c>
-      <c r="O47" s="21" t="s">
+      <c r="O47" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U47" s="19" t="n">
+      <c r="U47" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="V47" s="20" t="s">
+      <c r="V47" s="23" t="s">
         <v>534</v>
       </c>
-      <c r="W47" s="21" t="s">
+      <c r="W47" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="19" t="n">
+      <c r="E48" s="22" t="n">
         <v>47</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="23" t="s">
         <v>535</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M48" s="19" t="n">
+      <c r="M48" s="22" t="n">
         <v>47</v>
       </c>
-      <c r="N48" s="20" t="s">
+      <c r="N48" s="23" t="s">
         <v>536</v>
       </c>
-      <c r="O48" s="21" t="s">
+      <c r="O48" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U48" s="19" t="n">
+      <c r="U48" s="22" t="n">
         <v>47</v>
       </c>
-      <c r="V48" s="20" t="s">
+      <c r="V48" s="23" t="s">
         <v>537</v>
       </c>
-      <c r="W48" s="21" t="s">
+      <c r="W48" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="19" t="n">
+      <c r="E49" s="22" t="n">
         <v>48</v>
       </c>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="23" t="s">
         <v>538</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="G49" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M49" s="19" t="n">
+      <c r="M49" s="22" t="n">
         <v>48</v>
       </c>
-      <c r="N49" s="20" t="s">
+      <c r="N49" s="23" t="s">
         <v>539</v>
       </c>
-      <c r="O49" s="21" t="s">
+      <c r="O49" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="U49" s="19" t="n">
+      <c r="U49" s="22" t="n">
         <v>48</v>
       </c>
-      <c r="V49" s="20" t="s">
+      <c r="V49" s="23" t="s">
         <v>540</v>
       </c>
-      <c r="W49" s="21" t="s">
+      <c r="W49" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="19" t="n">
+      <c r="E50" s="22" t="n">
         <v>49</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F50" s="23" t="s">
         <v>541</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G50" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M50" s="19" t="n">
+      <c r="M50" s="22" t="n">
         <v>49</v>
       </c>
-      <c r="N50" s="20" t="s">
+      <c r="N50" s="23" t="s">
         <v>542</v>
       </c>
-      <c r="O50" s="21" t="s">
+      <c r="O50" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U50" s="19" t="n">
+      <c r="U50" s="22" t="n">
         <v>49</v>
       </c>
-      <c r="V50" s="20" t="s">
+      <c r="V50" s="23" t="s">
         <v>543</v>
       </c>
-      <c r="W50" s="21" t="s">
+      <c r="W50" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E51" s="19" t="n">
+      <c r="E51" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F51" s="23" t="s">
         <v>544</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M51" s="19" t="n">
+      <c r="M51" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="N51" s="20" t="s">
+      <c r="N51" s="23" t="s">
         <v>545</v>
       </c>
-      <c r="O51" s="21" t="s">
+      <c r="O51" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U51" s="19" t="n">
+      <c r="U51" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="V51" s="20" t="s">
+      <c r="V51" s="23" t="s">
         <v>546</v>
       </c>
-      <c r="W51" s="21" t="s">
+      <c r="W51" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="19" t="n">
+      <c r="E52" s="22" t="n">
         <v>51</v>
       </c>
-      <c r="F52" s="20" t="s">
+      <c r="F52" s="23" t="s">
         <v>547</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M52" s="19" t="n">
+      <c r="M52" s="22" t="n">
         <v>51</v>
       </c>
-      <c r="N52" s="20" t="s">
+      <c r="N52" s="23" t="s">
         <v>548</v>
       </c>
-      <c r="O52" s="21" t="s">
+      <c r="O52" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U52" s="19" t="n">
+      <c r="U52" s="22" t="n">
         <v>51</v>
       </c>
-      <c r="V52" s="20" t="s">
+      <c r="V52" s="23" t="s">
         <v>549</v>
       </c>
-      <c r="W52" s="21" t="s">
+      <c r="W52" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="19" t="n">
+      <c r="E53" s="22" t="n">
         <v>52</v>
       </c>
-      <c r="F53" s="20" t="s">
+      <c r="F53" s="23" t="s">
         <v>550</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="G53" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M53" s="19" t="n">
+      <c r="M53" s="22" t="n">
         <v>52</v>
       </c>
-      <c r="N53" s="20" t="s">
+      <c r="N53" s="23" t="s">
         <v>551</v>
       </c>
-      <c r="O53" s="21" t="s">
+      <c r="O53" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U53" s="19" t="n">
+      <c r="U53" s="22" t="n">
         <v>52</v>
       </c>
-      <c r="V53" s="20" t="s">
+      <c r="V53" s="23" t="s">
         <v>552</v>
       </c>
-      <c r="W53" s="21" t="s">
+      <c r="W53" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="19" t="n">
+      <c r="E54" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="23" t="s">
         <v>553</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="G54" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M54" s="19" t="n">
+      <c r="M54" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="N54" s="20" t="s">
+      <c r="N54" s="23" t="s">
         <v>554</v>
       </c>
-      <c r="O54" s="21" t="s">
+      <c r="O54" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U54" s="19" t="n">
+      <c r="U54" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="V54" s="20" t="s">
+      <c r="V54" s="23" t="s">
         <v>555</v>
       </c>
-      <c r="W54" s="21" t="s">
+      <c r="W54" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="19" t="n">
+      <c r="E55" s="22" t="n">
         <v>54</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="F55" s="23" t="s">
         <v>556</v>
       </c>
-      <c r="G55" s="21" t="s">
+      <c r="G55" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M55" s="19" t="n">
+      <c r="M55" s="22" t="n">
         <v>54</v>
       </c>
-      <c r="N55" s="20" t="s">
+      <c r="N55" s="23" t="s">
         <v>557</v>
       </c>
-      <c r="O55" s="21" t="s">
+      <c r="O55" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U55" s="19" t="n">
+      <c r="U55" s="22" t="n">
         <v>54</v>
       </c>
-      <c r="V55" s="20" t="s">
+      <c r="V55" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="W55" s="21" t="s">
+      <c r="W55" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E56" s="19" t="n">
+      <c r="E56" s="22" t="n">
         <v>55</v>
       </c>
-      <c r="F56" s="20" t="s">
+      <c r="F56" s="23" t="s">
         <v>559</v>
       </c>
-      <c r="G56" s="21" t="s">
+      <c r="G56" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="M56" s="19" t="n">
+      <c r="M56" s="22" t="n">
         <v>55</v>
       </c>
-      <c r="N56" s="20" t="s">
+      <c r="N56" s="23" t="s">
         <v>560</v>
       </c>
-      <c r="O56" s="21" t="s">
+      <c r="O56" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U56" s="19" t="n">
+      <c r="U56" s="22" t="n">
         <v>55</v>
       </c>
-      <c r="V56" s="20" t="s">
+      <c r="V56" s="23" t="s">
         <v>561</v>
       </c>
-      <c r="W56" s="21" t="s">
+      <c r="W56" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E57" s="19" t="n">
+      <c r="E57" s="22" t="n">
         <v>56</v>
       </c>
-      <c r="F57" s="20" t="s">
+      <c r="F57" s="23" t="s">
         <v>562</v>
       </c>
-      <c r="G57" s="21" t="s">
+      <c r="G57" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M57" s="19" t="n">
+      <c r="M57" s="22" t="n">
         <v>56</v>
       </c>
-      <c r="N57" s="20" t="s">
+      <c r="N57" s="23" t="s">
         <v>563</v>
       </c>
-      <c r="O57" s="21" t="s">
+      <c r="O57" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="U57" s="19" t="n">
+      <c r="U57" s="22" t="n">
         <v>56</v>
       </c>
-      <c r="V57" s="20" t="s">
+      <c r="V57" s="23" t="s">
         <v>564</v>
       </c>
-      <c r="W57" s="21" t="s">
+      <c r="W57" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="19" t="n">
+      <c r="E58" s="22" t="n">
         <v>57</v>
       </c>
-      <c r="F58" s="20" t="s">
+      <c r="F58" s="23" t="s">
         <v>565</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M58" s="19" t="n">
+      <c r="M58" s="22" t="n">
         <v>57</v>
       </c>
-      <c r="N58" s="20" t="s">
+      <c r="N58" s="23" t="s">
         <v>566</v>
       </c>
-      <c r="O58" s="21" t="s">
+      <c r="O58" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U58" s="19" t="n">
+      <c r="U58" s="22" t="n">
         <v>57</v>
       </c>
-      <c r="V58" s="20" t="s">
+      <c r="V58" s="23" t="s">
         <v>567</v>
       </c>
-      <c r="W58" s="21" t="s">
+      <c r="W58" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E59" s="19" t="n">
+      <c r="E59" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F59" s="23" t="s">
         <v>568</v>
       </c>
-      <c r="G59" s="21" t="s">
+      <c r="G59" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="M59" s="19" t="n">
+      <c r="M59" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="N59" s="20" t="s">
+      <c r="N59" s="23" t="s">
         <v>569</v>
       </c>
-      <c r="O59" s="21" t="s">
+      <c r="O59" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U59" s="19" t="n">
+      <c r="U59" s="22" t="n">
         <v>58</v>
       </c>
-      <c r="V59" s="20" t="s">
+      <c r="V59" s="23" t="s">
         <v>570</v>
       </c>
-      <c r="W59" s="21" t="s">
+      <c r="W59" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E60" s="19" t="n">
+      <c r="E60" s="22" t="n">
         <v>59</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="23" t="s">
         <v>571</v>
       </c>
-      <c r="G60" s="21" t="s">
+      <c r="G60" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="M60" s="19" t="n">
+      <c r="M60" s="22" t="n">
         <v>59</v>
       </c>
-      <c r="N60" s="20" t="s">
+      <c r="N60" s="23" t="s">
         <v>572</v>
       </c>
-      <c r="O60" s="21" t="s">
+      <c r="O60" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="U60" s="19" t="n">
+      <c r="U60" s="22" t="n">
         <v>59</v>
       </c>
-      <c r="V60" s="20" t="s">
+      <c r="V60" s="23" t="s">
         <v>573</v>
       </c>
-      <c r="W60" s="21" t="s">
+      <c r="W60" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E61" s="19" t="n">
+      <c r="E61" s="22" t="n">
         <v>60</v>
       </c>
-      <c r="F61" s="20" t="s">
+      <c r="F61" s="23" t="s">
         <v>574</v>
       </c>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="M61" s="19" t="n">
+      <c r="M61" s="22" t="n">
         <v>60</v>
       </c>
-      <c r="N61" s="20" t="s">
+      <c r="N61" s="23" t="s">
         <v>575</v>
       </c>
-      <c r="O61" s="21" t="s">
+      <c r="O61" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U61" s="19" t="n">
+      <c r="U61" s="22" t="n">
         <v>60</v>
       </c>
-      <c r="V61" s="20" t="s">
+      <c r="V61" s="23" t="s">
         <v>576</v>
       </c>
-      <c r="W61" s="21" t="s">
+      <c r="W61" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E62" s="19" t="n">
+      <c r="E62" s="22" t="n">
         <v>61</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="23" t="s">
         <v>577</v>
       </c>
-      <c r="G62" s="21" t="s">
+      <c r="G62" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="M62" s="19" t="n">
+      <c r="M62" s="22" t="n">
         <v>61</v>
       </c>
-      <c r="N62" s="20" t="s">
+      <c r="N62" s="23" t="s">
         <v>578</v>
       </c>
-      <c r="O62" s="21" t="s">
+      <c r="O62" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="U62" s="19" t="n">
+      <c r="U62" s="22" t="n">
         <v>61</v>
       </c>
-      <c r="V62" s="20" t="s">
+      <c r="V62" s="23" t="s">
         <v>579</v>
       </c>
-      <c r="W62" s="21" t="s">
+      <c r="W62" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E63" s="19" t="n">
+      <c r="E63" s="22" t="n">
         <v>62</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F63" s="23" t="s">
         <v>580</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G63" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M63" s="19" t="n">
+      <c r="M63" s="22" t="n">
         <v>62</v>
       </c>
-      <c r="N63" s="20" t="s">
+      <c r="N63" s="23" t="s">
         <v>581</v>
       </c>
-      <c r="O63" s="21" t="s">
+      <c r="O63" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="U63" s="19" t="n">
+      <c r="U63" s="22" t="n">
         <v>62</v>
       </c>
-      <c r="V63" s="20" t="s">
+      <c r="V63" s="23" t="s">
         <v>582</v>
       </c>
-      <c r="W63" s="21" t="s">
+      <c r="W63" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F64" s="23"/>
-      <c r="G64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="W64" s="22"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="25"/>
+      <c r="O64" s="25"/>
+      <c r="W64" s="25"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G65" s="22"/>
-      <c r="O65" s="22"/>
-      <c r="W65" s="22"/>
+      <c r="G65" s="25"/>
+      <c r="O65" s="25"/>
+      <c r="W65" s="25"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C25 G2:G65 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33 AE2:AE17 AI2:AI17 AM2:AM17">
@@ -13370,13 +13426,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>583</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>584</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="27" t="s">
         <v>585</v>
       </c>
     </row>

</xml_diff>

<commit_message>
version updated, handling sorted
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -6884,9 +6884,9 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>

</xml_diff>

<commit_message>
testing spreadsheets also fixed
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="596">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -2406,7 +2406,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="BV10" activeCellId="0" sqref="BV10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2704,8 +2704,9 @@
       <c r="AP2" s="10"/>
       <c r="AQ2" s="10"/>
       <c r="AR2" s="10"/>
-      <c r="AT2" s="2" t="s">
-        <v>45</v>
+      <c r="AT2" s="2" t="str">
+        <f aca="false">IF(L2="x","x","")</f>
+        <v>x</v>
       </c>
       <c r="AU2" s="2" t="str">
         <f aca="false">IF(M2="x","x","")</f>

</xml_diff>

<commit_message>
Version for reaper removed, works also for v7
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="574">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -24630,7 +24630,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>46</v>
@@ -24639,7 +24639,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>46</v>
@@ -24648,7 +24648,7 @@
         <v>46</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>46</v>
@@ -24657,7 +24657,7 @@
         <v>46</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>46</v>
@@ -24671,7 +24671,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>46</v>
@@ -24680,7 +24680,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>46</v>
@@ -24689,7 +24689,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>46</v>
@@ -24698,7 +24698,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>46</v>
@@ -24712,7 +24712,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>46</v>
@@ -24721,7 +24721,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>46</v>
@@ -24730,7 +24730,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>46</v>
@@ -24739,7 +24739,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>46</v>
@@ -24753,7 +24753,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>46</v>
@@ -24762,7 +24762,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>46</v>
@@ -24771,7 +24771,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>46</v>
@@ -24780,7 +24780,7 @@
         <v>15</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P5" s="10" t="s">
         <v>46</v>
@@ -24794,7 +24794,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>46</v>
@@ -24803,7 +24803,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>46</v>
@@ -24812,7 +24812,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>46</v>
@@ -24821,7 +24821,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>46</v>
@@ -24835,7 +24835,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>46</v>
@@ -24844,7 +24844,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>46</v>
@@ -24853,7 +24853,7 @@
         <v>25</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>46</v>
@@ -24862,7 +24862,7 @@
         <v>25</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>46</v>
@@ -24876,7 +24876,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>46</v>
@@ -24885,7 +24885,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>46</v>
@@ -24894,7 +24894,7 @@
         <v>30</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>46</v>
@@ -24903,7 +24903,7 @@
         <v>30</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>46</v>
@@ -24917,7 +24917,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>46</v>
@@ -24926,7 +24926,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>46</v>
@@ -24935,7 +24935,7 @@
         <v>35</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>46</v>
@@ -24944,7 +24944,7 @@
         <v>35</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P9" s="10" t="s">
         <v>46</v>
@@ -24958,7 +24958,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>46</v>
@@ -24967,7 +24967,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>46</v>
@@ -24976,7 +24976,7 @@
         <v>40</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>46</v>
@@ -24985,7 +24985,7 @@
         <v>40</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P10" s="10" t="s">
         <v>46</v>
@@ -24999,7 +24999,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>46</v>
@@ -25008,7 +25008,7 @@
         <v>45</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>46</v>
@@ -25017,7 +25017,7 @@
         <v>45</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>46</v>
@@ -25026,7 +25026,7 @@
         <v>45</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P11" s="10" t="s">
         <v>46</v>
@@ -25040,7 +25040,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>46</v>
@@ -25049,7 +25049,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>46</v>
@@ -25058,7 +25058,7 @@
         <v>50</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>46</v>
@@ -25067,7 +25067,7 @@
         <v>50</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P12" s="10" t="s">
         <v>46</v>
@@ -25084,7 +25084,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>46</v>
@@ -25093,7 +25093,7 @@
         <v>55</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>46</v>
@@ -25102,7 +25102,7 @@
         <v>55</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>46</v>
@@ -25111,7 +25111,7 @@
         <v>55</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P13" s="10" t="s">
         <v>46</v>
@@ -25125,7 +25125,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>46</v>
@@ -25134,7 +25134,7 @@
         <v>60</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>46</v>
@@ -25143,7 +25143,7 @@
         <v>60</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>46</v>
@@ -25152,7 +25152,7 @@
         <v>60</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P14" s="10" t="s">
         <v>46</v>
@@ -25166,7 +25166,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>46</v>
@@ -25175,7 +25175,7 @@
         <v>46</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>46</v>
@@ -25184,7 +25184,7 @@
         <v>46</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>46</v>
@@ -25193,7 +25193,7 @@
         <v>46</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P15" s="10" t="s">
         <v>46</v>
@@ -25207,40 +25207,40 @@
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I16" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M16" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q16" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25248,40 +25248,40 @@
         <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I17" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M17" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q17" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q17" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25289,40 +25289,40 @@
         <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I18" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M18" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q18" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25330,40 +25330,40 @@
         <v>18</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I19" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M19" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q19" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25371,40 +25371,40 @@
         <v>19</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I20" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M20" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q20" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25412,40 +25412,40 @@
         <v>20</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I21" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M21" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q21" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25453,40 +25453,40 @@
         <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I22" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M22" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q22" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25494,40 +25494,40 @@
         <v>22</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I23" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M23" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q23" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q23" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25535,40 +25535,40 @@
         <v>23</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I24" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M24" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q24" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25576,40 +25576,40 @@
         <v>24</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E25" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I25" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M25" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q25" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q25" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25617,40 +25617,40 @@
         <v>25</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E26" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I26" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M26" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q26" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25658,40 +25658,40 @@
         <v>26</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E27" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I27" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M27" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q27" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q27" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25699,40 +25699,40 @@
         <v>27</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E28" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I28" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M28" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P28" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q28" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25740,40 +25740,40 @@
         <v>28</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E29" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I29" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M29" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q29" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q29" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25781,40 +25781,40 @@
         <v>29</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E30" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I30" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M30" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q30" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25822,40 +25822,40 @@
         <v>30</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E31" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I31" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M31" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q31" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q31" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25863,40 +25863,40 @@
         <v>31</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E32" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="I32" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M32" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P32" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q32" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q32" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25907,40 +25907,40 @@
         <v>32</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E33" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I33" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="M33" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q33" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q33" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25948,22 +25948,22 @@
         <v>33</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E34" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q34" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q34" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25971,22 +25971,22 @@
         <v>34</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E35" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P35" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q35" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q35" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25994,22 +25994,22 @@
         <v>35</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E36" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q36" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26017,22 +26017,22 @@
         <v>36</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E37" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P37" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q37" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q37" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26040,22 +26040,22 @@
         <v>37</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E38" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P38" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q38" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q38" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26063,22 +26063,22 @@
         <v>38</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E39" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P39" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q39" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q39" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26086,22 +26086,22 @@
         <v>39</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E40" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P40" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q40" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q40" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26109,22 +26109,22 @@
         <v>40</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E41" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O41" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P41" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q41" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q41" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26132,22 +26132,22 @@
         <v>41</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E42" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O42" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P42" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q42" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q42" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26155,22 +26155,22 @@
         <v>42</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E43" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O43" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P43" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q43" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q43" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26178,22 +26178,22 @@
         <v>43</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E44" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O44" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q44" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q44" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26201,22 +26201,22 @@
         <v>44</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E45" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O45" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P45" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q45" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q45" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26224,22 +26224,22 @@
         <v>45</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E46" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O46" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q46" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q46" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26247,22 +26247,22 @@
         <v>46</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E47" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O47" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P47" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q47" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q47" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26270,22 +26270,22 @@
         <v>47</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E48" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O48" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P48" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q48" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q48" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26296,22 +26296,22 @@
         <v>48</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E49" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P49" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q49" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q49" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26319,22 +26319,22 @@
         <v>49</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E50" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P50" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q50" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q50" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26342,22 +26342,22 @@
         <v>50</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E51" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O51" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P51" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q51" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q51" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26365,22 +26365,22 @@
         <v>51</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E52" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P52" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q52" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q52" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26388,22 +26388,22 @@
         <v>52</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E53" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P53" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q53" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q53" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26411,22 +26411,22 @@
         <v>53</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E54" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O54" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P54" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q54" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q54" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26434,22 +26434,22 @@
         <v>54</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E55" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O55" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P55" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q55" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q55" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26457,22 +26457,22 @@
         <v>55</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E56" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O56" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P56" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q56" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q56" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26480,22 +26480,22 @@
         <v>56</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E57" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O57" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P57" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q57" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q57" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26503,22 +26503,22 @@
         <v>57</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E58" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O58" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P58" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q58" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q58" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26526,22 +26526,22 @@
         <v>58</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E59" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O59" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P59" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q59" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q59" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26549,22 +26549,22 @@
         <v>59</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E60" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O60" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P60" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q60" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q60" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26572,22 +26572,22 @@
         <v>60</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E61" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O61" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P61" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q61" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q61" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26595,22 +26595,22 @@
         <v>61</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E62" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O62" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P62" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q62" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q62" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26618,22 +26618,22 @@
         <v>62</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E63" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O63" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P63" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q63" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q63" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26641,22 +26641,22 @@
         <v>63</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E64" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O64" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P64" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q64" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q64" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26667,22 +26667,22 @@
         <v>64</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E65" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O65" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P65" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q65" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q65" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26693,13 +26693,13 @@
         <v>65</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P66" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q66" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q66" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26707,13 +26707,13 @@
         <v>66</v>
       </c>
       <c r="O67" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P67" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q67" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q67" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26721,13 +26721,13 @@
         <v>67</v>
       </c>
       <c r="O68" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P68" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q68" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q68" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26735,13 +26735,13 @@
         <v>68</v>
       </c>
       <c r="O69" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P69" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q69" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q69" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26749,13 +26749,13 @@
         <v>69</v>
       </c>
       <c r="O70" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P70" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q70" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q70" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26763,13 +26763,13 @@
         <v>70</v>
       </c>
       <c r="O71" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P71" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q71" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q71" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26777,13 +26777,13 @@
         <v>71</v>
       </c>
       <c r="O72" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P72" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q72" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q72" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26791,13 +26791,13 @@
         <v>72</v>
       </c>
       <c r="O73" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P73" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q73" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q73" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26805,13 +26805,13 @@
         <v>73</v>
       </c>
       <c r="O74" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P74" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q74" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q74" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26819,13 +26819,13 @@
         <v>74</v>
       </c>
       <c r="O75" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P75" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q75" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q75" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26833,13 +26833,13 @@
         <v>75</v>
       </c>
       <c r="O76" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P76" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q76" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q76" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26847,13 +26847,13 @@
         <v>76</v>
       </c>
       <c r="O77" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P77" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q77" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q77" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26861,13 +26861,13 @@
         <v>77</v>
       </c>
       <c r="O78" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P78" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q78" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q78" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26875,13 +26875,13 @@
         <v>78</v>
       </c>
       <c r="O79" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P79" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q79" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q79" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26889,13 +26889,13 @@
         <v>79</v>
       </c>
       <c r="O80" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P80" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q80" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q80" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26903,13 +26903,13 @@
         <v>80</v>
       </c>
       <c r="O81" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P81" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q81" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q81" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26917,13 +26917,13 @@
         <v>81</v>
       </c>
       <c r="O82" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P82" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q82" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q82" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26931,13 +26931,13 @@
         <v>82</v>
       </c>
       <c r="O83" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P83" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q83" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q83" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26945,13 +26945,13 @@
         <v>83</v>
       </c>
       <c r="O84" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P84" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q84" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q84" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26959,13 +26959,13 @@
         <v>84</v>
       </c>
       <c r="O85" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P85" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q85" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q85" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26973,13 +26973,13 @@
         <v>85</v>
       </c>
       <c r="O86" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P86" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q86" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q86" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26987,13 +26987,13 @@
         <v>86</v>
       </c>
       <c r="O87" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P87" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q87" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q87" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27001,13 +27001,13 @@
         <v>87</v>
       </c>
       <c r="O88" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P88" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q88" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q88" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27015,13 +27015,13 @@
         <v>88</v>
       </c>
       <c r="O89" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P89" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q89" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q89" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27029,13 +27029,13 @@
         <v>89</v>
       </c>
       <c r="O90" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P90" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q90" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q90" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27043,13 +27043,13 @@
         <v>90</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P91" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q91" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q91" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27057,13 +27057,13 @@
         <v>91</v>
       </c>
       <c r="O92" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P92" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q92" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q92" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27071,13 +27071,13 @@
         <v>92</v>
       </c>
       <c r="O93" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P93" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q93" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q93" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27085,13 +27085,13 @@
         <v>93</v>
       </c>
       <c r="O94" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P94" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q94" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q94" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27099,13 +27099,13 @@
         <v>94</v>
       </c>
       <c r="O95" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P95" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q95" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q95" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27116,13 +27116,13 @@
         <v>95</v>
       </c>
       <c r="O96" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P96" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q96" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q96" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27133,13 +27133,13 @@
         <v>96</v>
       </c>
       <c r="O97" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P97" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q97" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q97" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27147,13 +27147,13 @@
         <v>97</v>
       </c>
       <c r="O98" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P98" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q98" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q98" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27161,13 +27161,13 @@
         <v>98</v>
       </c>
       <c r="O99" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P99" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q99" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q99" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27175,13 +27175,13 @@
         <v>99</v>
       </c>
       <c r="O100" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P100" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q100" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q100" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27189,13 +27189,13 @@
         <v>100</v>
       </c>
       <c r="O101" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P101" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q101" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q101" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27203,13 +27203,13 @@
         <v>101</v>
       </c>
       <c r="O102" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P102" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q102" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q102" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27217,13 +27217,13 @@
         <v>102</v>
       </c>
       <c r="O103" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P103" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q103" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q103" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27231,13 +27231,13 @@
         <v>103</v>
       </c>
       <c r="O104" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P104" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q104" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q104" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27245,13 +27245,13 @@
         <v>104</v>
       </c>
       <c r="O105" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P105" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q105" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q105" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27259,13 +27259,13 @@
         <v>105</v>
       </c>
       <c r="O106" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P106" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q106" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q106" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27273,13 +27273,13 @@
         <v>106</v>
       </c>
       <c r="O107" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P107" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q107" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q107" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27287,13 +27287,13 @@
         <v>107</v>
       </c>
       <c r="O108" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P108" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q108" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q108" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27301,13 +27301,13 @@
         <v>108</v>
       </c>
       <c r="O109" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P109" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q109" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q109" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27315,13 +27315,13 @@
         <v>109</v>
       </c>
       <c r="O110" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P110" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q110" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q110" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27329,13 +27329,13 @@
         <v>110</v>
       </c>
       <c r="O111" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P111" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q111" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q111" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27343,13 +27343,13 @@
         <v>111</v>
       </c>
       <c r="O112" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P112" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q112" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q112" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27357,13 +27357,13 @@
         <v>112</v>
       </c>
       <c r="O113" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P113" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q113" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q113" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27371,13 +27371,13 @@
         <v>113</v>
       </c>
       <c r="O114" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P114" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q114" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q114" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27385,13 +27385,13 @@
         <v>114</v>
       </c>
       <c r="O115" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P115" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q115" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q115" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27399,13 +27399,13 @@
         <v>115</v>
       </c>
       <c r="O116" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P116" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q116" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q116" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27413,13 +27413,13 @@
         <v>116</v>
       </c>
       <c r="O117" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P117" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q117" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q117" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27427,13 +27427,13 @@
         <v>117</v>
       </c>
       <c r="O118" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P118" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q118" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q118" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27441,13 +27441,13 @@
         <v>118</v>
       </c>
       <c r="O119" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P119" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q119" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q119" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27455,13 +27455,13 @@
         <v>119</v>
       </c>
       <c r="O120" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P120" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q120" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q120" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27469,13 +27469,13 @@
         <v>120</v>
       </c>
       <c r="O121" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P121" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q121" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q121" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27483,13 +27483,13 @@
         <v>121</v>
       </c>
       <c r="O122" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P122" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q122" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q122" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27497,13 +27497,13 @@
         <v>122</v>
       </c>
       <c r="O123" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P123" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q123" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q123" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27511,13 +27511,13 @@
         <v>123</v>
       </c>
       <c r="O124" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P124" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q124" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q124" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27525,13 +27525,13 @@
         <v>124</v>
       </c>
       <c r="O125" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P125" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q125" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q125" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27539,13 +27539,13 @@
         <v>125</v>
       </c>
       <c r="O126" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P126" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q126" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q126" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27553,13 +27553,13 @@
         <v>126</v>
       </c>
       <c r="O127" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P127" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q127" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q127" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27567,13 +27567,13 @@
         <v>127</v>
       </c>
       <c r="O128" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P128" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q128" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="Q128" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27584,13 +27584,13 @@
         <v>128</v>
       </c>
       <c r="O129" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P129" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q129" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Q129" s="10" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixed, bypass option, spreadsheets updated, overview updated
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2797" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="582">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -2374,7 +2374,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2848,13 +2848,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>51</v>
@@ -3033,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="11" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>51</v>
@@ -3220,13 +3220,13 @@
         <v>4</v>
       </c>
       <c r="F5" s="11" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>51</v>
@@ -3405,7 +3405,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="11" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>51</v>
@@ -3592,13 +3592,13 @@
         <v>6</v>
       </c>
       <c r="F7" s="11" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>51</v>
@@ -3777,7 +3777,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="11" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>51</v>
@@ -3964,13 +3964,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>51</v>
@@ -4149,7 +4149,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="11" t="n">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>51</v>
@@ -4336,13 +4336,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="11" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>51</v>
@@ -4521,7 +4521,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="11" t="n">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>51</v>
@@ -4708,13 +4708,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="11" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>51</v>
@@ -4892,15 +4892,9 @@
       <c r="E14" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="F14" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
       <c r="I14" s="11" t="s">
         <v>52</v>
       </c>
@@ -5079,14 +5073,14 @@
       <c r="E15" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="F15" s="11" t="n">
-        <v>5</v>
+      <c r="F15" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>51</v>
@@ -5270,7 +5264,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>51</v>
@@ -5454,13 +5448,13 @@
         <v>16</v>
       </c>
       <c r="F17" s="11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>51</v>
@@ -5641,10 +5635,10 @@
         <v>17</v>
       </c>
       <c r="F18" s="11" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>51</v>
@@ -5828,13 +5822,13 @@
         <v>18</v>
       </c>
       <c r="F19" s="11" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>51</v>
@@ -6015,10 +6009,10 @@
         <v>19</v>
       </c>
       <c r="F20" s="11" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>51</v>
@@ -6202,13 +6196,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="11" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>51</v>
@@ -6389,10 +6383,10 @@
         <v>21</v>
       </c>
       <c r="F22" s="11" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>51</v>
@@ -6576,13 +6570,13 @@
         <v>22</v>
       </c>
       <c r="F23" s="11" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>51</v>
@@ -6763,10 +6757,10 @@
         <v>23</v>
       </c>
       <c r="F24" s="11" t="n">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>51</v>
@@ -6950,13 +6944,13 @@
         <v>24</v>
       </c>
       <c r="F25" s="11" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>51</v>
@@ -7137,10 +7131,10 @@
         <v>25</v>
       </c>
       <c r="F26" s="11" t="n">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>51</v>
@@ -7324,13 +7318,13 @@
         <v>26</v>
       </c>
       <c r="F27" s="11" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I27" s="11" t="s">
         <v>51</v>
@@ -7510,14 +7504,14 @@
       <c r="E28" s="11" t="n">
         <v>27</v>
       </c>
-      <c r="F28" s="11" t="n">
-        <v>5</v>
+      <c r="F28" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>52</v>
@@ -7697,14 +7691,14 @@
       <c r="E29" s="11" t="n">
         <v>28</v>
       </c>
-      <c r="F29" s="11" t="n">
-        <v>5</v>
+      <c r="F29" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>51</v>
@@ -7884,14 +7878,14 @@
       <c r="E30" s="11" t="n">
         <v>29</v>
       </c>
-      <c r="F30" s="11" t="n">
-        <v>5</v>
+      <c r="F30" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>52</v>
@@ -8071,14 +8065,14 @@
       <c r="E31" s="11" t="n">
         <v>30</v>
       </c>
-      <c r="F31" s="11" t="n">
-        <v>5</v>
+      <c r="F31" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I31" s="11" t="s">
         <v>51</v>
@@ -8258,14 +8252,14 @@
       <c r="E32" s="11" t="n">
         <v>31</v>
       </c>
-      <c r="F32" s="11" t="n">
-        <v>5</v>
+      <c r="F32" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I32" s="11" t="s">
         <v>52</v>
@@ -8445,14 +8439,14 @@
       <c r="E33" s="11" t="n">
         <v>32</v>
       </c>
-      <c r="F33" s="11" t="n">
-        <v>5</v>
+      <c r="F33" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I33" s="11" t="s">
         <v>51</v>
@@ -8632,14 +8626,14 @@
       <c r="E34" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="F34" s="11" t="n">
-        <v>5</v>
+      <c r="F34" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I34" s="11" t="s">
         <v>52</v>
@@ -8819,14 +8813,14 @@
       <c r="E35" s="11" t="n">
         <v>34</v>
       </c>
-      <c r="F35" s="11" t="n">
-        <v>5</v>
+      <c r="F35" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I35" s="11" t="s">
         <v>51</v>
@@ -9006,14 +9000,14 @@
       <c r="E36" s="11" t="n">
         <v>35</v>
       </c>
-      <c r="F36" s="11" t="n">
-        <v>5</v>
+      <c r="F36" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>52</v>
@@ -9193,14 +9187,14 @@
       <c r="E37" s="11" t="n">
         <v>36</v>
       </c>
-      <c r="F37" s="11" t="n">
-        <v>5</v>
+      <c r="F37" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I37" s="11" t="s">
         <v>51</v>
@@ -9380,14 +9374,14 @@
       <c r="E38" s="11" t="n">
         <v>37</v>
       </c>
-      <c r="F38" s="11" t="n">
-        <v>5</v>
+      <c r="F38" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I38" s="11" t="s">
         <v>52</v>
@@ -9565,14 +9559,14 @@
       <c r="E39" s="11" t="n">
         <v>38</v>
       </c>
-      <c r="F39" s="11" t="n">
-        <v>5</v>
+      <c r="F39" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I39" s="11" t="s">
         <v>51</v>
@@ -9750,14 +9744,14 @@
       <c r="E40" s="11" t="n">
         <v>39</v>
       </c>
-      <c r="F40" s="11" t="n">
-        <v>5</v>
+      <c r="F40" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I40" s="11" t="s">
         <v>52</v>
@@ -9935,14 +9929,14 @@
       <c r="E41" s="11" t="n">
         <v>40</v>
       </c>
-      <c r="F41" s="11" t="n">
-        <v>5</v>
+      <c r="F41" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I41" s="11" t="s">
         <v>51</v>
@@ -10120,14 +10114,14 @@
       <c r="E42" s="11" t="n">
         <v>41</v>
       </c>
-      <c r="F42" s="11" t="n">
-        <v>5</v>
+      <c r="F42" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I42" s="11" t="s">
         <v>52</v>
@@ -10305,14 +10299,14 @@
       <c r="E43" s="11" t="n">
         <v>42</v>
       </c>
-      <c r="F43" s="11" t="n">
-        <v>5</v>
+      <c r="F43" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I43" s="11" t="s">
         <v>51</v>
@@ -10490,14 +10484,14 @@
       <c r="E44" s="11" t="n">
         <v>43</v>
       </c>
-      <c r="F44" s="11" t="n">
-        <v>5</v>
+      <c r="F44" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I44" s="11" t="s">
         <v>52</v>
@@ -10675,14 +10669,14 @@
       <c r="E45" s="11" t="n">
         <v>44</v>
       </c>
-      <c r="F45" s="11" t="n">
-        <v>5</v>
+      <c r="F45" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I45" s="11" t="s">
         <v>51</v>
@@ -10860,14 +10854,14 @@
       <c r="E46" s="11" t="n">
         <v>45</v>
       </c>
-      <c r="F46" s="11" t="n">
-        <v>5</v>
+      <c r="F46" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I46" s="11" t="s">
         <v>52</v>
@@ -11045,14 +11039,14 @@
       <c r="E47" s="11" t="n">
         <v>46</v>
       </c>
-      <c r="F47" s="11" t="n">
-        <v>5</v>
+      <c r="F47" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I47" s="11" t="s">
         <v>51</v>
@@ -11230,14 +11224,14 @@
       <c r="E48" s="11" t="n">
         <v>47</v>
       </c>
-      <c r="F48" s="11" t="n">
-        <v>5</v>
+      <c r="F48" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I48" s="11" t="s">
         <v>52</v>
@@ -11415,14 +11409,14 @@
       <c r="E49" s="11" t="n">
         <v>48</v>
       </c>
-      <c r="F49" s="11" t="n">
-        <v>5</v>
+      <c r="F49" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I49" s="11" t="s">
         <v>51</v>
@@ -11600,14 +11594,14 @@
       <c r="E50" s="11" t="n">
         <v>49</v>
       </c>
-      <c r="F50" s="11" t="n">
-        <v>5</v>
+      <c r="F50" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>52</v>
@@ -11787,14 +11781,14 @@
       <c r="E51" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="F51" s="11" t="n">
-        <v>5</v>
+      <c r="F51" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>51</v>
@@ -11974,14 +11968,14 @@
       <c r="E52" s="11" t="n">
         <v>51</v>
       </c>
-      <c r="F52" s="11" t="n">
-        <v>5</v>
+      <c r="F52" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>52</v>
@@ -12161,14 +12155,14 @@
       <c r="E53" s="11" t="n">
         <v>52</v>
       </c>
-      <c r="F53" s="11" t="n">
-        <v>5</v>
+      <c r="F53" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>51</v>
@@ -12348,14 +12342,14 @@
       <c r="E54" s="11" t="n">
         <v>53</v>
       </c>
-      <c r="F54" s="11" t="n">
-        <v>5</v>
+      <c r="F54" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>52</v>
@@ -12535,14 +12529,14 @@
       <c r="E55" s="11" t="n">
         <v>54</v>
       </c>
-      <c r="F55" s="11" t="n">
-        <v>5</v>
+      <c r="F55" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>51</v>
@@ -12722,14 +12716,14 @@
       <c r="E56" s="11" t="n">
         <v>55</v>
       </c>
-      <c r="F56" s="11" t="n">
-        <v>5</v>
+      <c r="F56" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>52</v>
@@ -12909,14 +12903,14 @@
       <c r="E57" s="11" t="n">
         <v>56</v>
       </c>
-      <c r="F57" s="11" t="n">
-        <v>5</v>
+      <c r="F57" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>51</v>
@@ -13096,14 +13090,14 @@
       <c r="E58" s="11" t="n">
         <v>57</v>
       </c>
-      <c r="F58" s="11" t="n">
-        <v>5</v>
+      <c r="F58" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I58" s="11" t="s">
         <v>52</v>
@@ -13283,14 +13277,14 @@
       <c r="E59" s="11" t="n">
         <v>58</v>
       </c>
-      <c r="F59" s="11" t="n">
-        <v>5</v>
+      <c r="F59" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I59" s="11" t="s">
         <v>51</v>
@@ -13470,14 +13464,14 @@
       <c r="E60" s="11" t="n">
         <v>59</v>
       </c>
-      <c r="F60" s="11" t="n">
-        <v>5</v>
+      <c r="F60" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I60" s="11" t="s">
         <v>52</v>
@@ -13657,14 +13651,14 @@
       <c r="E61" s="11" t="n">
         <v>60</v>
       </c>
-      <c r="F61" s="11" t="n">
-        <v>5</v>
+      <c r="F61" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I61" s="11" t="s">
         <v>51</v>
@@ -13844,14 +13838,14 @@
       <c r="E62" s="11" t="n">
         <v>61</v>
       </c>
-      <c r="F62" s="11" t="n">
-        <v>5</v>
+      <c r="F62" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I62" s="11" t="s">
         <v>52</v>
@@ -14031,14 +14025,14 @@
       <c r="E63" s="11" t="n">
         <v>62</v>
       </c>
-      <c r="F63" s="11" t="n">
-        <v>5</v>
+      <c r="F63" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I63" s="11" t="s">
         <v>51</v>
@@ -14218,14 +14212,14 @@
       <c r="E64" s="11" t="n">
         <v>63</v>
       </c>
-      <c r="F64" s="11" t="n">
-        <v>5</v>
+      <c r="F64" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I64" s="11" t="s">
         <v>52</v>
@@ -14405,14 +14399,14 @@
       <c r="E65" s="11" t="n">
         <v>64</v>
       </c>
-      <c r="F65" s="11" t="n">
-        <v>5</v>
+      <c r="F65" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I65" s="11" t="s">
         <v>51</v>
@@ -14592,14 +14586,14 @@
       <c r="E66" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="F66" s="11" t="n">
-        <v>5</v>
+      <c r="F66" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>52</v>
@@ -14779,14 +14773,14 @@
       <c r="E67" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="F67" s="11" t="n">
-        <v>5</v>
+      <c r="F67" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>51</v>
@@ -14966,14 +14960,14 @@
       <c r="E68" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F68" s="11" t="n">
-        <v>5</v>
+      <c r="F68" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I68" s="11" t="s">
         <v>52</v>
@@ -15153,14 +15147,14 @@
       <c r="E69" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F69" s="11" t="n">
-        <v>5</v>
+      <c r="F69" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I69" s="11" t="s">
         <v>51</v>
@@ -15340,14 +15334,14 @@
       <c r="E70" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F70" s="11" t="n">
-        <v>5</v>
+      <c r="F70" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I70" s="11" t="s">
         <v>52</v>
@@ -15527,14 +15521,14 @@
       <c r="E71" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="F71" s="11" t="n">
-        <v>5</v>
+      <c r="F71" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I71" s="11" t="s">
         <v>51</v>
@@ -15714,14 +15708,14 @@
       <c r="E72" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="F72" s="11" t="n">
-        <v>5</v>
+      <c r="F72" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I72" s="11" t="s">
         <v>52</v>
@@ -15901,14 +15895,14 @@
       <c r="E73" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="F73" s="11" t="n">
-        <v>5</v>
+      <c r="F73" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I73" s="11" t="s">
         <v>51</v>
@@ -16088,14 +16082,14 @@
       <c r="E74" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="F74" s="11" t="n">
-        <v>5</v>
+      <c r="F74" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I74" s="11" t="s">
         <v>52</v>
@@ -16275,14 +16269,14 @@
       <c r="E75" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F75" s="11" t="n">
-        <v>5</v>
+      <c r="F75" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I75" s="11" t="s">
         <v>51</v>
@@ -16462,14 +16456,14 @@
       <c r="E76" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="F76" s="11" t="n">
-        <v>5</v>
+      <c r="F76" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I76" s="11" t="s">
         <v>52</v>
@@ -16649,14 +16643,14 @@
       <c r="E77" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="F77" s="11" t="n">
-        <v>5</v>
+      <c r="F77" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I77" s="11" t="s">
         <v>51</v>
@@ -16836,14 +16830,14 @@
       <c r="E78" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="F78" s="11" t="n">
-        <v>5</v>
+      <c r="F78" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I78" s="11" t="s">
         <v>52</v>
@@ -17023,14 +17017,14 @@
       <c r="E79" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="F79" s="11" t="n">
-        <v>5</v>
+      <c r="F79" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I79" s="11" t="s">
         <v>51</v>
@@ -17210,14 +17204,14 @@
       <c r="E80" s="11" t="n">
         <v>15</v>
       </c>
-      <c r="F80" s="11" t="n">
-        <v>5</v>
+      <c r="F80" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>52</v>
@@ -17397,14 +17391,14 @@
       <c r="E81" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="F81" s="11" t="n">
-        <v>5</v>
+      <c r="F81" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I81" s="11" t="s">
         <v>51</v>
@@ -17584,14 +17578,14 @@
       <c r="E82" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="F82" s="11" t="n">
-        <v>5</v>
+      <c r="F82" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I82" s="11" t="s">
         <v>52</v>
@@ -17771,14 +17765,14 @@
       <c r="E83" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="F83" s="11" t="n">
-        <v>5</v>
+      <c r="F83" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I83" s="11" t="s">
         <v>51</v>
@@ -17958,14 +17952,14 @@
       <c r="E84" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="F84" s="11" t="n">
-        <v>5</v>
+      <c r="F84" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I84" s="11" t="s">
         <v>52</v>
@@ -18145,14 +18139,14 @@
       <c r="E85" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="F85" s="11" t="n">
-        <v>5</v>
+      <c r="F85" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I85" s="11" t="s">
         <v>51</v>
@@ -18332,14 +18326,14 @@
       <c r="E86" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="F86" s="11" t="n">
-        <v>5</v>
+      <c r="F86" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I86" s="11" t="s">
         <v>52</v>
@@ -18519,14 +18513,14 @@
       <c r="E87" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="F87" s="11" t="n">
-        <v>5</v>
+      <c r="F87" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I87" s="11" t="s">
         <v>51</v>
@@ -18706,14 +18700,14 @@
       <c r="E88" s="11" t="n">
         <v>23</v>
       </c>
-      <c r="F88" s="11" t="n">
-        <v>5</v>
+      <c r="F88" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I88" s="11" t="s">
         <v>52</v>
@@ -18893,14 +18887,14 @@
       <c r="E89" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="F89" s="11" t="n">
-        <v>5</v>
+      <c r="F89" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I89" s="11" t="s">
         <v>51</v>
@@ -19080,14 +19074,14 @@
       <c r="E90" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="F90" s="11" t="n">
-        <v>5</v>
+      <c r="F90" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I90" s="11" t="s">
         <v>52</v>
@@ -19267,14 +19261,14 @@
       <c r="E91" s="11" t="n">
         <v>26</v>
       </c>
-      <c r="F91" s="11" t="n">
-        <v>5</v>
+      <c r="F91" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I91" s="11" t="s">
         <v>51</v>
@@ -19454,14 +19448,14 @@
       <c r="E92" s="11" t="n">
         <v>27</v>
       </c>
-      <c r="F92" s="11" t="n">
-        <v>5</v>
+      <c r="F92" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I92" s="11" t="s">
         <v>52</v>
@@ -19641,14 +19635,14 @@
       <c r="E93" s="11" t="n">
         <v>28</v>
       </c>
-      <c r="F93" s="11" t="n">
-        <v>5</v>
+      <c r="F93" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I93" s="11" t="s">
         <v>51</v>
@@ -19828,14 +19822,14 @@
       <c r="E94" s="11" t="n">
         <v>29</v>
       </c>
-      <c r="F94" s="11" t="n">
-        <v>5</v>
+      <c r="F94" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I94" s="11" t="s">
         <v>52</v>
@@ -20015,14 +20009,14 @@
       <c r="E95" s="11" t="n">
         <v>30</v>
       </c>
-      <c r="F95" s="11" t="n">
-        <v>5</v>
+      <c r="F95" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>51</v>
@@ -20202,14 +20196,14 @@
       <c r="E96" s="11" t="n">
         <v>31</v>
       </c>
-      <c r="F96" s="11" t="n">
-        <v>5</v>
+      <c r="F96" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>52</v>
@@ -20389,14 +20383,14 @@
       <c r="E97" s="11" t="n">
         <v>32</v>
       </c>
-      <c r="F97" s="11" t="n">
-        <v>5</v>
+      <c r="F97" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>51</v>
@@ -20576,14 +20570,14 @@
       <c r="E98" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="F98" s="11" t="n">
-        <v>5</v>
+      <c r="F98" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>52</v>
@@ -20761,14 +20755,14 @@
       <c r="E99" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="F99" s="11" t="n">
-        <v>5</v>
+      <c r="F99" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I99" s="11" t="s">
         <v>51</v>
@@ -20946,14 +20940,14 @@
       <c r="E100" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F100" s="11" t="n">
-        <v>5</v>
+      <c r="F100" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>52</v>
@@ -21131,14 +21125,14 @@
       <c r="E101" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F101" s="11" t="n">
-        <v>5</v>
+      <c r="F101" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G101" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>51</v>
@@ -21316,14 +21310,14 @@
       <c r="E102" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F102" s="11" t="n">
-        <v>5</v>
+      <c r="F102" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I102" s="11" t="s">
         <v>52</v>
@@ -21501,14 +21495,14 @@
       <c r="E103" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="F103" s="11" t="n">
-        <v>5</v>
+      <c r="F103" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G103" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>51</v>
@@ -21686,14 +21680,14 @@
       <c r="E104" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="F104" s="11" t="n">
-        <v>5</v>
+      <c r="F104" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G104" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I104" s="11" t="s">
         <v>52</v>
@@ -21871,14 +21865,14 @@
       <c r="E105" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="F105" s="11" t="n">
-        <v>5</v>
+      <c r="F105" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G105" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I105" s="11" t="s">
         <v>51</v>
@@ -22056,14 +22050,14 @@
       <c r="E106" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="F106" s="11" t="n">
-        <v>5</v>
+      <c r="F106" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H106" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I106" s="11" t="s">
         <v>52</v>
@@ -22241,14 +22235,14 @@
       <c r="E107" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="F107" s="11" t="n">
-        <v>5</v>
+      <c r="F107" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H107" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I107" s="11" t="s">
         <v>51</v>
@@ -22426,14 +22420,14 @@
       <c r="E108" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="F108" s="11" t="n">
-        <v>5</v>
+      <c r="F108" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G108" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H108" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I108" s="11" t="s">
         <v>52</v>
@@ -22611,14 +22605,14 @@
       <c r="E109" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="F109" s="11" t="n">
-        <v>5</v>
+      <c r="F109" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H109" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I109" s="11" t="s">
         <v>51</v>
@@ -22792,14 +22786,14 @@
       <c r="E110" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="F110" s="11" t="n">
-        <v>5</v>
+      <c r="F110" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H110" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I110" s="11" t="s">
         <v>52</v>
@@ -22973,14 +22967,14 @@
       <c r="E111" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="F111" s="11" t="n">
-        <v>5</v>
+      <c r="F111" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I111" s="11" t="s">
         <v>51</v>
@@ -23154,14 +23148,14 @@
       <c r="E112" s="11" t="n">
         <v>15</v>
       </c>
-      <c r="F112" s="11" t="n">
-        <v>5</v>
+      <c r="F112" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I112" s="11" t="s">
         <v>52</v>
@@ -23335,14 +23329,14 @@
       <c r="E113" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="F113" s="11" t="n">
-        <v>5</v>
+      <c r="F113" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H113" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I113" s="11" t="s">
         <v>51</v>
@@ -23516,14 +23510,14 @@
       <c r="E114" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="F114" s="11" t="n">
-        <v>5</v>
+      <c r="F114" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I114" s="11" t="s">
         <v>52</v>
@@ -23697,14 +23691,14 @@
       <c r="E115" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="F115" s="11" t="n">
-        <v>5</v>
+      <c r="F115" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H115" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I115" s="11" t="s">
         <v>51</v>
@@ -23878,14 +23872,14 @@
       <c r="E116" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="F116" s="11" t="n">
-        <v>5</v>
+      <c r="F116" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H116" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I116" s="11" t="s">
         <v>52</v>
@@ -24059,14 +24053,14 @@
       <c r="E117" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="F117" s="11" t="n">
-        <v>5</v>
+      <c r="F117" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H117" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>51</v>
@@ -24240,14 +24234,14 @@
       <c r="E118" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="F118" s="11" t="n">
-        <v>5</v>
+      <c r="F118" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>52</v>
@@ -24421,14 +24415,14 @@
       <c r="E119" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="F119" s="11" t="n">
-        <v>5</v>
+      <c r="F119" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>51</v>
@@ -24602,14 +24596,14 @@
       <c r="E120" s="11" t="n">
         <v>23</v>
       </c>
-      <c r="F120" s="11" t="n">
-        <v>5</v>
+      <c r="F120" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G120" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>52</v>
@@ -24783,14 +24777,14 @@
       <c r="E121" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="F121" s="11" t="n">
-        <v>5</v>
+      <c r="F121" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G121" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H121" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I121" s="11" t="s">
         <v>51</v>
@@ -24968,14 +24962,14 @@
       <c r="E122" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="F122" s="11" t="n">
-        <v>5</v>
+      <c r="F122" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G122" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H122" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I122" s="11" t="s">
         <v>52</v>
@@ -25153,14 +25147,14 @@
       <c r="E123" s="11" t="n">
         <v>26</v>
       </c>
-      <c r="F123" s="11" t="n">
-        <v>5</v>
+      <c r="F123" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H123" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I123" s="11" t="s">
         <v>51</v>
@@ -25338,14 +25332,14 @@
       <c r="E124" s="11" t="n">
         <v>27</v>
       </c>
-      <c r="F124" s="11" t="n">
-        <v>5</v>
+      <c r="F124" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H124" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I124" s="11" t="s">
         <v>52</v>
@@ -25523,14 +25517,14 @@
       <c r="E125" s="11" t="n">
         <v>28</v>
       </c>
-      <c r="F125" s="11" t="n">
-        <v>5</v>
+      <c r="F125" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G125" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H125" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I125" s="11" t="s">
         <v>51</v>
@@ -25708,14 +25702,14 @@
       <c r="E126" s="11" t="n">
         <v>29</v>
       </c>
-      <c r="F126" s="11" t="n">
-        <v>5</v>
+      <c r="F126" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H126" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I126" s="11" t="s">
         <v>52</v>
@@ -25893,14 +25887,14 @@
       <c r="E127" s="11" t="n">
         <v>30</v>
       </c>
-      <c r="F127" s="11" t="n">
-        <v>5</v>
+      <c r="F127" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G127" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H127" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I127" s="11" t="s">
         <v>51</v>
@@ -26078,14 +26072,14 @@
       <c r="E128" s="11" t="n">
         <v>31</v>
       </c>
-      <c r="F128" s="11" t="n">
-        <v>5</v>
+      <c r="F128" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G128" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I128" s="11" t="s">
         <v>52</v>
@@ -26263,14 +26257,14 @@
       <c r="E129" s="11" t="n">
         <v>32</v>
       </c>
-      <c r="F129" s="11" t="n">
-        <v>5</v>
+      <c r="F129" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G129" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H129" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I129" s="11" t="s">
         <v>51</v>
@@ -26451,7 +26445,7 @@
       <c r="AB133" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O4:O1048576 O1 C1:E1048576 F1:H1 G130:H1048576 F5:F1048576">
+  <conditionalFormatting sqref="O4:O1048576 O1 C1:E1048576 F1:H1 G130:H1048576 F3:F13 F18:F1048576 G28:H28">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"purple"</formula>
     </cfRule>
@@ -26474,7 +26468,7 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2" type="list">
       <formula1>"-,blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
@@ -26515,12 +26509,16 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F129" type="list">
-      <formula1>"+5,+10,+15,+20,+25,+30,+35,+40,+45,+50,+55,+60,"</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F13 F15:F29 G28:H28 F30:F129" type="list">
+      <formula1>"-,+5,+10,+15,+20,+25,+30,+35,+40,+45,+50,+55,+60,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:H129" type="list">
-      <formula1>"yes,no"</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G13 G15:G27 G29:G129" type="list">
+      <formula1>"-,yes,no"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H13 H15:H27 H29:H129" type="list">
+      <formula1>"-,yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Name support for UFX Send and Return Color support for UFX Send and Return version increased spreadsheets updated typo fixed
</commit_message>
<xml_diff>
--- a/testing/dLiveChannelListTesting.xlsx
+++ b/testing/dLiveChannelListTesting.xlsx
@@ -23,8 +23,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*) Only for CSV Director Import</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="614">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -35,19 +58,19 @@
     <t xml:space="preserve">Color</t>
   </si>
   <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phantom</t>
+    <t xml:space="preserve">Source*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pad*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phantom*</t>
   </si>
   <si>
     <t xml:space="preserve">Mute</t>
@@ -716,6 +739,24 @@
     <t xml:space="preserve">FX Return Color</t>
   </si>
   <si>
+    <t xml:space="preserve">UFX Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFX Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFX Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFX Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFX Return Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFX Return Color</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca1</t>
   </si>
   <si>
@@ -746,6 +787,12 @@
     <t xml:space="preserve">FxRet1</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca2</t>
   </si>
   <si>
@@ -776,6 +823,12 @@
     <t xml:space="preserve">FxRet2</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca3</t>
   </si>
   <si>
@@ -806,6 +859,12 @@
     <t xml:space="preserve">FxRet3</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca4</t>
   </si>
   <si>
@@ -836,6 +895,12 @@
     <t xml:space="preserve">FxRet4</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca5</t>
   </si>
   <si>
@@ -866,6 +931,12 @@
     <t xml:space="preserve">FxRet5</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca6</t>
   </si>
   <si>
@@ -896,6 +967,12 @@
     <t xml:space="preserve">FxRet6</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca7</t>
   </si>
   <si>
@@ -926,6 +1003,12 @@
     <t xml:space="preserve">FxRet7</t>
   </si>
   <si>
+    <t xml:space="preserve">UFx7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dca8</t>
   </si>
   <si>
@@ -954,6 +1037,12 @@
   </si>
   <si>
     <t xml:space="preserve">FxRet8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFx8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFxRet8</t>
   </si>
   <si>
     <t xml:space="preserve">Dca9</t>
@@ -1816,7 +1905,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1846,6 +1935,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2090,11 +2185,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2138,7 +2233,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2150,11 +2245,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -26557,6 +26652,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -29634,7 +29730,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AU73"/>
+  <dimension ref="A1:BC73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -29676,6 +29772,9 @@
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="43" min="43" style="3" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="3" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="3" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="11.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="16.61"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29782,13 +29881,31 @@
       <c r="AU1" s="25" t="s">
         <v>228</v>
       </c>
+      <c r="AW1" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="AX1" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="AY1" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="BA1" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="BB1" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="BC1" s="25" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>49</v>
@@ -29797,7 +29914,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>49</v>
@@ -29810,7 +29927,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>49</v>
@@ -29824,7 +29941,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="28" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="Q2" s="11" t="s">
         <v>49</v>
@@ -29838,7 +29955,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>49</v>
@@ -29851,7 +29968,7 @@
         <v>1</v>
       </c>
       <c r="Z2" s="28" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="AA2" s="11" t="s">
         <v>49</v>
@@ -29865,7 +29982,7 @@
         <v>1</v>
       </c>
       <c r="AE2" s="28" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="AF2" s="11" t="s">
         <v>49</v>
@@ -29878,7 +29995,7 @@
         <v>1</v>
       </c>
       <c r="AJ2" s="28" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="AK2" s="11" t="s">
         <v>49</v>
@@ -29892,7 +30009,7 @@
         <v>1</v>
       </c>
       <c r="AO2" s="28" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="AP2" s="11" t="s">
         <v>49</v>
@@ -29906,9 +30023,28 @@
         <v>1</v>
       </c>
       <c r="AT2" s="28" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="AU2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW2" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="AY2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC2" s="11" t="s">
         <v>49</v>
       </c>
     </row>
@@ -29917,7 +30053,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>67</v>
@@ -29926,7 +30062,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>67</v>
@@ -29939,7 +30075,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>67</v>
@@ -29953,7 +30089,7 @@
         <v>2</v>
       </c>
       <c r="P3" s="28" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="Q3" s="11" t="s">
         <v>67</v>
@@ -29967,7 +30103,7 @@
         <v>2</v>
       </c>
       <c r="U3" s="28" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="V3" s="11" t="s">
         <v>67</v>
@@ -29980,7 +30116,7 @@
         <v>2</v>
       </c>
       <c r="Z3" s="28" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="AA3" s="11" t="s">
         <v>67</v>
@@ -29994,7 +30130,7 @@
         <v>2</v>
       </c>
       <c r="AE3" s="28" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="AF3" s="11" t="s">
         <v>67</v>
@@ -30007,7 +30143,7 @@
         <v>2</v>
       </c>
       <c r="AJ3" s="28" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="AK3" s="11" t="s">
         <v>67</v>
@@ -30021,7 +30157,7 @@
         <v>2</v>
       </c>
       <c r="AO3" s="28" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="AP3" s="11" t="s">
         <v>67</v>
@@ -30035,9 +30171,28 @@
         <v>2</v>
       </c>
       <c r="AT3" s="28" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="AU3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW3" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX3" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="AY3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB3" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="BC3" s="11" t="s">
         <v>67</v>
       </c>
     </row>
@@ -30046,7 +30201,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>80</v>
@@ -30055,7 +30210,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>80</v>
@@ -30068,7 +30223,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>80</v>
@@ -30082,7 +30237,7 @@
         <v>3</v>
       </c>
       <c r="P4" s="28" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>80</v>
@@ -30096,7 +30251,7 @@
         <v>3</v>
       </c>
       <c r="U4" s="28" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="V4" s="11" t="s">
         <v>80</v>
@@ -30109,7 +30264,7 @@
         <v>3</v>
       </c>
       <c r="Z4" s="28" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="AA4" s="11" t="s">
         <v>80</v>
@@ -30123,7 +30278,7 @@
         <v>3</v>
       </c>
       <c r="AE4" s="28" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="AF4" s="11" t="s">
         <v>80</v>
@@ -30136,7 +30291,7 @@
         <v>3</v>
       </c>
       <c r="AJ4" s="28" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="AK4" s="11" t="s">
         <v>80</v>
@@ -30150,7 +30305,7 @@
         <v>3</v>
       </c>
       <c r="AO4" s="28" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="AP4" s="11" t="s">
         <v>80</v>
@@ -30164,9 +30319,28 @@
         <v>3</v>
       </c>
       <c r="AT4" s="28" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="AU4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW4" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX4" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="AY4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB4" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="BC4" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -30175,7 +30349,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>93</v>
@@ -30184,7 +30358,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>93</v>
@@ -30197,7 +30371,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>93</v>
@@ -30211,7 +30385,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="Q5" s="11" t="s">
         <v>93</v>
@@ -30225,7 +30399,7 @@
         <v>4</v>
       </c>
       <c r="U5" s="28" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="V5" s="11" t="s">
         <v>93</v>
@@ -30238,7 +30412,7 @@
         <v>4</v>
       </c>
       <c r="Z5" s="28" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="AA5" s="11" t="s">
         <v>93</v>
@@ -30252,7 +30426,7 @@
         <v>4</v>
       </c>
       <c r="AE5" s="28" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="AF5" s="11" t="s">
         <v>93</v>
@@ -30265,7 +30439,7 @@
         <v>4</v>
       </c>
       <c r="AJ5" s="28" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="AK5" s="11" t="s">
         <v>93</v>
@@ -30279,7 +30453,7 @@
         <v>4</v>
       </c>
       <c r="AO5" s="28" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="AP5" s="11" t="s">
         <v>93</v>
@@ -30293,9 +30467,28 @@
         <v>4</v>
       </c>
       <c r="AT5" s="28" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="AU5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW5" s="26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AX5" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="AY5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="26" t="n">
+        <v>4</v>
+      </c>
+      <c r="BB5" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="BC5" s="11" t="s">
         <v>93</v>
       </c>
     </row>
@@ -30304,7 +30497,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>106</v>
@@ -30313,7 +30506,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>106</v>
@@ -30326,7 +30519,7 @@
         <v>5</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>106</v>
@@ -30340,7 +30533,7 @@
         <v>5</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="Q6" s="11" t="s">
         <v>106</v>
@@ -30354,7 +30547,7 @@
         <v>5</v>
       </c>
       <c r="U6" s="28" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="V6" s="11" t="s">
         <v>106</v>
@@ -30367,7 +30560,7 @@
         <v>5</v>
       </c>
       <c r="Z6" s="28" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="AA6" s="11" t="s">
         <v>106</v>
@@ -30381,7 +30574,7 @@
         <v>5</v>
       </c>
       <c r="AE6" s="28" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="AF6" s="11" t="s">
         <v>106</v>
@@ -30394,7 +30587,7 @@
         <v>5</v>
       </c>
       <c r="AJ6" s="28" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="AK6" s="11" t="s">
         <v>106</v>
@@ -30408,7 +30601,7 @@
         <v>5</v>
       </c>
       <c r="AO6" s="28" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="AP6" s="11" t="s">
         <v>106</v>
@@ -30422,9 +30615,28 @@
         <v>5</v>
       </c>
       <c r="AT6" s="28" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="AU6" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW6" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="AX6" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="AY6" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="BB6" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="BC6" s="11" t="s">
         <v>106</v>
       </c>
     </row>
@@ -30433,7 +30645,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>119</v>
@@ -30443,7 +30655,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>119</v>
@@ -30456,7 +30668,7 @@
         <v>6</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="L7" s="30" t="s">
         <v>119</v>
@@ -30470,7 +30682,7 @@
         <v>6</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="Q7" s="30" t="s">
         <v>119</v>
@@ -30484,7 +30696,7 @@
         <v>6</v>
       </c>
       <c r="U7" s="28" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="V7" s="30" t="s">
         <v>119</v>
@@ -30497,7 +30709,7 @@
         <v>6</v>
       </c>
       <c r="Z7" s="28" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="AA7" s="30" t="s">
         <v>119</v>
@@ -30511,7 +30723,7 @@
         <v>6</v>
       </c>
       <c r="AE7" s="28" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="AF7" s="30" t="s">
         <v>119</v>
@@ -30524,7 +30736,7 @@
         <v>6</v>
       </c>
       <c r="AJ7" s="28" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="AK7" s="30" t="s">
         <v>119</v>
@@ -30538,7 +30750,7 @@
         <v>6</v>
       </c>
       <c r="AO7" s="28" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="AP7" s="30" t="s">
         <v>119</v>
@@ -30552,9 +30764,28 @@
         <v>6</v>
       </c>
       <c r="AT7" s="28" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="AU7" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW7" s="26" t="n">
+        <v>6</v>
+      </c>
+      <c r="AX7" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="AY7" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="26" t="n">
+        <v>6</v>
+      </c>
+      <c r="BB7" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="BC7" s="30" t="s">
         <v>119</v>
       </c>
     </row>
@@ -30563,7 +30794,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>133</v>
@@ -30572,7 +30803,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="G8" s="30" t="s">
         <v>133</v>
@@ -30585,7 +30816,7 @@
         <v>7</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="L8" s="30" t="s">
         <v>133</v>
@@ -30599,7 +30830,7 @@
         <v>7</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="Q8" s="30" t="s">
         <v>133</v>
@@ -30613,7 +30844,7 @@
         <v>7</v>
       </c>
       <c r="U8" s="28" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="V8" s="30" t="s">
         <v>133</v>
@@ -30626,7 +30857,7 @@
         <v>7</v>
       </c>
       <c r="Z8" s="28" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="AA8" s="30" t="s">
         <v>133</v>
@@ -30640,7 +30871,7 @@
         <v>7</v>
       </c>
       <c r="AE8" s="28" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="AF8" s="30" t="s">
         <v>133</v>
@@ -30653,7 +30884,7 @@
         <v>7</v>
       </c>
       <c r="AJ8" s="28" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="AK8" s="30" t="s">
         <v>133</v>
@@ -30667,7 +30898,7 @@
         <v>7</v>
       </c>
       <c r="AO8" s="28" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="AP8" s="30" t="s">
         <v>133</v>
@@ -30681,9 +30912,28 @@
         <v>7</v>
       </c>
       <c r="AT8" s="28" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="AU8" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="AW8" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="AX8" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="AY8" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="BB8" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="BC8" s="30" t="s">
         <v>133</v>
       </c>
     </row>
@@ -30692,7 +30942,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>146</v>
@@ -30701,7 +30951,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>146</v>
@@ -30714,7 +30964,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="28" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>146</v>
@@ -30728,7 +30978,7 @@
         <v>8</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="Q9" s="30" t="s">
         <v>146</v>
@@ -30742,7 +30992,7 @@
         <v>8</v>
       </c>
       <c r="U9" s="28" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="V9" s="30" t="s">
         <v>146</v>
@@ -30755,7 +31005,7 @@
         <v>8</v>
       </c>
       <c r="Z9" s="28" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="AA9" s="30" t="s">
         <v>146</v>
@@ -30769,7 +31019,7 @@
         <v>8</v>
       </c>
       <c r="AE9" s="28" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="AF9" s="30" t="s">
         <v>146</v>
@@ -30782,7 +31032,7 @@
         <v>8</v>
       </c>
       <c r="AJ9" s="28" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="AK9" s="30" t="s">
         <v>146</v>
@@ -30796,7 +31046,7 @@
         <v>8</v>
       </c>
       <c r="AO9" s="28" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="AP9" s="30" t="s">
         <v>146</v>
@@ -30810,9 +31060,28 @@
         <v>8</v>
       </c>
       <c r="AT9" s="28" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="AU9" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="AW9" s="26" t="n">
+        <v>8</v>
+      </c>
+      <c r="AX9" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="AY9" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="26" t="n">
+        <v>8</v>
+      </c>
+      <c r="BB9" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="BC9" s="30" t="s">
         <v>146</v>
       </c>
     </row>
@@ -30821,7 +31090,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>49</v>
@@ -30830,7 +31099,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="G10" s="30" t="s">
         <v>49</v>
@@ -30843,7 +31112,7 @@
         <v>9</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="L10" s="30" t="s">
         <v>49</v>
@@ -30857,7 +31126,7 @@
         <v>9</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>312</v>
+        <v>334</v>
       </c>
       <c r="Q10" s="30" t="s">
         <v>49</v>
@@ -30871,7 +31140,7 @@
         <v>9</v>
       </c>
       <c r="U10" s="28" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
       <c r="V10" s="30" t="s">
         <v>49</v>
@@ -30884,7 +31153,7 @@
         <v>9</v>
       </c>
       <c r="Z10" s="28" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
       <c r="AA10" s="30" t="s">
         <v>49</v>
@@ -30898,7 +31167,7 @@
         <v>9</v>
       </c>
       <c r="AE10" s="28" t="s">
-        <v>315</v>
+        <v>337</v>
       </c>
       <c r="AF10" s="30" t="s">
         <v>49</v>
@@ -30911,7 +31180,7 @@
         <v>9</v>
       </c>
       <c r="AJ10" s="28" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="AK10" s="30" t="s">
         <v>49</v>
@@ -30925,7 +31194,7 @@
         <v>9</v>
       </c>
       <c r="AO10" s="28" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="AP10" s="30" t="s">
         <v>49</v>
@@ -30939,7 +31208,7 @@
         <v>9</v>
       </c>
       <c r="AT10" s="28" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="AU10" s="30" t="s">
         <v>49</v>
@@ -30950,7 +31219,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>67</v>
@@ -30959,7 +31228,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>67</v>
@@ -30972,7 +31241,7 @@
         <v>10</v>
       </c>
       <c r="K11" s="28" t="s">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="L11" s="30" t="s">
         <v>67</v>
@@ -30986,7 +31255,7 @@
         <v>10</v>
       </c>
       <c r="P11" s="28" t="s">
-        <v>322</v>
+        <v>344</v>
       </c>
       <c r="Q11" s="30" t="s">
         <v>67</v>
@@ -31000,7 +31269,7 @@
         <v>10</v>
       </c>
       <c r="U11" s="28" t="s">
-        <v>323</v>
+        <v>345</v>
       </c>
       <c r="V11" s="30" t="s">
         <v>67</v>
@@ -31013,7 +31282,7 @@
         <v>10</v>
       </c>
       <c r="Z11" s="28" t="s">
-        <v>324</v>
+        <v>346</v>
       </c>
       <c r="AA11" s="30" t="s">
         <v>67</v>
@@ -31027,7 +31296,7 @@
         <v>10</v>
       </c>
       <c r="AE11" s="28" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="AF11" s="30" t="s">
         <v>67</v>
@@ -31040,7 +31309,7 @@
         <v>10</v>
       </c>
       <c r="AJ11" s="28" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="AK11" s="30" t="s">
         <v>67</v>
@@ -31054,7 +31323,7 @@
         <v>10</v>
       </c>
       <c r="AO11" s="28" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="AP11" s="30" t="s">
         <v>67</v>
@@ -31068,7 +31337,7 @@
         <v>10</v>
       </c>
       <c r="AT11" s="28" t="s">
-        <v>328</v>
+        <v>350</v>
       </c>
       <c r="AU11" s="30" t="s">
         <v>67</v>
@@ -31079,7 +31348,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>80</v>
@@ -31088,7 +31357,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>80</v>
@@ -31101,7 +31370,7 @@
         <v>11</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="L12" s="30" t="s">
         <v>80</v>
@@ -31115,7 +31384,7 @@
         <v>11</v>
       </c>
       <c r="P12" s="28" t="s">
-        <v>332</v>
+        <v>354</v>
       </c>
       <c r="Q12" s="30" t="s">
         <v>80</v>
@@ -31129,7 +31398,7 @@
         <v>11</v>
       </c>
       <c r="U12" s="28" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="V12" s="30" t="s">
         <v>80</v>
@@ -31142,7 +31411,7 @@
         <v>11</v>
       </c>
       <c r="Z12" s="28" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="AA12" s="30" t="s">
         <v>80</v>
@@ -31156,7 +31425,7 @@
         <v>11</v>
       </c>
       <c r="AE12" s="28" t="s">
-        <v>335</v>
+        <v>357</v>
       </c>
       <c r="AF12" s="30" t="s">
         <v>80</v>
@@ -31169,7 +31438,7 @@
         <v>11</v>
       </c>
       <c r="AJ12" s="28" t="s">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="AK12" s="30" t="s">
         <v>80</v>
@@ -31183,7 +31452,7 @@
         <v>11</v>
       </c>
       <c r="AO12" s="28" t="s">
-        <v>337</v>
+        <v>359</v>
       </c>
       <c r="AP12" s="30" t="s">
         <v>80</v>
@@ -31197,7 +31466,7 @@
         <v>11</v>
       </c>
       <c r="AT12" s="28" t="s">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="AU12" s="30" t="s">
         <v>80</v>
@@ -31208,7 +31477,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>93</v>
@@ -31217,7 +31486,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>93</v>
@@ -31230,7 +31499,7 @@
         <v>12</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>341</v>
+        <v>363</v>
       </c>
       <c r="L13" s="30" t="s">
         <v>93</v>
@@ -31244,7 +31513,7 @@
         <v>12</v>
       </c>
       <c r="P13" s="28" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="Q13" s="30" t="s">
         <v>93</v>
@@ -31258,7 +31527,7 @@
         <v>12</v>
       </c>
       <c r="U13" s="28" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="V13" s="30" t="s">
         <v>93</v>
@@ -31271,7 +31540,7 @@
         <v>12</v>
       </c>
       <c r="Z13" s="28" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="AA13" s="30" t="s">
         <v>93</v>
@@ -31285,7 +31554,7 @@
         <v>12</v>
       </c>
       <c r="AE13" s="28" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="AF13" s="30" t="s">
         <v>93</v>
@@ -31298,7 +31567,7 @@
         <v>12</v>
       </c>
       <c r="AJ13" s="28" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="AK13" s="30" t="s">
         <v>93</v>
@@ -31312,7 +31581,7 @@
         <v>12</v>
       </c>
       <c r="AO13" s="28" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="AP13" s="30" t="s">
         <v>93</v>
@@ -31326,7 +31595,7 @@
         <v>12</v>
       </c>
       <c r="AT13" s="28" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
       <c r="AU13" s="30" t="s">
         <v>93</v>
@@ -31337,7 +31606,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>106</v>
@@ -31346,7 +31615,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="G14" s="30" t="s">
         <v>106</v>
@@ -31359,7 +31628,7 @@
         <v>13</v>
       </c>
       <c r="K14" s="28" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="L14" s="30" t="s">
         <v>106</v>
@@ -31373,7 +31642,7 @@
         <v>13</v>
       </c>
       <c r="P14" s="28" t="s">
-        <v>352</v>
+        <v>374</v>
       </c>
       <c r="Q14" s="30" t="s">
         <v>106</v>
@@ -31387,7 +31656,7 @@
         <v>13</v>
       </c>
       <c r="U14" s="28" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
       <c r="V14" s="30" t="s">
         <v>106</v>
@@ -31400,7 +31669,7 @@
         <v>13</v>
       </c>
       <c r="Z14" s="28" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="AA14" s="30" t="s">
         <v>106</v>
@@ -31414,7 +31683,7 @@
         <v>13</v>
       </c>
       <c r="AE14" s="28" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
       <c r="AF14" s="30" t="s">
         <v>106</v>
@@ -31427,7 +31696,7 @@
         <v>13</v>
       </c>
       <c r="AJ14" s="28" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="AK14" s="30" t="s">
         <v>106</v>
@@ -31441,7 +31710,7 @@
         <v>13</v>
       </c>
       <c r="AO14" s="28" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="AP14" s="30" t="s">
         <v>106</v>
@@ -31455,7 +31724,7 @@
         <v>13</v>
       </c>
       <c r="AT14" s="28" t="s">
-        <v>358</v>
+        <v>380</v>
       </c>
       <c r="AU14" s="30" t="s">
         <v>106</v>
@@ -31466,7 +31735,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>359</v>
+        <v>381</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>119</v>
@@ -31475,7 +31744,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>360</v>
+        <v>382</v>
       </c>
       <c r="G15" s="30" t="s">
         <v>119</v>
@@ -31488,7 +31757,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>361</v>
+        <v>383</v>
       </c>
       <c r="L15" s="30" t="s">
         <v>119</v>
@@ -31502,7 +31771,7 @@
         <v>14</v>
       </c>
       <c r="P15" s="28" t="s">
-        <v>362</v>
+        <v>384</v>
       </c>
       <c r="Q15" s="30" t="s">
         <v>119</v>
@@ -31516,7 +31785,7 @@
         <v>14</v>
       </c>
       <c r="U15" s="28" t="s">
-        <v>363</v>
+        <v>385</v>
       </c>
       <c r="V15" s="30" t="s">
         <v>119</v>
@@ -31529,7 +31798,7 @@
         <v>14</v>
       </c>
       <c r="Z15" s="28" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="AA15" s="30" t="s">
         <v>119</v>
@@ -31543,7 +31812,7 @@
         <v>14</v>
       </c>
       <c r="AE15" s="28" t="s">
-        <v>365</v>
+        <v>387</v>
       </c>
       <c r="AF15" s="30" t="s">
         <v>119</v>
@@ -31556,7 +31825,7 @@
         <v>14</v>
       </c>
       <c r="AJ15" s="28" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="AK15" s="30" t="s">
         <v>119</v>
@@ -31570,7 +31839,7 @@
         <v>14</v>
       </c>
       <c r="AO15" s="28" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="AP15" s="30" t="s">
         <v>119</v>
@@ -31584,7 +31853,7 @@
         <v>14</v>
       </c>
       <c r="AT15" s="28" t="s">
-        <v>368</v>
+        <v>390</v>
       </c>
       <c r="AU15" s="30" t="s">
         <v>119</v>
@@ -31595,7 +31864,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>369</v>
+        <v>391</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>133</v>
@@ -31604,7 +31873,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>370</v>
+        <v>392</v>
       </c>
       <c r="G16" s="30" t="s">
         <v>133</v>
@@ -31617,7 +31886,7 @@
         <v>15</v>
       </c>
       <c r="K16" s="28" t="s">
-        <v>371</v>
+        <v>393</v>
       </c>
       <c r="L16" s="30" t="s">
         <v>133</v>
@@ -31631,7 +31900,7 @@
         <v>15</v>
       </c>
       <c r="P16" s="28" t="s">
-        <v>372</v>
+        <v>394</v>
       </c>
       <c r="Q16" s="30" t="s">
         <v>133</v>
@@ -31645,7 +31914,7 @@
         <v>15</v>
       </c>
       <c r="U16" s="28" t="s">
-        <v>373</v>
+        <v>395</v>
       </c>
       <c r="V16" s="30" t="s">
         <v>133</v>
@@ -31658,7 +31927,7 @@
         <v>15</v>
       </c>
       <c r="Z16" s="28" t="s">
-        <v>374</v>
+        <v>396</v>
       </c>
       <c r="AA16" s="30" t="s">
         <v>133</v>
@@ -31672,7 +31941,7 @@
         <v>15</v>
       </c>
       <c r="AE16" s="28" t="s">
-        <v>375</v>
+        <v>397</v>
       </c>
       <c r="AF16" s="30" t="s">
         <v>133</v>
@@ -31685,7 +31954,7 @@
         <v>15</v>
       </c>
       <c r="AJ16" s="28" t="s">
-        <v>376</v>
+        <v>398</v>
       </c>
       <c r="AK16" s="30" t="s">
         <v>53</v>
@@ -31699,7 +31968,7 @@
         <v>15</v>
       </c>
       <c r="AO16" s="28" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="AP16" s="30" t="s">
         <v>53</v>
@@ -31713,7 +31982,7 @@
         <v>15</v>
       </c>
       <c r="AT16" s="28" t="s">
-        <v>378</v>
+        <v>400</v>
       </c>
       <c r="AU16" s="30" t="s">
         <v>53</v>
@@ -31724,7 +31993,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>379</v>
+        <v>401</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>146</v>
@@ -31733,7 +32002,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>380</v>
+        <v>402</v>
       </c>
       <c r="G17" s="30" t="s">
         <v>146</v>
@@ -31746,7 +32015,7 @@
         <v>16</v>
       </c>
       <c r="K17" s="28" t="s">
-        <v>381</v>
+        <v>403</v>
       </c>
       <c r="L17" s="30" t="s">
         <v>146</v>
@@ -31760,7 +32029,7 @@
         <v>16</v>
       </c>
       <c r="P17" s="28" t="s">
-        <v>382</v>
+        <v>404</v>
       </c>
       <c r="Q17" s="30" t="s">
         <v>146</v>
@@ -31774,7 +32043,7 @@
         <v>16</v>
       </c>
       <c r="U17" s="28" t="s">
-        <v>383</v>
+        <v>405</v>
       </c>
       <c r="V17" s="30" t="s">
         <v>146</v>
@@ -31787,7 +32056,7 @@
         <v>16</v>
       </c>
       <c r="Z17" s="28" t="s">
-        <v>384</v>
+        <v>406</v>
       </c>
       <c r="AA17" s="30" t="s">
         <v>146</v>
@@ -31801,7 +32070,7 @@
         <v>16</v>
       </c>
       <c r="AE17" s="28" t="s">
-        <v>385</v>
+        <v>407</v>
       </c>
       <c r="AF17" s="30" t="s">
         <v>146</v>
@@ -31814,7 +32083,7 @@
         <v>16</v>
       </c>
       <c r="AJ17" s="28" t="s">
-        <v>386</v>
+        <v>408</v>
       </c>
       <c r="AK17" s="30"/>
       <c r="AL17" s="2" t="n">
@@ -31826,7 +32095,7 @@
         <v>16</v>
       </c>
       <c r="AO17" s="28" t="s">
-        <v>387</v>
+        <v>409</v>
       </c>
       <c r="AP17" s="30"/>
       <c r="AQ17" s="2" t="n">
@@ -31838,7 +32107,7 @@
         <v>16</v>
       </c>
       <c r="AT17" s="28" t="s">
-        <v>388</v>
+        <v>410</v>
       </c>
       <c r="AU17" s="30"/>
     </row>
@@ -31847,7 +32116,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>49</v>
@@ -31856,7 +32125,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>390</v>
+        <v>412</v>
       </c>
       <c r="G18" s="30" t="s">
         <v>49</v>
@@ -31869,7 +32138,7 @@
         <v>17</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>391</v>
+        <v>413</v>
       </c>
       <c r="L18" s="30" t="s">
         <v>49</v>
@@ -31883,7 +32152,7 @@
         <v>17</v>
       </c>
       <c r="P18" s="28" t="s">
-        <v>392</v>
+        <v>414</v>
       </c>
       <c r="Q18" s="30" t="s">
         <v>49</v>
@@ -31897,7 +32166,7 @@
         <v>17</v>
       </c>
       <c r="U18" s="28" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
       <c r="V18" s="30" t="s">
         <v>49</v>
@@ -31910,7 +32179,7 @@
         <v>17</v>
       </c>
       <c r="Z18" s="28" t="s">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="AA18" s="30" t="s">
         <v>49</v>
@@ -31924,7 +32193,7 @@
         <v>17</v>
       </c>
       <c r="AE18" s="28" t="s">
-        <v>395</v>
+        <v>417</v>
       </c>
       <c r="AF18" s="30" t="s">
         <v>49</v>
@@ -31939,7 +32208,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>67</v>
@@ -31948,7 +32217,7 @@
         <v>18</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>67</v>
@@ -31961,7 +32230,7 @@
         <v>18</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>398</v>
+        <v>420</v>
       </c>
       <c r="L19" s="30" t="s">
         <v>67</v>
@@ -31975,7 +32244,7 @@
         <v>18</v>
       </c>
       <c r="P19" s="28" t="s">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="Q19" s="30" t="s">
         <v>67</v>
@@ -31989,7 +32258,7 @@
         <v>18</v>
       </c>
       <c r="U19" s="28" t="s">
-        <v>400</v>
+        <v>422</v>
       </c>
       <c r="V19" s="30" t="s">
         <v>67</v>
@@ -32002,7 +32271,7 @@
         <v>18</v>
       </c>
       <c r="Z19" s="28" t="s">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="AA19" s="30" t="s">
         <v>67</v>
@@ -32016,7 +32285,7 @@
         <v>18</v>
       </c>
       <c r="AE19" s="28" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="AF19" s="30" t="s">
         <v>67</v>
@@ -32031,7 +32300,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>80</v>
@@ -32040,7 +32309,7 @@
         <v>19</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>404</v>
+        <v>426</v>
       </c>
       <c r="G20" s="30" t="s">
         <v>80</v>
@@ -32053,7 +32322,7 @@
         <v>19</v>
       </c>
       <c r="K20" s="28" t="s">
-        <v>405</v>
+        <v>427</v>
       </c>
       <c r="L20" s="30" t="s">
         <v>80</v>
@@ -32067,7 +32336,7 @@
         <v>19</v>
       </c>
       <c r="P20" s="28" t="s">
-        <v>406</v>
+        <v>428</v>
       </c>
       <c r="Q20" s="30" t="s">
         <v>80</v>
@@ -32081,7 +32350,7 @@
         <v>19</v>
       </c>
       <c r="U20" s="28" t="s">
-        <v>407</v>
+        <v>429</v>
       </c>
       <c r="V20" s="30" t="s">
         <v>80</v>
@@ -32094,7 +32363,7 @@
         <v>19</v>
       </c>
       <c r="Z20" s="28" t="s">
-        <v>408</v>
+        <v>430</v>
       </c>
       <c r="AA20" s="30" t="s">
         <v>80</v>
@@ -32108,7 +32377,7 @@
         <v>19</v>
       </c>
       <c r="AE20" s="28" t="s">
-        <v>409</v>
+        <v>431</v>
       </c>
       <c r="AF20" s="30" t="s">
         <v>80</v>
@@ -32123,7 +32392,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>410</v>
+        <v>432</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>93</v>
@@ -32132,7 +32401,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>411</v>
+        <v>433</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>93</v>
@@ -32145,7 +32414,7 @@
         <v>20</v>
       </c>
       <c r="K21" s="28" t="s">
-        <v>412</v>
+        <v>434</v>
       </c>
       <c r="L21" s="30" t="s">
         <v>93</v>
@@ -32159,7 +32428,7 @@
         <v>20</v>
       </c>
       <c r="P21" s="28" t="s">
-        <v>413</v>
+        <v>435</v>
       </c>
       <c r="Q21" s="30" t="s">
         <v>93</v>
@@ -32173,7 +32442,7 @@
         <v>20</v>
       </c>
       <c r="U21" s="28" t="s">
-        <v>414</v>
+        <v>436</v>
       </c>
       <c r="V21" s="30" t="s">
         <v>93</v>
@@ -32186,7 +32455,7 @@
         <v>20</v>
       </c>
       <c r="Z21" s="28" t="s">
-        <v>415</v>
+        <v>437</v>
       </c>
       <c r="AA21" s="30" t="s">
         <v>93</v>
@@ -32200,7 +32469,7 @@
         <v>20</v>
       </c>
       <c r="AE21" s="28" t="s">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="AF21" s="30" t="s">
         <v>93</v>
@@ -32215,7 +32484,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>417</v>
+        <v>439</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>106</v>
@@ -32224,7 +32493,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>418</v>
+        <v>440</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>106</v>
@@ -32237,7 +32506,7 @@
         <v>21</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>419</v>
+        <v>441</v>
       </c>
       <c r="L22" s="30" t="s">
         <v>106</v>
@@ -32251,7 +32520,7 @@
         <v>21</v>
       </c>
       <c r="P22" s="28" t="s">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="Q22" s="30" t="s">
         <v>106</v>
@@ -32265,7 +32534,7 @@
         <v>21</v>
       </c>
       <c r="U22" s="28" t="s">
-        <v>421</v>
+        <v>443</v>
       </c>
       <c r="V22" s="30" t="s">
         <v>106</v>
@@ -32278,7 +32547,7 @@
         <v>21</v>
       </c>
       <c r="Z22" s="28" t="s">
-        <v>422</v>
+        <v>444</v>
       </c>
       <c r="AA22" s="30" t="s">
         <v>106</v>
@@ -32292,7 +32561,7 @@
         <v>21</v>
       </c>
       <c r="AE22" s="28" t="s">
-        <v>423</v>
+        <v>445</v>
       </c>
       <c r="AF22" s="30" t="s">
         <v>106</v>
@@ -32307,7 +32576,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>119</v>
@@ -32316,7 +32585,7 @@
         <v>22</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>425</v>
+        <v>447</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>119</v>
@@ -32329,7 +32598,7 @@
         <v>22</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>426</v>
+        <v>448</v>
       </c>
       <c r="L23" s="30" t="s">
         <v>119</v>
@@ -32343,7 +32612,7 @@
         <v>22</v>
       </c>
       <c r="P23" s="28" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="Q23" s="30" t="s">
         <v>119</v>
@@ -32357,7 +32626,7 @@
         <v>22</v>
       </c>
       <c r="U23" s="28" t="s">
-        <v>428</v>
+        <v>450</v>
       </c>
       <c r="V23" s="30" t="s">
         <v>119</v>
@@ -32370,7 +32639,7 @@
         <v>22</v>
       </c>
       <c r="Z23" s="28" t="s">
-        <v>429</v>
+        <v>451</v>
       </c>
       <c r="AA23" s="30" t="s">
         <v>119</v>
@@ -32384,7 +32653,7 @@
         <v>22</v>
       </c>
       <c r="AE23" s="28" t="s">
-        <v>430</v>
+        <v>452</v>
       </c>
       <c r="AF23" s="30" t="s">
         <v>119</v>
@@ -32399,7 +32668,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>431</v>
+        <v>453</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>53</v>
@@ -32408,7 +32677,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>432</v>
+        <v>454</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>133</v>
@@ -32421,7 +32690,7 @@
         <v>23</v>
       </c>
       <c r="K24" s="28" t="s">
-        <v>433</v>
+        <v>455</v>
       </c>
       <c r="L24" s="30" t="s">
         <v>133</v>
@@ -32435,7 +32704,7 @@
         <v>23</v>
       </c>
       <c r="P24" s="28" t="s">
-        <v>434</v>
+        <v>456</v>
       </c>
       <c r="Q24" s="30" t="s">
         <v>133</v>
@@ -32449,7 +32718,7 @@
         <v>23</v>
       </c>
       <c r="U24" s="28" t="s">
-        <v>435</v>
+        <v>457</v>
       </c>
       <c r="V24" s="30" t="s">
         <v>133</v>
@@ -32462,7 +32731,7 @@
         <v>23</v>
       </c>
       <c r="Z24" s="28" t="s">
-        <v>436</v>
+        <v>458</v>
       </c>
       <c r="AA24" s="30" t="s">
         <v>133</v>
@@ -32476,7 +32745,7 @@
         <v>23</v>
       </c>
       <c r="AE24" s="28" t="s">
-        <v>437</v>
+        <v>459</v>
       </c>
       <c r="AF24" s="30" t="s">
         <v>133</v>
@@ -32491,14 +32760,14 @@
         <v>24</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>438</v>
+        <v>460</v>
       </c>
       <c r="C25" s="30"/>
       <c r="E25" s="26" t="n">
         <v>24</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>439</v>
+        <v>461</v>
       </c>
       <c r="G25" s="30" t="s">
         <v>146</v>
@@ -32511,7 +32780,7 @@
         <v>24</v>
       </c>
       <c r="K25" s="28" t="s">
-        <v>440</v>
+        <v>462</v>
       </c>
       <c r="L25" s="30" t="s">
         <v>146</v>
@@ -32525,7 +32794,7 @@
         <v>24</v>
       </c>
       <c r="P25" s="28" t="s">
-        <v>441</v>
+        <v>463</v>
       </c>
       <c r="Q25" s="30" t="s">
         <v>146</v>
@@ -32539,7 +32808,7 @@
         <v>24</v>
       </c>
       <c r="U25" s="28" t="s">
-        <v>442</v>
+        <v>464</v>
       </c>
       <c r="V25" s="30" t="s">
         <v>146</v>
@@ -32552,7 +32821,7 @@
         <v>24</v>
       </c>
       <c r="Z25" s="28" t="s">
-        <v>443</v>
+        <v>465</v>
       </c>
       <c r="AA25" s="30" t="s">
         <v>146</v>
@@ -32566,7 +32835,7 @@
         <v>24</v>
       </c>
       <c r="AE25" s="28" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
       <c r="AF25" s="30" t="s">
         <v>146</v>
@@ -32581,7 +32850,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>445</v>
+        <v>467</v>
       </c>
       <c r="G26" s="30" t="s">
         <v>49</v>
@@ -32594,7 +32863,7 @@
         <v>25</v>
       </c>
       <c r="K26" s="28" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="L26" s="30" t="s">
         <v>49</v>
@@ -32608,7 +32877,7 @@
         <v>25</v>
       </c>
       <c r="P26" s="28" t="s">
-        <v>447</v>
+        <v>469</v>
       </c>
       <c r="Q26" s="30" t="s">
         <v>49</v>
@@ -32622,7 +32891,7 @@
         <v>25</v>
       </c>
       <c r="U26" s="28" t="s">
-        <v>448</v>
+        <v>470</v>
       </c>
       <c r="V26" s="30" t="s">
         <v>49</v>
@@ -32635,7 +32904,7 @@
         <v>25</v>
       </c>
       <c r="Z26" s="28" t="s">
-        <v>449</v>
+        <v>471</v>
       </c>
       <c r="AA26" s="30" t="s">
         <v>49</v>
@@ -32649,7 +32918,7 @@
         <v>25</v>
       </c>
       <c r="AE26" s="28" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
       <c r="AF26" s="30" t="s">
         <v>49</v>
@@ -32664,7 +32933,7 @@
         <v>26</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>451</v>
+        <v>473</v>
       </c>
       <c r="G27" s="30" t="s">
         <v>67</v>
@@ -32677,7 +32946,7 @@
         <v>26</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>452</v>
+        <v>474</v>
       </c>
       <c r="L27" s="30" t="s">
         <v>67</v>
@@ -32691,7 +32960,7 @@
         <v>26</v>
       </c>
       <c r="P27" s="28" t="s">
-        <v>453</v>
+        <v>475</v>
       </c>
       <c r="Q27" s="30" t="s">
         <v>67</v>
@@ -32705,7 +32974,7 @@
         <v>26</v>
       </c>
       <c r="U27" s="28" t="s">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="V27" s="30" t="s">
         <v>67</v>
@@ -32718,7 +32987,7 @@
         <v>26</v>
       </c>
       <c r="Z27" s="28" t="s">
-        <v>455</v>
+        <v>477</v>
       </c>
       <c r="AA27" s="30" t="s">
         <v>67</v>
@@ -32732,7 +33001,7 @@
         <v>26</v>
       </c>
       <c r="AE27" s="28" t="s">
-        <v>456</v>
+        <v>478</v>
       </c>
       <c r="AF27" s="30" t="s">
         <v>67</v>
@@ -32747,7 +33016,7 @@
         <v>27</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>457</v>
+        <v>479</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>80</v>
@@ -32760,7 +33029,7 @@
         <v>27</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>458</v>
+        <v>480</v>
       </c>
       <c r="L28" s="30" t="s">
         <v>80</v>
@@ -32774,7 +33043,7 @@
         <v>27</v>
       </c>
       <c r="P28" s="28" t="s">
-        <v>459</v>
+        <v>481</v>
       </c>
       <c r="Q28" s="30" t="s">
         <v>80</v>
@@ -32788,7 +33057,7 @@
         <v>27</v>
       </c>
       <c r="U28" s="28" t="s">
-        <v>460</v>
+        <v>482</v>
       </c>
       <c r="V28" s="30" t="s">
         <v>80</v>
@@ -32801,7 +33070,7 @@
         <v>27</v>
       </c>
       <c r="Z28" s="28" t="s">
-        <v>461</v>
+        <v>483</v>
       </c>
       <c r="AA28" s="30" t="s">
         <v>80</v>
@@ -32815,7 +33084,7 @@
         <v>27</v>
       </c>
       <c r="AE28" s="28" t="s">
-        <v>462</v>
+        <v>484</v>
       </c>
       <c r="AF28" s="30" t="s">
         <v>80</v>
@@ -32830,7 +33099,7 @@
         <v>28</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>463</v>
+        <v>485</v>
       </c>
       <c r="G29" s="30" t="s">
         <v>93</v>
@@ -32843,7 +33112,7 @@
         <v>28</v>
       </c>
       <c r="K29" s="28" t="s">
-        <v>464</v>
+        <v>486</v>
       </c>
       <c r="L29" s="30" t="s">
         <v>93</v>
@@ -32857,7 +33126,7 @@
         <v>28</v>
       </c>
       <c r="P29" s="28" t="s">
-        <v>465</v>
+        <v>487</v>
       </c>
       <c r="Q29" s="30" t="s">
         <v>93</v>
@@ -32871,7 +33140,7 @@
         <v>28</v>
       </c>
       <c r="U29" s="28" t="s">
-        <v>466</v>
+        <v>488</v>
       </c>
       <c r="V29" s="30" t="s">
         <v>93</v>
@@ -32884,7 +33153,7 @@
         <v>28</v>
       </c>
       <c r="Z29" s="28" t="s">
-        <v>467</v>
+        <v>489</v>
       </c>
       <c r="AA29" s="30" t="s">
         <v>93</v>
@@ -32898,7 +33167,7 @@
         <v>28</v>
       </c>
       <c r="AE29" s="28" t="s">
-        <v>468</v>
+        <v>490</v>
       </c>
       <c r="AF29" s="30" t="s">
         <v>93</v>
@@ -32913,7 +33182,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>469</v>
+        <v>491</v>
       </c>
       <c r="G30" s="30" t="s">
         <v>106</v>
@@ -32926,7 +33195,7 @@
         <v>29</v>
       </c>
       <c r="K30" s="28" t="s">
-        <v>470</v>
+        <v>492</v>
       </c>
       <c r="L30" s="30" t="s">
         <v>106</v>
@@ -32940,7 +33209,7 @@
         <v>29</v>
       </c>
       <c r="P30" s="28" t="s">
-        <v>471</v>
+        <v>493</v>
       </c>
       <c r="Q30" s="30" t="s">
         <v>106</v>
@@ -32954,7 +33223,7 @@
         <v>29</v>
       </c>
       <c r="U30" s="28" t="s">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="V30" s="30" t="s">
         <v>106</v>
@@ -32967,7 +33236,7 @@
         <v>29</v>
       </c>
       <c r="Z30" s="28" t="s">
-        <v>473</v>
+        <v>495</v>
       </c>
       <c r="AA30" s="30" t="s">
         <v>106</v>
@@ -32981,7 +33250,7 @@
         <v>29</v>
       </c>
       <c r="AE30" s="28" t="s">
-        <v>474</v>
+        <v>496</v>
       </c>
       <c r="AF30" s="30" t="s">
         <v>106</v>
@@ -32996,7 +33265,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>475</v>
+        <v>497</v>
       </c>
       <c r="G31" s="30" t="s">
         <v>119</v>
@@ -33009,7 +33278,7 @@
         <v>30</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>476</v>
+        <v>498</v>
       </c>
       <c r="L31" s="30" t="s">
         <v>53</v>
@@ -33023,7 +33292,7 @@
         <v>30</v>
       </c>
       <c r="P31" s="28" t="s">
-        <v>477</v>
+        <v>499</v>
       </c>
       <c r="Q31" s="30" t="s">
         <v>119</v>
@@ -33037,7 +33306,7 @@
         <v>30</v>
       </c>
       <c r="U31" s="28" t="s">
-        <v>478</v>
+        <v>500</v>
       </c>
       <c r="V31" s="30" t="s">
         <v>53</v>
@@ -33050,7 +33319,7 @@
         <v>30</v>
       </c>
       <c r="Z31" s="28" t="s">
-        <v>479</v>
+        <v>501</v>
       </c>
       <c r="AA31" s="30" t="s">
         <v>119</v>
@@ -33064,7 +33333,7 @@
         <v>30</v>
       </c>
       <c r="AE31" s="28" t="s">
-        <v>480</v>
+        <v>502</v>
       </c>
       <c r="AF31" s="30" t="s">
         <v>53</v>
@@ -33079,7 +33348,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>481</v>
+        <v>503</v>
       </c>
       <c r="G32" s="30" t="s">
         <v>133</v>
@@ -33092,7 +33361,7 @@
         <v>31</v>
       </c>
       <c r="K32" s="28" t="s">
-        <v>482</v>
+        <v>504</v>
       </c>
       <c r="L32" s="30"/>
       <c r="M32" s="2" t="n">
@@ -33104,7 +33373,7 @@
         <v>31</v>
       </c>
       <c r="P32" s="28" t="s">
-        <v>483</v>
+        <v>505</v>
       </c>
       <c r="Q32" s="30" t="s">
         <v>133</v>
@@ -33118,7 +33387,7 @@
         <v>31</v>
       </c>
       <c r="U32" s="28" t="s">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="V32" s="30"/>
       <c r="W32" s="2" t="n">
@@ -33129,7 +33398,7 @@
         <v>31</v>
       </c>
       <c r="Z32" s="28" t="s">
-        <v>485</v>
+        <v>507</v>
       </c>
       <c r="AA32" s="30" t="s">
         <v>133</v>
@@ -33143,7 +33412,7 @@
         <v>31</v>
       </c>
       <c r="AE32" s="28" t="s">
-        <v>486</v>
+        <v>508</v>
       </c>
       <c r="AF32" s="30"/>
       <c r="AG32" s="2" t="n">
@@ -33156,7 +33425,7 @@
         <v>32</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>487</v>
+        <v>509</v>
       </c>
       <c r="G33" s="30" t="s">
         <v>146</v>
@@ -33170,7 +33439,7 @@
         <v>32</v>
       </c>
       <c r="P33" s="28" t="s">
-        <v>488</v>
+        <v>510</v>
       </c>
       <c r="Q33" s="30" t="s">
         <v>146</v>
@@ -33185,7 +33454,7 @@
         <v>32</v>
       </c>
       <c r="Z33" s="28" t="s">
-        <v>489</v>
+        <v>511</v>
       </c>
       <c r="AA33" s="30" t="s">
         <v>146</v>
@@ -33202,7 +33471,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>490</v>
+        <v>512</v>
       </c>
       <c r="G34" s="30" t="s">
         <v>49</v>
@@ -33215,7 +33484,7 @@
         <v>33</v>
       </c>
       <c r="P34" s="28" t="s">
-        <v>491</v>
+        <v>513</v>
       </c>
       <c r="Q34" s="30" t="s">
         <v>49</v>
@@ -33229,7 +33498,7 @@
         <v>33</v>
       </c>
       <c r="Z34" s="28" t="s">
-        <v>492</v>
+        <v>514</v>
       </c>
       <c r="AA34" s="30" t="s">
         <v>49</v>
@@ -33246,7 +33515,7 @@
         <v>34</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>493</v>
+        <v>515</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>67</v>
@@ -33259,7 +33528,7 @@
         <v>34</v>
       </c>
       <c r="P35" s="28" t="s">
-        <v>494</v>
+        <v>516</v>
       </c>
       <c r="Q35" s="30" t="s">
         <v>67</v>
@@ -33273,7 +33542,7 @@
         <v>34</v>
       </c>
       <c r="Z35" s="28" t="s">
-        <v>495</v>
+        <v>517</v>
       </c>
       <c r="AA35" s="30" t="s">
         <v>67</v>
@@ -33290,7 +33559,7 @@
         <v>35</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>496</v>
+        <v>518</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>80</v>
@@ -33303,7 +33572,7 @@
         <v>35</v>
       </c>
       <c r="P36" s="28" t="s">
-        <v>497</v>
+        <v>519</v>
       </c>
       <c r="Q36" s="30" t="s">
         <v>80</v>
@@ -33317,7 +33586,7 @@
         <v>35</v>
       </c>
       <c r="Z36" s="28" t="s">
-        <v>498</v>
+        <v>520</v>
       </c>
       <c r="AA36" s="30" t="s">
         <v>80</v>
@@ -33333,7 +33602,7 @@
         <v>36</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>499</v>
+        <v>521</v>
       </c>
       <c r="G37" s="30" t="s">
         <v>93</v>
@@ -33346,7 +33615,7 @@
         <v>36</v>
       </c>
       <c r="P37" s="28" t="s">
-        <v>500</v>
+        <v>522</v>
       </c>
       <c r="Q37" s="30" t="s">
         <v>93</v>
@@ -33360,7 +33629,7 @@
         <v>36</v>
       </c>
       <c r="Z37" s="28" t="s">
-        <v>501</v>
+        <v>523</v>
       </c>
       <c r="AA37" s="30" t="s">
         <v>93</v>
@@ -33376,7 +33645,7 @@
         <v>37</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>502</v>
+        <v>524</v>
       </c>
       <c r="G38" s="30" t="s">
         <v>106</v>
@@ -33389,7 +33658,7 @@
         <v>37</v>
       </c>
       <c r="P38" s="28" t="s">
-        <v>503</v>
+        <v>525</v>
       </c>
       <c r="Q38" s="30" t="s">
         <v>106</v>
@@ -33403,7 +33672,7 @@
         <v>37</v>
       </c>
       <c r="Z38" s="28" t="s">
-        <v>504</v>
+        <v>526</v>
       </c>
       <c r="AA38" s="30" t="s">
         <v>106</v>
@@ -33419,7 +33688,7 @@
         <v>38</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>505</v>
+        <v>527</v>
       </c>
       <c r="G39" s="30" t="s">
         <v>119</v>
@@ -33432,7 +33701,7 @@
         <v>38</v>
       </c>
       <c r="P39" s="28" t="s">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="Q39" s="30" t="s">
         <v>119</v>
@@ -33446,7 +33715,7 @@
         <v>38</v>
       </c>
       <c r="Z39" s="28" t="s">
-        <v>507</v>
+        <v>529</v>
       </c>
       <c r="AA39" s="30" t="s">
         <v>119</v>
@@ -33462,7 +33731,7 @@
         <v>39</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>508</v>
+        <v>530</v>
       </c>
       <c r="G40" s="30" t="s">
         <v>133</v>
@@ -33475,7 +33744,7 @@
         <v>39</v>
       </c>
       <c r="P40" s="28" t="s">
-        <v>509</v>
+        <v>531</v>
       </c>
       <c r="Q40" s="30" t="s">
         <v>133</v>
@@ -33489,7 +33758,7 @@
         <v>39</v>
       </c>
       <c r="Z40" s="28" t="s">
-        <v>510</v>
+        <v>532</v>
       </c>
       <c r="AA40" s="30" t="s">
         <v>133</v>
@@ -33505,7 +33774,7 @@
         <v>40</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>511</v>
+        <v>533</v>
       </c>
       <c r="G41" s="30" t="s">
         <v>146</v>
@@ -33518,7 +33787,7 @@
         <v>40</v>
       </c>
       <c r="P41" s="28" t="s">
-        <v>512</v>
+        <v>534</v>
       </c>
       <c r="Q41" s="30" t="s">
         <v>146</v>
@@ -33532,7 +33801,7 @@
         <v>40</v>
       </c>
       <c r="Z41" s="28" t="s">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="AA41" s="30" t="s">
         <v>146</v>
@@ -33548,7 +33817,7 @@
         <v>41</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>514</v>
+        <v>536</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>49</v>
@@ -33561,7 +33830,7 @@
         <v>41</v>
       </c>
       <c r="P42" s="28" t="s">
-        <v>515</v>
+        <v>537</v>
       </c>
       <c r="Q42" s="30" t="s">
         <v>49</v>
@@ -33575,7 +33844,7 @@
         <v>41</v>
       </c>
       <c r="Z42" s="28" t="s">
-        <v>516</v>
+        <v>538</v>
       </c>
       <c r="AA42" s="30" t="s">
         <v>49</v>
@@ -33591,7 +33860,7 @@
         <v>42</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>517</v>
+        <v>539</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>67</v>
@@ -33604,7 +33873,7 @@
         <v>42</v>
       </c>
       <c r="P43" s="28" t="s">
-        <v>518</v>
+        <v>540</v>
       </c>
       <c r="Q43" s="30" t="s">
         <v>67</v>
@@ -33618,7 +33887,7 @@
         <v>42</v>
       </c>
       <c r="Z43" s="28" t="s">
-        <v>519</v>
+        <v>541</v>
       </c>
       <c r="AA43" s="30" t="s">
         <v>67</v>
@@ -33634,7 +33903,7 @@
         <v>43</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>520</v>
+        <v>542</v>
       </c>
       <c r="G44" s="30" t="s">
         <v>80</v>
@@ -33647,7 +33916,7 @@
         <v>43</v>
       </c>
       <c r="P44" s="28" t="s">
-        <v>521</v>
+        <v>543</v>
       </c>
       <c r="Q44" s="30" t="s">
         <v>80</v>
@@ -33661,7 +33930,7 @@
         <v>43</v>
       </c>
       <c r="Z44" s="28" t="s">
-        <v>522</v>
+        <v>544</v>
       </c>
       <c r="AA44" s="30" t="s">
         <v>80</v>
@@ -33677,7 +33946,7 @@
         <v>44</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>523</v>
+        <v>545</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>93</v>
@@ -33690,7 +33959,7 @@
         <v>44</v>
       </c>
       <c r="P45" s="28" t="s">
-        <v>524</v>
+        <v>546</v>
       </c>
       <c r="Q45" s="30" t="s">
         <v>93</v>
@@ -33704,7 +33973,7 @@
         <v>44</v>
       </c>
       <c r="Z45" s="28" t="s">
-        <v>525</v>
+        <v>547</v>
       </c>
       <c r="AA45" s="30" t="s">
         <v>93</v>
@@ -33720,7 +33989,7 @@
         <v>45</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>526</v>
+        <v>548</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>106</v>
@@ -33733,7 +34002,7 @@
         <v>45</v>
       </c>
       <c r="P46" s="28" t="s">
-        <v>527</v>
+        <v>549</v>
       </c>
       <c r="Q46" s="30" t="s">
         <v>106</v>
@@ -33747,7 +34016,7 @@
         <v>45</v>
       </c>
       <c r="Z46" s="28" t="s">
-        <v>528</v>
+        <v>550</v>
       </c>
       <c r="AA46" s="30" t="s">
         <v>106</v>
@@ -33763,7 +34032,7 @@
         <v>46</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>529</v>
+        <v>551</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>119</v>
@@ -33776,7 +34045,7 @@
         <v>46</v>
       </c>
       <c r="P47" s="28" t="s">
-        <v>530</v>
+        <v>552</v>
       </c>
       <c r="Q47" s="30" t="s">
         <v>119</v>
@@ -33790,7 +34059,7 @@
         <v>46</v>
       </c>
       <c r="Z47" s="28" t="s">
-        <v>531</v>
+        <v>553</v>
       </c>
       <c r="AA47" s="30" t="s">
         <v>119</v>
@@ -33806,7 +34075,7 @@
         <v>47</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>532</v>
+        <v>554</v>
       </c>
       <c r="G48" s="30" t="s">
         <v>133</v>
@@ -33819,7 +34088,7 @@
         <v>47</v>
       </c>
       <c r="P48" s="28" t="s">
-        <v>533</v>
+        <v>555</v>
       </c>
       <c r="Q48" s="30" t="s">
         <v>133</v>
@@ -33833,7 +34102,7 @@
         <v>47</v>
       </c>
       <c r="Z48" s="28" t="s">
-        <v>534</v>
+        <v>556</v>
       </c>
       <c r="AA48" s="30" t="s">
         <v>133</v>
@@ -33849,7 +34118,7 @@
         <v>48</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>535</v>
+        <v>557</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>146</v>
@@ -33862,7 +34131,7 @@
         <v>48</v>
       </c>
       <c r="P49" s="28" t="s">
-        <v>536</v>
+        <v>558</v>
       </c>
       <c r="Q49" s="30" t="s">
         <v>146</v>
@@ -33876,7 +34145,7 @@
         <v>48</v>
       </c>
       <c r="Z49" s="28" t="s">
-        <v>537</v>
+        <v>559</v>
       </c>
       <c r="AA49" s="30" t="s">
         <v>146</v>
@@ -33892,7 +34161,7 @@
         <v>49</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>538</v>
+        <v>560</v>
       </c>
       <c r="G50" s="30" t="s">
         <v>49</v>
@@ -33905,7 +34174,7 @@
         <v>49</v>
       </c>
       <c r="P50" s="28" t="s">
-        <v>539</v>
+        <v>561</v>
       </c>
       <c r="Q50" s="30" t="s">
         <v>49</v>
@@ -33919,7 +34188,7 @@
         <v>49</v>
       </c>
       <c r="Z50" s="28" t="s">
-        <v>540</v>
+        <v>562</v>
       </c>
       <c r="AA50" s="30" t="s">
         <v>49</v>
@@ -33935,7 +34204,7 @@
         <v>50</v>
       </c>
       <c r="F51" s="28" t="s">
-        <v>541</v>
+        <v>563</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>67</v>
@@ -33948,7 +34217,7 @@
         <v>50</v>
       </c>
       <c r="P51" s="28" t="s">
-        <v>542</v>
+        <v>564</v>
       </c>
       <c r="Q51" s="30" t="s">
         <v>67</v>
@@ -33962,7 +34231,7 @@
         <v>50</v>
       </c>
       <c r="Z51" s="28" t="s">
-        <v>543</v>
+        <v>565</v>
       </c>
       <c r="AA51" s="30" t="s">
         <v>67</v>
@@ -33978,7 +34247,7 @@
         <v>51</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>544</v>
+        <v>566</v>
       </c>
       <c r="G52" s="30" t="s">
         <v>80</v>
@@ -33991,7 +34260,7 @@
         <v>51</v>
       </c>
       <c r="P52" s="28" t="s">
-        <v>545</v>
+        <v>567</v>
       </c>
       <c r="Q52" s="30" t="s">
         <v>80</v>
@@ -34005,7 +34274,7 @@
         <v>51</v>
       </c>
       <c r="Z52" s="28" t="s">
-        <v>546</v>
+        <v>568</v>
       </c>
       <c r="AA52" s="30" t="s">
         <v>80</v>
@@ -34021,7 +34290,7 @@
         <v>52</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>93</v>
@@ -34034,7 +34303,7 @@
         <v>52</v>
       </c>
       <c r="P53" s="28" t="s">
-        <v>548</v>
+        <v>570</v>
       </c>
       <c r="Q53" s="30" t="s">
         <v>93</v>
@@ -34048,7 +34317,7 @@
         <v>52</v>
       </c>
       <c r="Z53" s="28" t="s">
-        <v>549</v>
+        <v>571</v>
       </c>
       <c r="AA53" s="30" t="s">
         <v>93</v>
@@ -34064,7 +34333,7 @@
         <v>53</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>550</v>
+        <v>572</v>
       </c>
       <c r="G54" s="30" t="s">
         <v>106</v>
@@ -34077,7 +34346,7 @@
         <v>53</v>
       </c>
       <c r="P54" s="28" t="s">
-        <v>551</v>
+        <v>573</v>
       </c>
       <c r="Q54" s="30" t="s">
         <v>106</v>
@@ -34091,7 +34360,7 @@
         <v>53</v>
       </c>
       <c r="Z54" s="28" t="s">
-        <v>552</v>
+        <v>574</v>
       </c>
       <c r="AA54" s="30" t="s">
         <v>106</v>
@@ -34107,7 +34376,7 @@
         <v>54</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>553</v>
+        <v>575</v>
       </c>
       <c r="G55" s="30" t="s">
         <v>119</v>
@@ -34120,7 +34389,7 @@
         <v>54</v>
       </c>
       <c r="P55" s="28" t="s">
-        <v>554</v>
+        <v>576</v>
       </c>
       <c r="Q55" s="30" t="s">
         <v>119</v>
@@ -34134,7 +34403,7 @@
         <v>54</v>
       </c>
       <c r="Z55" s="28" t="s">
-        <v>555</v>
+        <v>577</v>
       </c>
       <c r="AA55" s="30" t="s">
         <v>119</v>
@@ -34150,7 +34419,7 @@
         <v>55</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>556</v>
+        <v>578</v>
       </c>
       <c r="G56" s="30" t="s">
         <v>133</v>
@@ -34163,7 +34432,7 @@
         <v>55</v>
       </c>
       <c r="P56" s="28" t="s">
-        <v>557</v>
+        <v>579</v>
       </c>
       <c r="Q56" s="30" t="s">
         <v>133</v>
@@ -34177,7 +34446,7 @@
         <v>55</v>
       </c>
       <c r="Z56" s="28" t="s">
-        <v>558</v>
+        <v>580</v>
       </c>
       <c r="AA56" s="30" t="s">
         <v>133</v>
@@ -34193,7 +34462,7 @@
         <v>56</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="G57" s="30" t="s">
         <v>146</v>
@@ -34206,7 +34475,7 @@
         <v>56</v>
       </c>
       <c r="P57" s="28" t="s">
-        <v>560</v>
+        <v>582</v>
       </c>
       <c r="Q57" s="30" t="s">
         <v>146</v>
@@ -34220,7 +34489,7 @@
         <v>56</v>
       </c>
       <c r="Z57" s="28" t="s">
-        <v>561</v>
+        <v>583</v>
       </c>
       <c r="AA57" s="30" t="s">
         <v>146</v>
@@ -34236,7 +34505,7 @@
         <v>57</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>562</v>
+        <v>584</v>
       </c>
       <c r="G58" s="30" t="s">
         <v>49</v>
@@ -34249,7 +34518,7 @@
         <v>57</v>
       </c>
       <c r="P58" s="28" t="s">
-        <v>563</v>
+        <v>585</v>
       </c>
       <c r="Q58" s="30" t="s">
         <v>49</v>
@@ -34263,7 +34532,7 @@
         <v>57</v>
       </c>
       <c r="Z58" s="28" t="s">
-        <v>564</v>
+        <v>586</v>
       </c>
       <c r="AA58" s="30" t="s">
         <v>49</v>
@@ -34279,7 +34548,7 @@
         <v>58</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>565</v>
+        <v>587</v>
       </c>
       <c r="G59" s="30" t="s">
         <v>67</v>
@@ -34292,7 +34561,7 @@
         <v>58</v>
       </c>
       <c r="P59" s="28" t="s">
-        <v>566</v>
+        <v>588</v>
       </c>
       <c r="Q59" s="30" t="s">
         <v>67</v>
@@ -34306,7 +34575,7 @@
         <v>58</v>
       </c>
       <c r="Z59" s="28" t="s">
-        <v>567</v>
+        <v>589</v>
       </c>
       <c r="AA59" s="30" t="s">
         <v>67</v>
@@ -34322,7 +34591,7 @@
         <v>59</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="G60" s="30" t="s">
         <v>80</v>
@@ -34335,7 +34604,7 @@
         <v>59</v>
       </c>
       <c r="P60" s="28" t="s">
-        <v>569</v>
+        <v>591</v>
       </c>
       <c r="Q60" s="30" t="s">
         <v>80</v>
@@ -34349,7 +34618,7 @@
         <v>59</v>
       </c>
       <c r="Z60" s="28" t="s">
-        <v>570</v>
+        <v>592</v>
       </c>
       <c r="AA60" s="30" t="s">
         <v>80</v>
@@ -34365,7 +34634,7 @@
         <v>60</v>
       </c>
       <c r="F61" s="28" t="s">
-        <v>571</v>
+        <v>593</v>
       </c>
       <c r="G61" s="30" t="s">
         <v>93</v>
@@ -34378,7 +34647,7 @@
         <v>60</v>
       </c>
       <c r="P61" s="28" t="s">
-        <v>572</v>
+        <v>594</v>
       </c>
       <c r="Q61" s="30" t="s">
         <v>93</v>
@@ -34392,7 +34661,7 @@
         <v>60</v>
       </c>
       <c r="Z61" s="28" t="s">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="AA61" s="30" t="s">
         <v>93</v>
@@ -34408,7 +34677,7 @@
         <v>61</v>
       </c>
       <c r="F62" s="28" t="s">
-        <v>574</v>
+        <v>596</v>
       </c>
       <c r="G62" s="30" t="s">
         <v>53</v>
@@ -34421,7 +34690,7 @@
         <v>61</v>
       </c>
       <c r="P62" s="28" t="s">
-        <v>575</v>
+        <v>597</v>
       </c>
       <c r="Q62" s="30" t="s">
         <v>53</v>
@@ -34435,7 +34704,7 @@
         <v>61</v>
       </c>
       <c r="Z62" s="28" t="s">
-        <v>576</v>
+        <v>598</v>
       </c>
       <c r="AA62" s="30" t="s">
         <v>53</v>
@@ -34451,7 +34720,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="28" t="s">
-        <v>577</v>
+        <v>599</v>
       </c>
       <c r="G63" s="30"/>
       <c r="H63" s="2" t="n">
@@ -34462,7 +34731,7 @@
         <v>62</v>
       </c>
       <c r="P63" s="28" t="s">
-        <v>578</v>
+        <v>600</v>
       </c>
       <c r="Q63" s="30"/>
       <c r="R63" s="29" t="n">
@@ -34474,7 +34743,7 @@
         <v>62</v>
       </c>
       <c r="Z63" s="28" t="s">
-        <v>579</v>
+        <v>601</v>
       </c>
       <c r="AA63" s="30"/>
       <c r="AB63" s="2" t="n">
@@ -34556,7 +34825,7 @@
       <c r="G73" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L33 Q64:Q65 V33 AA64:AA65 AF33 G3:G25 AK3:AK15 AP3:AP15 AU3:AU15 L3:L30 Q3:Q61 V3:V30 AA3:AA61 AF3:AF30">
+  <conditionalFormatting sqref="L33 Q64:Q65 V33 AA64:AA65 AF33 G3:G25 AK3:AK15 AP3:AP15 AU3:AU15 L3:L30 Q3:Q61 V3:V30 AA3:AA61 AF3:AF30 AY3:AY9 BC3:BC9">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"purple"</formula>
     </cfRule>
@@ -34602,7 +34871,7 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C25 Q2:Q63 AA2:AA63 L2:L32 V2:V32 AF2:AF32 AK2:AK17 AP2:AP17 AU2:AU17 G2:G73">
+  <conditionalFormatting sqref="C2:C25 Q2:Q63 AA2:AA63 L2:L32 V2:V32 AF2:AF32 AK2:AK17 AP2:AP17 AU2:AU17 G2:G73 AY2:AY9 BC2:BC9">
     <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"purple"</formula>
     </cfRule>
@@ -34626,7 +34895,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C18 G2:G26 L2:L32 Q2:Q63 V2:V32 AA2:AA63 AF2:AF32 AK2:AK17 AP2:AP17 AU2:AU17 C19:C25 G27:G73" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C10 G2:G26 L2:L32 Q2:Q63 V2:V32 AA2:AA63 AF2:AF32 AK2:AK17 AP2:AP17 AU2:AU17 AY2:AY9 BC2:BC9 C11:C25 G27:G73" type="list">
       <formula1>"-,blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -34653,7 +34922,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34661,15 +34930,15 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="33"/>
       <c r="B1" s="34" t="s">
-        <v>580</v>
+        <v>602</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>581</v>
+        <v>603</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>582</v>
+        <v>604</v>
       </c>
       <c r="B2" s="36" t="n">
         <f aca="false">Groups!R65</f>
@@ -34682,7 +34951,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="37" t="s">
-        <v>583</v>
+        <v>605</v>
       </c>
       <c r="B3" s="36" t="n">
         <f aca="false">Groups!AL65</f>
@@ -34695,7 +34964,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
-        <v>584</v>
+        <v>606</v>
       </c>
       <c r="B4" s="36" t="n">
         <f aca="false">Groups!H65</f>
@@ -34708,7 +34977,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
-        <v>585</v>
+        <v>607</v>
       </c>
       <c r="B5" s="36" t="n">
         <f aca="false">Groups!AB65</f>
@@ -34721,7 +34990,7 @@
     </row>
     <row r="7" customFormat="false" ht="99.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="39" t="s">
-        <v>586</v>
+        <v>608</v>
       </c>
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
@@ -34751,7 +35020,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34763,24 +35032,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>588</v>
+        <v>610</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>589</v>
+        <v>611</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>591</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>